<commit_message>
add idea for sensitivities image
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391936D6-0C40-4F2A-AF8A-0C08D793FA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE0ED68-3512-4FB3-8A5C-9C3DAAA6018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>run_name</t>
   </si>
@@ -191,13 +191,46 @@
   </si>
   <si>
     <t>sens_10op_elpricevar_10pdown_PV</t>
+  </si>
+  <si>
+    <t>share electrolyser</t>
+  </si>
+  <si>
+    <t>Size electrolyser</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>District Heating Price</t>
+  </si>
+  <si>
+    <t>Power Price Variance</t>
+  </si>
+  <si>
+    <t>Power Price Level</t>
+  </si>
+  <si>
+    <t>WACC</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>+10%</t>
+  </si>
+  <si>
+    <t>Lifetime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,16 +238,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -222,17 +267,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -241,6 +320,23 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -270,20 +366,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -297,8 +379,1200 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Demand</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Base</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>+10%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison_sensitivities!$L$2:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="1">
+                  <c:v>1415.6985910000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-20BE-45F6-B90D-79B066E72F95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>District Heating Price</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="70000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Base</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>+10%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison_sensitivities!$M$2:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="1">
+                  <c:v>1415.6985910000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-20BE-45F6-B90D-79B066E72F95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power Price Level</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Base</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>+10%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison_sensitivities!$N$2:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1386.4903242285111</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1415.6985910000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1446.2267744709779</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-20BE-45F6-B90D-79B066E72F95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power Price Variance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Base</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>+10%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison_sensitivities!$O$2:$O$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1413.163937994756</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1415.6985910000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-20BE-45F6-B90D-79B066E72F95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WACC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="70000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Base</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>+10%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison_sensitivities!$P$2:$P$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1361.6928989999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1415.6985910000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1471.0608961910209</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-20BE-45F6-B90D-79B066E72F95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lifetime</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-10%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Base</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>+10%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison_sensitivities!$Q$2:$Q$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1459.447003719521</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1415.6985910000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1381.239008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-20BE-45F6-B90D-79B066E72F95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1747964879"/>
+        <c:axId val="1747965359"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1747964879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1747965359"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1747965359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1480"/>
+          <c:min val="1350"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1747964879"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{656F513E-DC43-8422-1B4F-351870668BA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73A3E7BD-A6FC-4C2D-BF58-717B292B5EEE}" name="Table1" displayName="Table1" ref="A1:I21" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73A3E7BD-A6FC-4C2D-BF58-717B292B5EEE}" name="Table1" displayName="Table1" ref="A1:I21" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:I21" xr:uid="{73A3E7BD-A6FC-4C2D-BF58-717B292B5EEE}">
     <filterColumn colId="1">
       <filters>
@@ -311,7 +1585,7 @@
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F67D044D-4890-48DB-B8DF-8989FCB998C3}" name="run_name"/>
-    <tableColumn id="9" xr3:uid="{E40D363F-DC65-4691-BE18-FF9BF756B0CE}" name="PV" dataDxfId="2">
+    <tableColumn id="9" xr3:uid="{E40D363F-DC65-4691-BE18-FF9BF756B0CE}" name="PV" dataDxfId="3">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{29706D13-ED84-4EF4-A454-0BFD2B9E1BAB}" name="LCOE [Euro/MWh]"/>
@@ -327,11 +1601,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3A20CD82-EF7A-4E40-8E75-04BE9F55963D}" name="Table2" displayName="Table2" ref="A1:I9" totalsRowShown="0">
-  <autoFilter ref="A1:I9" xr:uid="{3A20CD82-EF7A-4E40-8E75-04BE9F55963D}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3A20CD82-EF7A-4E40-8E75-04BE9F55963D}" name="Table2" displayName="Table2" ref="A1:K9" totalsRowShown="0">
+  <autoFilter ref="A1:K9" xr:uid="{3A20CD82-EF7A-4E40-8E75-04BE9F55963D}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{6128FCF1-7EAF-4DB9-AB65-A4970FF7A7B8}" name="run_name"/>
-    <tableColumn id="9" xr3:uid="{E1E483D4-117D-4835-9726-D5751F56EFA1}" name="PV" dataDxfId="1">
+    <tableColumn id="9" xr3:uid="{E1E483D4-117D-4835-9726-D5751F56EFA1}" name="PV" dataDxfId="2">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{57DD338E-2930-40CB-AC06-11C7900CEBAE}" name="LCOE [Euro/MWh]"/>
@@ -341,6 +1615,10 @@
     <tableColumn id="6" xr3:uid="{B1C9F88F-C828-404D-9F5C-8363B244D4A6}" name="energy_production [MWh]"/>
     <tableColumn id="7" xr3:uid="{DFDA2CA3-CD6F-466B-81A4-84B9B62CB2C6}" name="energy_production [t]"/>
     <tableColumn id="8" xr3:uid="{C340BB5F-846A-40DD-949F-DC14F9BEBD65}" name="pcf_value"/>
+    <tableColumn id="10" xr3:uid="{85810B0D-702B-4A48-ACC1-7F4EFAC09120}" name="share electrolyser"/>
+    <tableColumn id="11" xr3:uid="{3E078780-172C-4BE9-A08D-3FB4DFE536AE}" name="Size electrolyser" dataDxfId="0">
+      <calculatedColumnFormula>Table2[[#This Row],[share electrolyser]]*52</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -351,7 +1629,7 @@
   <autoFilter ref="A1:I21" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8869914E-4BE8-401C-AC76-C6570071019E}" name="run_name"/>
-    <tableColumn id="9" xr3:uid="{91B3AAB6-6FBC-4E2C-8674-ECB365CA16C8}" name="PV" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{91B3AAB6-6FBC-4E2C-8674-ECB365CA16C8}" name="PV" dataDxfId="1">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{EDC23835-EE0F-4ABC-9DD3-CB899B7BD1E4}" name="LCOE [Euro/MWh]"/>
@@ -1340,10 +2618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66730D5D-FFCC-4E02-B3EF-17A6B47B78F2}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1358,7 +2636,7 @@
     <col min="9" max="9" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1386,8 +2664,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1416,8 +2700,15 @@
       <c r="I2">
         <v>9.8181474069999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <v>0.82802811702252532</v>
+      </c>
+      <c r="K2">
+        <f>Table2[[#This Row],[share electrolyser]]*52</f>
+        <v>43.057462085171316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1446,8 +2737,15 @@
       <c r="I3">
         <v>9.8181474069999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <v>0.82802811702252532</v>
+      </c>
+      <c r="K3">
+        <f>Table2[[#This Row],[share electrolyser]]*52</f>
+        <v>43.057462085171316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1476,8 +2774,15 @@
       <c r="I4">
         <v>9.8181474069999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <v>0.81315475028895645</v>
+      </c>
+      <c r="K4">
+        <f>Table2[[#This Row],[share electrolyser]]*52</f>
+        <v>42.284047015025735</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1506,8 +2811,15 @@
       <c r="I5">
         <v>9.8181474069999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <v>0.81315475028895645</v>
+      </c>
+      <c r="K5">
+        <f>Table2[[#This Row],[share electrolyser]]*52</f>
+        <v>42.284047015025735</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1536,8 +2848,15 @@
       <c r="I6">
         <v>9.8181474069999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <f>Table2[[#This Row],[share electrolyser]]*52</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1566,8 +2885,15 @@
       <c r="I7">
         <v>9.8181474069999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f>Table2[[#This Row],[share electrolyser]]*52</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1596,8 +2922,15 @@
       <c r="I8">
         <v>9.8181474069999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f>Table2[[#This Row],[share electrolyser]]*52</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1625,6 +2958,13 @@
       </c>
       <c r="I9">
         <v>9.8181474069999997</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f>Table2[[#This Row],[share electrolyser]]*52</f>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1637,15 +2977,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
     <col min="3" max="3" width="17.54296875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="16.90625" customWidth="1"/>
@@ -1655,7 +2996,7 @@
     <col min="9" max="9" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1683,8 +3024,29 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1713,8 +3075,29 @@
       <c r="I2">
         <v>9.8181474069999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K2" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3">
+        <f>D16</f>
+        <v>1386.4903242285111</v>
+      </c>
+      <c r="O2" s="3">
+        <f>D20</f>
+        <v>1413.163937994756</v>
+      </c>
+      <c r="P2" s="3">
+        <f>D4</f>
+        <v>1361.6928989999999</v>
+      </c>
+      <c r="Q2">
+        <f>D8</f>
+        <v>1459.447003719521</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1743,8 +3126,35 @@
       <c r="I3">
         <v>9.8181474069999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="1">
+        <f>$D$2</f>
+        <v>1415.6985910000001</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" ref="M3:Q3" si="0">$D$2</f>
+        <v>1415.6985910000001</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" si="0"/>
+        <v>1415.6985910000001</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" si="0"/>
+        <v>1415.6985910000001</v>
+      </c>
+      <c r="P3" s="1">
+        <f t="shared" si="0"/>
+        <v>1415.6985910000001</v>
+      </c>
+      <c r="Q3" s="1">
+        <f t="shared" si="0"/>
+        <v>1415.6985910000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1773,8 +3183,26 @@
       <c r="I4">
         <v>10.431312399999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3">
+        <f>D18</f>
+        <v>1446.2267744709779</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3">
+        <f>D6</f>
+        <v>1471.0608961910209</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>D10</f>
+        <v>1381.239008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1804,7 +3232,7 @@
         <v>10.431312399999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1834,7 +3262,7 @@
         <v>9.2601513577926973</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1864,7 +3292,7 @@
         <v>9.2601513577926973</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1894,7 +3322,7 @@
         <v>9.3718871360488567</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1924,7 +3352,7 @@
         <v>9.3718871360488567</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1954,7 +3382,7 @@
         <v>10.200743660000001</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1984,7 +3412,7 @@
         <v>10.200743660000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -2014,7 +3442,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2044,7 +3472,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2074,7 +3502,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -2104,7 +3532,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2286,8 +3714,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add further prepared sensitivity results
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE0ED68-3512-4FB3-8A5C-9C3DAAA6018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B890DA1-FD6A-43D2-9A15-5D9BD37B96FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
+    <workbookView xWindow="-4590" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_operating_points" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
   <si>
     <t>run_name</t>
   </si>
@@ -220,10 +220,49 @@
     <t>Base</t>
   </si>
   <si>
-    <t>+10%</t>
-  </si>
-  <si>
     <t>Lifetime</t>
+  </si>
+  <si>
+    <t>sens_10op_elpricevar_10pup</t>
+  </si>
+  <si>
+    <t>sens_10op_elpricevar_10pup_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_WACC_05pdown</t>
+  </si>
+  <si>
+    <t>sens_10op_WACC_05pdown_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_WACC_05pup</t>
+  </si>
+  <si>
+    <t>sens_10op_WACC_05pup_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_lifetime_05pdown</t>
+  </si>
+  <si>
+    <t>sens_10op_lifetime_05pdown_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_lifetime_05pup</t>
+  </si>
+  <si>
+    <t>sens_10op_lifetime_05pup_PV</t>
+  </si>
+  <si>
+    <t>+10 %</t>
+  </si>
+  <si>
+    <t>-10 %</t>
+  </si>
+  <si>
+    <t>-5 %</t>
+  </si>
+  <si>
+    <t>+5 %</t>
   </si>
 </sst>
 </file>
@@ -297,16 +336,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,28 +466,34 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:f>Comparison_sensitivities!$K$2:$K$6</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-10%</c:v>
+                  <c:v>-10 %</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>-5 %</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Base</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>+10%</c:v>
+                <c:pt idx="3">
+                  <c:v>+5 %</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>+10 %</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison_sensitivities!$L$2:$L$4</c:f>
+              <c:f>Comparison_sensitivities!$L$2:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="1">
+                <c:ptCount val="5"/>
+                <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -493,28 +536,34 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:f>Comparison_sensitivities!$K$2:$K$6</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-10%</c:v>
+                  <c:v>-10 %</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>-5 %</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Base</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>+10%</c:v>
+                <c:pt idx="3">
+                  <c:v>+5 %</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>+10 %</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison_sensitivities!$M$2:$M$4</c:f>
+              <c:f>Comparison_sensitivities!$M$2:$M$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="1">
+                <c:ptCount val="5"/>
+                <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -557,34 +606,40 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:f>Comparison_sensitivities!$K$2:$K$6</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-10%</c:v>
+                  <c:v>-10 %</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>-5 %</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Base</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>+10%</c:v>
+                <c:pt idx="3">
+                  <c:v>+5 %</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>+10 %</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison_sensitivities!$N$2:$N$4</c:f>
+              <c:f>Comparison_sensitivities!$N$2:$N$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1386.4903242285111</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>1446.2267744709779</c:v>
                 </c:pt>
               </c:numCache>
@@ -627,32 +682,41 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:f>Comparison_sensitivities!$K$2:$K$6</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-10%</c:v>
+                  <c:v>-10 %</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>-5 %</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Base</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>+10%</c:v>
+                <c:pt idx="3">
+                  <c:v>+5 %</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>+10 %</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison_sensitivities!$O$2:$O$4</c:f>
+              <c:f>Comparison_sensitivities!$O$2:$O$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1413.163937994756</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1417.896003930397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -694,34 +758,46 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:f>Comparison_sensitivities!$K$2:$K$6</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-10%</c:v>
+                  <c:v>-10 %</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>-5 %</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Base</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>+10%</c:v>
+                <c:pt idx="3">
+                  <c:v>+5 %</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>+10 %</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison_sensitivities!$P$2:$P$4</c:f>
+              <c:f>Comparison_sensitivities!$P$2:$P$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1361.6928989999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1388.395832366482</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>1443.089109</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1471.0608961910209</c:v>
                 </c:pt>
               </c:numCache>
@@ -764,34 +840,46 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison_sensitivities!$K$2:$K$4</c:f>
+              <c:f>Comparison_sensitivities!$K$2:$K$6</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-10%</c:v>
+                  <c:v>-10 %</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>-5 %</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Base</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>+10%</c:v>
+                <c:pt idx="3">
+                  <c:v>+5 %</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>+10 %</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison_sensitivities!$Q$2:$Q$4</c:f>
+              <c:f>Comparison_sensitivities!$Q$2:$Q$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1459.447003719521</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1436.0983060000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>1397.35185</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1381.239008</c:v>
                 </c:pt>
               </c:numCache>
@@ -1535,15 +1623,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1616,7 +1704,7 @@
     <tableColumn id="7" xr3:uid="{DFDA2CA3-CD6F-466B-81A4-84B9B62CB2C6}" name="energy_production [t]"/>
     <tableColumn id="8" xr3:uid="{C340BB5F-846A-40DD-949F-DC14F9BEBD65}" name="pcf_value"/>
     <tableColumn id="10" xr3:uid="{85810B0D-702B-4A48-ACC1-7F4EFAC09120}" name="share electrolyser"/>
-    <tableColumn id="11" xr3:uid="{3E078780-172C-4BE9-A08D-3FB4DFE536AE}" name="Size electrolyser" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{3E078780-172C-4BE9-A08D-3FB4DFE536AE}" name="Size electrolyser" dataDxfId="1">
       <calculatedColumnFormula>Table2[[#This Row],[share electrolyser]]*52</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1625,11 +1713,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I21" totalsRowShown="0">
-  <autoFilter ref="A1:I21" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I31" totalsRowShown="0">
+  <autoFilter ref="A1:I31" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8869914E-4BE8-401C-AC76-C6570071019E}" name="run_name"/>
-    <tableColumn id="9" xr3:uid="{91B3AAB6-6FBC-4E2C-8674-ECB365CA16C8}" name="PV" dataDxfId="1">
+    <tableColumn id="9" xr3:uid="{91B3AAB6-6FBC-4E2C-8674-ECB365CA16C8}" name="PV" dataDxfId="0">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{EDC23835-EE0F-4ABC-9DD3-CB899B7BD1E4}" name="LCOE [Euro/MWh]"/>
@@ -2977,10 +3065,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3024,26 +3112,26 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>61</v>
+      <c r="Q1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -3075,20 +3163,18 @@
       <c r="I2">
         <v>9.8181474069999997</v>
       </c>
-      <c r="K2" s="4">
-        <v>-0.1</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3">
+      <c r="K2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2">
         <f>D16</f>
         <v>1386.4903242285111</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2">
         <f>D20</f>
         <v>1413.163937994756</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2">
         <f>D4</f>
         <v>1361.6928989999999</v>
       </c>
@@ -3126,32 +3212,16 @@
       <c r="I3">
         <v>9.8181474069999997</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" s="1">
-        <f>$D$2</f>
-        <v>1415.6985910000001</v>
-      </c>
-      <c r="M3" s="1">
-        <f t="shared" ref="M3:Q3" si="0">$D$2</f>
-        <v>1415.6985910000001</v>
-      </c>
-      <c r="N3" s="1">
-        <f t="shared" si="0"/>
-        <v>1415.6985910000001</v>
-      </c>
-      <c r="O3" s="1">
-        <f t="shared" si="0"/>
-        <v>1415.6985910000001</v>
-      </c>
-      <c r="P3" s="1">
-        <f t="shared" si="0"/>
-        <v>1415.6985910000001</v>
-      </c>
-      <c r="Q3" s="1">
-        <f t="shared" si="0"/>
-        <v>1415.6985910000001</v>
+      <c r="K3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3">
+        <f>D24</f>
+        <v>1388.395832366482</v>
+      </c>
+      <c r="Q3">
+        <f>D28</f>
+        <v>1436.0983060000001</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -3183,23 +3253,32 @@
       <c r="I4">
         <v>10.431312399999999</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3">
-        <f>D18</f>
-        <v>1446.2267744709779</v>
-      </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3">
-        <f>D6</f>
-        <v>1471.0608961910209</v>
-      </c>
-      <c r="Q4" s="3">
-        <f>D10</f>
-        <v>1381.239008</v>
+      <c r="K4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="1">
+        <f>$D$2</f>
+        <v>1415.6985910000001</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:Q4" si="0">$D$2</f>
+        <v>1415.6985910000001</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="0"/>
+        <v>1415.6985910000001</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="0"/>
+        <v>1415.6985910000001</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" si="0"/>
+        <v>1415.6985910000001</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" si="0"/>
+        <v>1415.6985910000001</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
@@ -3231,6 +3310,17 @@
       <c r="I5">
         <v>10.431312399999999</v>
       </c>
+      <c r="K5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P5">
+        <f>D26</f>
+        <v>1443.089109</v>
+      </c>
+      <c r="Q5">
+        <f>D30</f>
+        <v>1397.35185</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -3261,6 +3351,25 @@
       <c r="I6">
         <v>9.2601513577926973</v>
       </c>
+      <c r="K6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6">
+        <f>D18</f>
+        <v>1446.2267744709779</v>
+      </c>
+      <c r="O6">
+        <f>D22</f>
+        <v>1417.896003930397</v>
+      </c>
+      <c r="P6">
+        <f>D6</f>
+        <v>1471.0608961910209</v>
+      </c>
+      <c r="Q6">
+        <f>D10</f>
+        <v>1381.239008</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -3710,6 +3819,306 @@
       </c>
       <c r="I21">
         <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C22">
+        <v>256.50379970600142</v>
+      </c>
+      <c r="D22">
+        <v>1417.896003930397</v>
+      </c>
+      <c r="E22">
+        <v>289790455.41130489</v>
+      </c>
+      <c r="F22">
+        <v>15856884.178413169</v>
+      </c>
+      <c r="G22">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H22">
+        <v>32000.007075376889</v>
+      </c>
+      <c r="I22">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C23">
+        <v>203.14207603492159</v>
+      </c>
+      <c r="D23">
+        <v>1122.9242536374829</v>
+      </c>
+      <c r="E23">
+        <v>289790455.41130489</v>
+      </c>
+      <c r="F23">
+        <v>6417786.0820036363</v>
+      </c>
+      <c r="G23">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H23">
+        <v>32000.007075376889</v>
+      </c>
+      <c r="I23">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C24" s="4">
+        <v>251.16708525222791</v>
+      </c>
+      <c r="D24">
+        <v>1388.395832366482</v>
+      </c>
+      <c r="E24">
+        <v>288656108.20733207</v>
+      </c>
+      <c r="F24">
+        <v>15898080.2506778</v>
+      </c>
+      <c r="G24">
+        <v>176888.9279999992</v>
+      </c>
+      <c r="H24">
+        <v>32000.00707537675</v>
+      </c>
+      <c r="I24">
+        <v>10.117422927236451</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C25" s="4">
+        <v>197.89745178735001</v>
+      </c>
+      <c r="D25">
+        <v>1093.9331362689629</v>
+      </c>
+      <c r="E25">
+        <v>288656108.20733207</v>
+      </c>
+      <c r="F25">
+        <v>6475271.8921226691</v>
+      </c>
+      <c r="G25">
+        <v>176888.9279999992</v>
+      </c>
+      <c r="H25">
+        <v>32000.00707537675</v>
+      </c>
+      <c r="I25">
+        <v>10.117422927236451</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C26">
+        <v>261.06134630000003</v>
+      </c>
+      <c r="D26">
+        <v>1443.089109</v>
+      </c>
+      <c r="E26">
+        <v>288656108.19999999</v>
+      </c>
+      <c r="F26">
+        <v>15898080.25</v>
+      </c>
+      <c r="G26">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H26">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I26">
+        <v>9.5326505640000008</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C27">
+        <v>207.7917128</v>
+      </c>
+      <c r="D27">
+        <v>1148.6264120000001</v>
+      </c>
+      <c r="E27">
+        <v>288656108.19999999</v>
+      </c>
+      <c r="F27">
+        <v>6475271.892</v>
+      </c>
+      <c r="G27">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H27">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I27">
+        <v>9.5326505640000008</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C28">
+        <v>259.79667849999998</v>
+      </c>
+      <c r="D28">
+        <v>1436.0983060000001</v>
+      </c>
+      <c r="E28">
+        <v>288656108.19999999</v>
+      </c>
+      <c r="F28">
+        <v>15898080.25</v>
+      </c>
+      <c r="G28">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H28">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I28">
+        <v>9.6035991999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C29">
+        <v>206.52704499999999</v>
+      </c>
+      <c r="D29">
+        <v>1141.63561</v>
+      </c>
+      <c r="E29">
+        <v>288656108.19999999</v>
+      </c>
+      <c r="F29">
+        <v>6475271.892</v>
+      </c>
+      <c r="G29">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H29">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I29">
+        <v>9.6035991999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C30">
+        <v>252.78726940000001</v>
+      </c>
+      <c r="D30">
+        <v>1397.35185</v>
+      </c>
+      <c r="E30">
+        <v>288656108.19999999</v>
+      </c>
+      <c r="F30">
+        <v>15898080.25</v>
+      </c>
+      <c r="G30">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H30">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I30">
+        <v>10.01680316</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C31">
+        <v>199.51763600000001</v>
+      </c>
+      <c r="D31">
+        <v>1102.889154</v>
+      </c>
+      <c r="E31">
+        <v>288656108.19999999</v>
+      </c>
+      <c r="F31">
+        <v>6475271.892</v>
+      </c>
+      <c r="G31">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H31">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I31">
+        <v>10.01680316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add prepared outputs for demand sensitivity of 10%
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B890DA1-FD6A-43D2-9A15-5D9BD37B96FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48076620-9A81-4D95-A64C-47202475AFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4590" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
   <si>
     <t>run_name</t>
   </si>
@@ -263,6 +263,18 @@
   </si>
   <si>
     <t>+5 %</t>
+  </si>
+  <si>
+    <t>sens_10op_demand_10pdown</t>
+  </si>
+  <si>
+    <t>sens_10op_demand_10pdown_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_demand_10pup</t>
+  </si>
+  <si>
+    <t>sens_10op_demand_10pup_PV</t>
   </si>
 </sst>
 </file>
@@ -493,8 +505,20 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1498.8447471929501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1450</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1347.8877936210879</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -563,8 +587,20 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1405</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1410</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1420</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1425</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -636,8 +672,14 @@
                 <c:pt idx="0">
                   <c:v>1386.4903242285111</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>1400</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1430</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1446.2267744709779</c:v>
@@ -712,8 +754,14 @@
                 <c:pt idx="0">
                   <c:v>1413.163937994756</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>1414</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1416</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1417.896003930397</c:v>
@@ -1713,12 +1761,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I31" totalsRowShown="0">
-  <autoFilter ref="A1:I31" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I35" totalsRowShown="0">
+  <autoFilter ref="A1:I35" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8869914E-4BE8-401C-AC76-C6570071019E}" name="run_name"/>
     <tableColumn id="9" xr3:uid="{91B3AAB6-6FBC-4E2C-8674-ECB365CA16C8}" name="PV" dataDxfId="0">
-      <calculatedColumnFormula>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(ISNUMBER(SEARCH("PV", A2)),"PV revenue","no PV revenue")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{EDC23835-EE0F-4ABC-9DD3-CB899B7BD1E4}" name="LCOE [Euro/MWh]"/>
     <tableColumn id="3" xr3:uid="{0704ECC2-FF39-4625-8AC6-5CFC7159B06A}" name="LCOE [Euro/t]"/>
@@ -3065,10 +3113,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3139,7 +3187,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" ref="B2:B35" si="0">IF(ISNUMBER(SEARCH("PV", A2)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C2">
@@ -3165,6 +3213,13 @@
       </c>
       <c r="K2" s="2" t="s">
         <v>72</v>
+      </c>
+      <c r="L2">
+        <f>D32</f>
+        <v>1498.8447471929501</v>
+      </c>
+      <c r="M2">
+        <v>1405</v>
       </c>
       <c r="N2">
         <f>D16</f>
@@ -3188,7 +3243,7 @@
         <v>27</v>
       </c>
       <c r="B3" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C3">
@@ -3214,6 +3269,18 @@
       </c>
       <c r="K3" s="2" t="s">
         <v>73</v>
+      </c>
+      <c r="L3">
+        <v>1450</v>
+      </c>
+      <c r="M3">
+        <v>1410</v>
+      </c>
+      <c r="N3">
+        <v>1400</v>
+      </c>
+      <c r="O3">
+        <v>1414</v>
       </c>
       <c r="P3">
         <f>D24</f>
@@ -3229,7 +3296,7 @@
         <v>41</v>
       </c>
       <c r="B4" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C4">
@@ -3261,23 +3328,23 @@
         <v>1415.6985910000001</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" ref="M4:Q4" si="0">$D$2</f>
+        <f t="shared" ref="M4:Q4" si="1">$D$2</f>
         <v>1415.6985910000001</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1415.6985910000001</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1415.6985910000001</v>
       </c>
       <c r="P4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1415.6985910000001</v>
       </c>
       <c r="Q4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1415.6985910000001</v>
       </c>
     </row>
@@ -3286,7 +3353,7 @@
         <v>43</v>
       </c>
       <c r="B5" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C5">
@@ -3312,6 +3379,18 @@
       </c>
       <c r="K5" s="2" t="s">
         <v>74</v>
+      </c>
+      <c r="L5">
+        <v>1400</v>
+      </c>
+      <c r="M5">
+        <v>1420</v>
+      </c>
+      <c r="N5">
+        <v>1430</v>
+      </c>
+      <c r="O5">
+        <v>1416</v>
       </c>
       <c r="P5">
         <f>D26</f>
@@ -3327,7 +3406,7 @@
         <v>44</v>
       </c>
       <c r="B6" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C6">
@@ -3353,6 +3432,13 @@
       </c>
       <c r="K6" s="2" t="s">
         <v>71</v>
+      </c>
+      <c r="L6">
+        <f>D34</f>
+        <v>1347.8877936210879</v>
+      </c>
+      <c r="M6">
+        <v>1425</v>
       </c>
       <c r="N6">
         <f>D18</f>
@@ -3376,7 +3462,7 @@
         <v>42</v>
       </c>
       <c r="B7" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C7">
@@ -3406,7 +3492,7 @@
         <v>45</v>
       </c>
       <c r="B8" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C8">
@@ -3436,7 +3522,7 @@
         <v>46</v>
       </c>
       <c r="B9" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C9">
@@ -3466,7 +3552,7 @@
         <v>47</v>
       </c>
       <c r="B10" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C10">
@@ -3496,7 +3582,7 @@
         <v>48</v>
       </c>
       <c r="B11" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C11">
@@ -3526,7 +3612,7 @@
         <v>39</v>
       </c>
       <c r="B12" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C12">
@@ -3556,7 +3642,7 @@
         <v>40</v>
       </c>
       <c r="B13" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C13">
@@ -3586,7 +3672,7 @@
         <v>37</v>
       </c>
       <c r="B14" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C14">
@@ -3616,7 +3702,7 @@
         <v>38</v>
       </c>
       <c r="B15" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C15">
@@ -3646,7 +3732,7 @@
         <v>33</v>
       </c>
       <c r="B16" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C16">
@@ -3676,7 +3762,7 @@
         <v>34</v>
       </c>
       <c r="B17" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C17">
@@ -3706,7 +3792,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C18">
@@ -3736,7 +3822,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C19">
@@ -3766,7 +3852,7 @@
         <v>49</v>
       </c>
       <c r="B20" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C20">
@@ -3796,7 +3882,7 @@
         <v>50</v>
       </c>
       <c r="B21" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C21">
@@ -3826,7 +3912,7 @@
         <v>61</v>
       </c>
       <c r="B22" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C22">
@@ -3856,8 +3942,8 @@
         <v>62</v>
       </c>
       <c r="B23" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
-        <v>no PV revenue</v>
+        <f t="shared" si="0"/>
+        <v>PV revenue</v>
       </c>
       <c r="C23">
         <v>203.14207603492159</v>
@@ -3886,10 +3972,10 @@
         <v>63</v>
       </c>
       <c r="B24" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24">
         <v>251.16708525222791</v>
       </c>
       <c r="D24">
@@ -3916,10 +4002,10 @@
         <v>64</v>
       </c>
       <c r="B25" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
-        <v>no PV revenue</v>
-      </c>
-      <c r="C25" s="4">
+        <f t="shared" si="0"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C25">
         <v>197.89745178735001</v>
       </c>
       <c r="D25">
@@ -3946,7 +4032,7 @@
         <v>65</v>
       </c>
       <c r="B26" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C26">
@@ -3976,8 +4062,8 @@
         <v>66</v>
       </c>
       <c r="B27" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
-        <v>no PV revenue</v>
+        <f t="shared" si="0"/>
+        <v>PV revenue</v>
       </c>
       <c r="C27">
         <v>207.7917128</v>
@@ -4006,7 +4092,7 @@
         <v>67</v>
       </c>
       <c r="B28" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C28">
@@ -4036,8 +4122,8 @@
         <v>68</v>
       </c>
       <c r="B29" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
-        <v>no PV revenue</v>
+        <f t="shared" si="0"/>
+        <v>PV revenue</v>
       </c>
       <c r="C29">
         <v>206.52704499999999</v>
@@ -4066,7 +4152,7 @@
         <v>69</v>
       </c>
       <c r="B30" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C30">
@@ -4096,8 +4182,8 @@
         <v>70</v>
       </c>
       <c r="B31" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
-        <v>no PV revenue</v>
+        <f t="shared" si="0"/>
+        <v>PV revenue</v>
       </c>
       <c r="C31">
         <v>199.51763600000001</v>
@@ -4119,6 +4205,126 @@
       </c>
       <c r="I31">
         <v>10.01680316</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C32" s="4">
+        <v>271.14779346204119</v>
+      </c>
+      <c r="D32">
+        <v>1498.8447471929501</v>
+      </c>
+      <c r="E32">
+        <v>277512962.69202578</v>
+      </c>
+      <c r="F32">
+        <v>14901430.036319871</v>
+      </c>
+      <c r="G32">
+        <v>159200.03520000001</v>
+      </c>
+      <c r="H32">
+        <v>28800.006367839189</v>
+      </c>
+      <c r="I32">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C33" s="4">
+        <v>209.36483468310021</v>
+      </c>
+      <c r="D33">
+        <v>1157.322280609359</v>
+      </c>
+      <c r="E33">
+        <v>277512962.69202578</v>
+      </c>
+      <c r="F33">
+        <v>5065580.8239523079</v>
+      </c>
+      <c r="G33">
+        <v>159200.03520000001</v>
+      </c>
+      <c r="H33">
+        <v>28800.006367839189</v>
+      </c>
+      <c r="I33">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C34" s="4">
+        <v>243.83899784100089</v>
+      </c>
+      <c r="D34">
+        <v>1347.8877936210879</v>
+      </c>
+      <c r="E34">
+        <v>299683366.79336238</v>
+      </c>
+      <c r="F34">
+        <v>16922247.970495451</v>
+      </c>
+      <c r="G34">
+        <v>194577.82079999999</v>
+      </c>
+      <c r="H34">
+        <v>35200.007782914567</v>
+      </c>
+      <c r="I34">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C35" s="4">
+        <v>197.43082398181659</v>
+      </c>
+      <c r="D35">
+        <v>1091.353721455042</v>
+      </c>
+      <c r="E35">
+        <v>299683366.79336238</v>
+      </c>
+      <c r="F35">
+        <v>7892246.6336678583</v>
+      </c>
+      <c r="G35">
+        <v>194577.82079999999</v>
+      </c>
+      <c r="H35">
+        <v>35200.007782914567</v>
+      </c>
+      <c r="I35">
+        <v>9.8181474074492936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add prepared results for dh price sensitivities
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48076620-9A81-4D95-A64C-47202475AFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1B6982-349A-4D3E-8A87-29177509C991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4590" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_operating_points" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
   <si>
     <t>run_name</t>
   </si>
@@ -275,6 +275,18 @@
   </si>
   <si>
     <t>sens_10op_demand_10pup_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_dhprice_10pup</t>
+  </si>
+  <si>
+    <t>sens_10op_dhprice_10pup_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_dhprice_10pdown</t>
+  </si>
+  <si>
+    <t>sens_10op_dhprice_10pdown_PV</t>
   </si>
 </sst>
 </file>
@@ -348,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -356,6 +368,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,19 +602,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1405</c:v>
+                  <c:v>1436.962304287056</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1410</c:v>
+                  <c:v>1425</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1420</c:v>
+                  <c:v>1410</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1425</c:v>
+                  <c:v>1394.183473598318</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1761,8 +1775,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I35" totalsRowShown="0">
-  <autoFilter ref="A1:I35" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I39" totalsRowShown="0">
+  <autoFilter ref="A1:I39" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8869914E-4BE8-401C-AC76-C6570071019E}" name="run_name"/>
     <tableColumn id="9" xr3:uid="{91B3AAB6-6FBC-4E2C-8674-ECB365CA16C8}" name="PV" dataDxfId="0">
@@ -3113,10 +3127,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3187,7 +3201,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B35" si="0">IF(ISNUMBER(SEARCH("PV", A2)),"PV revenue","no PV revenue")</f>
+        <f t="shared" ref="B2:B37" si="0">IF(ISNUMBER(SEARCH("PV", A2)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C2">
@@ -3219,7 +3233,8 @@
         <v>1498.8447471929501</v>
       </c>
       <c r="M2">
-        <v>1405</v>
+        <f>D36</f>
+        <v>1436.962304287056</v>
       </c>
       <c r="N2">
         <f>D16</f>
@@ -3274,7 +3289,7 @@
         <v>1450</v>
       </c>
       <c r="M3">
-        <v>1410</v>
+        <v>1425</v>
       </c>
       <c r="N3">
         <v>1400</v>
@@ -3384,7 +3399,7 @@
         <v>1400</v>
       </c>
       <c r="M5">
-        <v>1420</v>
+        <v>1410</v>
       </c>
       <c r="N5">
         <v>1430</v>
@@ -3438,7 +3453,8 @@
         <v>1347.8877936210879</v>
       </c>
       <c r="M6">
-        <v>1425</v>
+        <f>D38</f>
+        <v>1394.183473598318</v>
       </c>
       <c r="N6">
         <f>D18</f>
@@ -4215,7 +4231,7 @@
         <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32">
         <v>271.14779346204119</v>
       </c>
       <c r="D32">
@@ -4245,7 +4261,7 @@
         <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33">
         <v>209.36483468310021</v>
       </c>
       <c r="D33">
@@ -4275,7 +4291,7 @@
         <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34">
         <v>243.83899784100089</v>
       </c>
       <c r="D34">
@@ -4305,7 +4321,7 @@
         <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35">
         <v>197.43082398181659</v>
       </c>
       <c r="D35">
@@ -4324,6 +4340,126 @@
         <v>35200.007782914567</v>
       </c>
       <c r="I35">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C36" s="4">
+        <v>259.95297967002011</v>
+      </c>
+      <c r="D36">
+        <v>1436.962304287056</v>
+      </c>
+      <c r="E36">
+        <v>288656108.20669693</v>
+      </c>
+      <c r="F36">
+        <v>16582541.6930892</v>
+      </c>
+      <c r="G36">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H36">
+        <v>32000.007075376881</v>
+      </c>
+      <c r="I36">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C37" s="5">
+        <v>206.68334620500781</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1142.499608188793</v>
+      </c>
+      <c r="E37" s="6">
+        <v>288656108.20669693</v>
+      </c>
+      <c r="F37" s="6">
+        <v>7159733.334510237</v>
+      </c>
+      <c r="G37" s="6">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H37" s="6">
+        <v>32000.007075376881</v>
+      </c>
+      <c r="I37" s="6">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="4" t="str">
+        <f t="shared" ref="B38:B39" si="2">IF(ISNUMBER(SEARCH("PV", A38)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C38" s="4">
+        <v>252.21409572632879</v>
+      </c>
+      <c r="D38">
+        <v>1394.183473598318</v>
+      </c>
+      <c r="E38">
+        <v>288656108.2073791</v>
+      </c>
+      <c r="F38">
+        <v>15213618.80830376</v>
+      </c>
+      <c r="G38">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H38">
+        <v>32000.007075376881</v>
+      </c>
+      <c r="I38">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C39" s="5">
+        <v>198.94446226144731</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1099.720777500778</v>
+      </c>
+      <c r="E39" s="6">
+        <v>288656108.2073791</v>
+      </c>
+      <c r="F39" s="6">
+        <v>5790810.4497479387</v>
+      </c>
+      <c r="G39" s="6">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H39" s="6">
+        <v>32000.007075376881</v>
+      </c>
+      <c r="I39" s="6">
         <v>9.8181474074492936</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update prepared results for 8 operating points
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1B6982-349A-4D3E-8A87-29177509C991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBB4F46-32C0-41BA-8148-5A65A735DF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_operating_points" sheetId="1" r:id="rId1"/>
@@ -360,16 +360,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1723,15 +1720,9 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73A3E7BD-A6FC-4C2D-BF58-717B292B5EEE}" name="Table1" displayName="Table1" ref="A1:I21" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A1:I21" xr:uid="{73A3E7BD-A6FC-4C2D-BF58-717B292B5EEE}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="no PV revenue"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I20">
-    <sortCondition ref="D1:D21"/>
+  <autoFilter ref="A1:I21" xr:uid="{73A3E7BD-A6FC-4C2D-BF58-717B292B5EEE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I21">
+    <sortCondition ref="A1:A21"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F67D044D-4890-48DB-B8DF-8989FCB998C3}" name="run_name"/>
@@ -2113,8 +2104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB416CA-7C9B-4F0E-AFD4-34077EF25340}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2160,143 +2151,143 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B2" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C2">
-        <v>254.96266482664441</v>
+        <v>256.10627770000002</v>
       </c>
       <c r="D2">
-        <v>1409.3769527917291</v>
+        <v>1415.6985910000001</v>
       </c>
       <c r="E2">
-        <v>286911074.34615147</v>
+        <v>288656108.19999999</v>
       </c>
       <c r="F2">
-        <v>15877545.80322974</v>
+        <v>15902102.699999999</v>
       </c>
       <c r="G2">
         <v>176888.92800000001</v>
       </c>
       <c r="H2">
-        <v>32000.007075376889</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I2">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B3" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C3">
-        <v>201.2788905306509</v>
+        <v>202.8139042</v>
       </c>
       <c r="D3">
-        <v>1112.6249782110981</v>
+        <v>1121.110193</v>
       </c>
       <c r="E3">
-        <v>286911074.34615147</v>
+        <v>288656108.19999999</v>
       </c>
       <c r="F3">
-        <v>6381480.5170174837</v>
+        <v>6475271.892</v>
       </c>
       <c r="G3">
         <v>176888.92800000001</v>
       </c>
       <c r="H3">
-        <v>32000.007075376889</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I3">
-        <v>9.8181474074492936</v>
+        <v>9.8181474069999997</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C4">
-        <v>255.44107389999999</v>
+        <v>254.96266482664441</v>
       </c>
       <c r="D4">
-        <v>1412.0214920000001</v>
+        <v>1409.3769527917291</v>
       </c>
       <c r="E4">
-        <v>287398388.39999998</v>
+        <v>286911074.34615147</v>
       </c>
       <c r="F4">
-        <v>15912537.050000001</v>
+        <v>15877545.80322974</v>
       </c>
       <c r="G4">
         <v>176888.92800000001</v>
       </c>
       <c r="H4">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I4">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C5">
-        <v>201.8789865</v>
+        <v>201.2788905306509</v>
       </c>
       <c r="D5">
-        <v>1115.942176</v>
+        <v>1112.6249782110981</v>
       </c>
       <c r="E5">
-        <v>287398388.39999998</v>
+        <v>286911074.34615147</v>
       </c>
       <c r="F5">
-        <v>6437996.8420000002</v>
+        <v>6381480.5170174837</v>
       </c>
       <c r="G5">
         <v>176888.92800000001</v>
       </c>
       <c r="H5">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I5">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C6">
-        <v>255.86895699999999</v>
+        <v>255.44107389999999</v>
       </c>
       <c r="D6">
-        <v>1414.386735</v>
+        <v>1412.0214920000001</v>
       </c>
       <c r="E6">
-        <v>288262500</v>
+        <v>287398388.39999998</v>
       </c>
       <c r="F6">
-        <v>15900213.17</v>
+        <v>15912537.050000001</v>
       </c>
       <c r="G6">
         <v>176888.92800000001</v>
@@ -2308,25 +2299,25 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C7">
-        <v>202.50746839999999</v>
+        <v>201.8789865</v>
       </c>
       <c r="D7">
-        <v>1119.416283</v>
+        <v>1115.942176</v>
       </c>
       <c r="E7">
-        <v>288262500</v>
+        <v>287398388.39999998</v>
       </c>
       <c r="F7">
-        <v>6461156.6449999996</v>
+        <v>6437996.8420000002</v>
       </c>
       <c r="G7">
         <v>176888.92800000001</v>
@@ -2340,23 +2331,23 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C8">
-        <v>255.97229770000001</v>
+        <v>255.86895699999999</v>
       </c>
       <c r="D8">
-        <v>1414.957979</v>
+        <v>1414.386735</v>
       </c>
       <c r="E8">
-        <v>288420132.5</v>
+        <v>288262500</v>
       </c>
       <c r="F8">
-        <v>15902437.77</v>
+        <v>15900213.17</v>
       </c>
       <c r="G8">
         <v>176888.92800000001</v>
@@ -2368,25 +2359,25 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C9">
-        <v>202.6404757</v>
+        <v>202.50746839999999</v>
       </c>
       <c r="D9">
-        <v>1120.1515179999999</v>
+        <v>1119.416283</v>
       </c>
       <c r="E9">
-        <v>288420132.5</v>
+        <v>288262500</v>
       </c>
       <c r="F9">
-        <v>6468628.9440000001</v>
+        <v>6461156.6449999996</v>
       </c>
       <c r="G9">
         <v>176888.92800000001</v>
@@ -2400,23 +2391,23 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B10" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C10">
-        <v>255.97229770000001</v>
+        <v>256.08701760000002</v>
       </c>
       <c r="D10">
-        <v>1414.957979</v>
+        <v>1415.5921249999999</v>
       </c>
       <c r="E10">
-        <v>288420132.5</v>
+        <v>288545796.10000002</v>
       </c>
       <c r="F10">
-        <v>15902437.77</v>
+        <v>15909931.33</v>
       </c>
       <c r="G10">
         <v>176888.92800000001</v>
@@ -2428,25 +2419,25 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B11" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C11">
-        <v>202.6404757</v>
+        <v>202.75017940000001</v>
       </c>
       <c r="D11">
-        <v>1120.1515179999999</v>
+        <v>1120.757936</v>
       </c>
       <c r="E11">
-        <v>288420132.5</v>
+        <v>288545796.10000002</v>
       </c>
       <c r="F11">
-        <v>6468628.9440000001</v>
+        <v>6475235.2039999999</v>
       </c>
       <c r="G11">
         <v>176888.92800000001</v>
@@ -2460,53 +2451,53 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B12" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C12">
-        <v>256.07102687952232</v>
+        <v>255.97229770000001</v>
       </c>
       <c r="D12">
-        <v>1415.5037319173589</v>
+        <v>1414.957979</v>
       </c>
       <c r="E12">
-        <v>288705429.34616148</v>
+        <v>288420132.5</v>
       </c>
       <c r="F12">
-        <v>15890843.7584353</v>
+        <v>15902437.77</v>
       </c>
       <c r="G12">
         <v>176888.92800000001</v>
       </c>
       <c r="H12">
-        <v>32000.007075376889</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I12">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B13" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C13">
-        <v>202.75017940000001</v>
+        <v>202.6404757</v>
       </c>
       <c r="D13">
-        <v>1120.757936</v>
+        <v>1120.1515179999999</v>
       </c>
       <c r="E13">
-        <v>288545796.10000002</v>
+        <v>288420132.5</v>
       </c>
       <c r="F13">
-        <v>6475235.2039999999</v>
+        <v>6468628.9440000001</v>
       </c>
       <c r="G13">
         <v>176888.92800000001</v>
@@ -2520,23 +2511,23 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B14" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C14">
-        <v>256.08701760000002</v>
+        <v>256.12943489999998</v>
       </c>
       <c r="D14">
-        <v>1415.5921249999999</v>
+        <v>1415.8265980000001</v>
       </c>
       <c r="E14">
-        <v>288545796.10000002</v>
+        <v>288709501.89999998</v>
       </c>
       <c r="F14">
-        <v>15909931.33</v>
+        <v>15900760.689999999</v>
       </c>
       <c r="G14">
         <v>176888.92800000001</v>
@@ -2548,175 +2539,175 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C15">
-        <v>202.75983826205081</v>
+        <v>202.83341619999999</v>
       </c>
       <c r="D15">
-        <v>1120.8113281707811</v>
+        <v>1121.2180510000001</v>
       </c>
       <c r="E15">
-        <v>288705429.34616148</v>
+        <v>288709501.89999998</v>
       </c>
       <c r="F15">
-        <v>6460684.7534849672</v>
+        <v>6473285.0750000002</v>
       </c>
       <c r="G15">
         <v>176888.92800000001</v>
       </c>
       <c r="H15">
-        <v>32000.007075376889</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I15">
-        <v>9.8181474074492936</v>
+        <v>9.8181474069999997</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B16" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C16">
-        <v>256.10627770000002</v>
+        <v>256.07102687952232</v>
       </c>
       <c r="D16">
-        <v>1415.6985910000001</v>
+        <v>1415.5037319173589</v>
       </c>
       <c r="E16">
-        <v>288656108.19999999</v>
+        <v>288705429.34616148</v>
       </c>
       <c r="F16">
-        <v>15902102.699999999</v>
+        <v>15890843.7584353</v>
       </c>
       <c r="G16">
         <v>176888.92800000001</v>
       </c>
       <c r="H16">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I16">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B17" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C17">
-        <v>202.8139042</v>
+        <v>202.75983826205081</v>
       </c>
       <c r="D17">
-        <v>1121.110193</v>
+        <v>1120.8113281707811</v>
       </c>
       <c r="E17">
-        <v>288656108.19999999</v>
+        <v>288705429.34616148</v>
       </c>
       <c r="F17">
-        <v>6475271.892</v>
+        <v>6460684.7534849672</v>
       </c>
       <c r="G17">
         <v>176888.92800000001</v>
       </c>
       <c r="H17">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I17">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C18">
-        <v>256.1063924</v>
+        <v>256.04429678074212</v>
       </c>
       <c r="D18">
-        <v>1415.6992250000001</v>
+        <v>1415.3559738713241</v>
       </c>
       <c r="E18">
-        <v>288687149.69999999</v>
+        <v>288557068.64214009</v>
       </c>
       <c r="F18">
-        <v>15898961.359999999</v>
+        <v>15901226.36532389</v>
       </c>
       <c r="G18">
         <v>176888.92800000001</v>
       </c>
       <c r="H18">
-        <v>32000.007079999999</v>
+        <v>32000.0070753769</v>
       </c>
       <c r="I18">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C19">
-        <v>202.82884859999999</v>
+        <v>202.7734041647862</v>
       </c>
       <c r="D19">
-        <v>1121.192802</v>
+        <v>1120.8863174664571</v>
       </c>
       <c r="E19">
-        <v>288687149.69999999</v>
+        <v>288557068.64214009</v>
       </c>
       <c r="F19">
-        <v>6474753.7419999996</v>
+        <v>6478195.2768843267</v>
       </c>
       <c r="G19">
         <v>176888.92800000001</v>
       </c>
       <c r="H19">
-        <v>32000.007079999999</v>
+        <v>32000.0070753769</v>
       </c>
       <c r="I19">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B20" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C20">
-        <v>256.12943489999998</v>
+        <v>256.1063924</v>
       </c>
       <c r="D20">
-        <v>1415.8265980000001</v>
+        <v>1415.6992250000001</v>
       </c>
       <c r="E20">
-        <v>288709501.89999998</v>
+        <v>288687149.69999999</v>
       </c>
       <c r="F20">
-        <v>15900760.689999999</v>
+        <v>15898961.359999999</v>
       </c>
       <c r="G20">
         <v>176888.92800000001</v>
@@ -2728,25 +2719,25 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B21" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C21">
-        <v>202.83341619999999</v>
+        <v>202.82884859999999</v>
       </c>
       <c r="D21">
-        <v>1121.2180510000001</v>
+        <v>1121.192802</v>
       </c>
       <c r="E21">
-        <v>288709501.89999998</v>
+        <v>288687149.69999999</v>
       </c>
       <c r="F21">
-        <v>6473285.0750000002</v>
+        <v>6474753.7419999996</v>
       </c>
       <c r="G21">
         <v>176888.92800000001</v>
@@ -3129,7 +3120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
@@ -4351,7 +4342,7 @@
         <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36">
         <v>259.95297967002011</v>
       </c>
       <c r="D36">
@@ -4381,25 +4372,25 @@
         <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37">
         <v>206.68334620500781</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37">
         <v>1142.499608188793</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37">
         <v>288656108.20669693</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37">
         <v>7159733.334510237</v>
       </c>
-      <c r="G37" s="6">
-        <v>176888.92800000001</v>
-      </c>
-      <c r="H37" s="6">
+      <c r="G37">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H37">
         <v>32000.007075376881</v>
       </c>
-      <c r="I37" s="6">
+      <c r="I37">
         <v>9.8181474074492936</v>
       </c>
     </row>
@@ -4407,11 +4398,11 @@
       <c r="A38" t="s">
         <v>79</v>
       </c>
-      <c r="B38" s="4" t="str">
+      <c r="B38" t="str">
         <f t="shared" ref="B38:B39" si="2">IF(ISNUMBER(SEARCH("PV", A38)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38">
         <v>252.21409572632879</v>
       </c>
       <c r="D38">
@@ -4437,29 +4428,29 @@
       <c r="A39" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="4" t="str">
+      <c r="B39" t="str">
         <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39">
         <v>198.94446226144731</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39">
         <v>1099.720777500778</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39">
         <v>288656108.2073791</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39">
         <v>5790810.4497479387</v>
       </c>
-      <c r="G39" s="6">
-        <v>176888.92800000001</v>
-      </c>
-      <c r="H39" s="6">
+      <c r="G39">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H39">
         <v>32000.007075376881</v>
       </c>
-      <c r="I39" s="6">
+      <c r="I39">
         <v>9.8181474074492936</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add control run of sensitivity demand 10p down
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBB4F46-32C0-41BA-8148-5A65A735DF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5D2A3D-3D41-48BC-B5E6-DE115A71AA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_operating_points" sheetId="1" r:id="rId1"/>
@@ -520,7 +520,7 @@
                   <c:v>1498.8447471929501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1450</c:v>
+                  <c:v>1455</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1415.6985910000001</c:v>
@@ -2104,7 +2104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB416CA-7C9B-4F0E-AFD4-34077EF25340}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+    <sheetView topLeftCell="C6" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -3120,8 +3120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3277,7 +3277,7 @@
         <v>73</v>
       </c>
       <c r="L3">
-        <v>1450</v>
+        <v>1455</v>
       </c>
       <c r="M3">
         <v>1425</v>

</xml_diff>

<commit_message>
update result comparison file
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5D2A3D-3D41-48BC-B5E6-DE115A71AA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D21903-3EFB-41EF-9DC5-2456E97447FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
+    <workbookView xWindow="-4590" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_operating_points" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
   <si>
     <t>run_name</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>sens_10op_dhprice_10pdown_PV</t>
+  </si>
+  <si>
+    <t>InvCost</t>
   </si>
 </sst>
 </file>
@@ -360,13 +363,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1766,8 +1771,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I39" totalsRowShown="0">
-  <autoFilter ref="A1:I39" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I43" totalsRowShown="0">
+  <autoFilter ref="A1:I43" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8869914E-4BE8-401C-AC76-C6570071019E}" name="run_name"/>
     <tableColumn id="9" xr3:uid="{91B3AAB6-6FBC-4E2C-8674-ECB365CA16C8}" name="PV" dataDxfId="0">
@@ -3118,10 +3123,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3137,7 +3142,7 @@
     <col min="9" max="9" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3186,8 +3191,11 @@
       <c r="Q1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -3243,8 +3251,12 @@
         <f>D8</f>
         <v>1459.447003719521</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R2">
+        <f>D40</f>
+        <v>1326.412694499294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3297,7 +3309,7 @@
         <v>1436.0983060000001</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -3334,7 +3346,7 @@
         <v>1415.6985910000001</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" ref="M4:Q4" si="1">$D$2</f>
+        <f t="shared" ref="M4:R4" si="1">$D$2</f>
         <v>1415.6985910000001</v>
       </c>
       <c r="N4" s="1">
@@ -3353,8 +3365,20 @@
         <f t="shared" si="1"/>
         <v>1415.6985910000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R4" s="1">
+        <f t="shared" si="1"/>
+        <v>1415.6985910000001</v>
+      </c>
+      <c r="T4" s="4">
+        <f>R2/P4</f>
+        <v>0.93693156363344432</v>
+      </c>
+      <c r="U4">
+        <f>1-T4</f>
+        <v>6.306843636655568E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -3406,8 +3430,16 @@
         <f>D30</f>
         <v>1397.35185</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="T5">
+        <f>R6/P4</f>
+        <v>1.0627747572707904</v>
+      </c>
+      <c r="U5">
+        <f>T5-1</f>
+        <v>6.2774757270790404E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3463,8 +3495,12 @@
         <f>D10</f>
         <v>1381.239008</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R6">
+        <f>D42</f>
+        <v>1504.5687264186249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -3494,7 +3530,7 @@
         <v>9.2601513577926973</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -3524,7 +3560,7 @@
         <v>9.3718871360488567</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -3554,7 +3590,7 @@
         <v>9.3718871360488567</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -3584,7 +3620,7 @@
         <v>10.200743660000001</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -3614,7 +3650,7 @@
         <v>10.200743660000001</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -3644,7 +3680,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -3674,7 +3710,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -3704,7 +3740,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -3734,7 +3770,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -4451,6 +4487,126 @@
         <v>32000.007075376881</v>
       </c>
       <c r="I39">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="5" t="str">
+        <f t="shared" ref="B40:B41" si="3">IF(ISNUMBER(SEARCH("PV", A40)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C40">
+        <v>239.95405528630451</v>
+      </c>
+      <c r="D40">
+        <v>1326.412694499294</v>
+      </c>
+      <c r="E40">
+        <v>261493301.12125921</v>
+      </c>
+      <c r="F40">
+        <v>15811545.29718912</v>
+      </c>
+      <c r="G40">
+        <v>176888.9279999978</v>
+      </c>
+      <c r="H40">
+        <v>32000.007075376489</v>
+      </c>
+      <c r="I40">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C41">
+        <v>186.74954755010739</v>
+      </c>
+      <c r="D41">
+        <v>1032.309998957538</v>
+      </c>
+      <c r="E41">
+        <v>261493301.12125921</v>
+      </c>
+      <c r="F41">
+        <v>6400256.9589656191</v>
+      </c>
+      <c r="G41">
+        <v>176888.9279999978</v>
+      </c>
+      <c r="H41">
+        <v>32000.007075376489</v>
+      </c>
+      <c r="I41">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="5" t="str">
+        <f t="shared" ref="B42:B43" si="4">IF(ISNUMBER(SEARCH("PV", A42)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C42">
+        <v>272.18328719130898</v>
+      </c>
+      <c r="D42">
+        <v>1504.5687264186249</v>
+      </c>
+      <c r="E42">
+        <v>315776480.57557988</v>
+      </c>
+      <c r="F42">
+        <v>15983677.849763259</v>
+      </c>
+      <c r="G42">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H42">
+        <v>32000.007075376889</v>
+      </c>
+      <c r="I42">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C43">
+        <v>218.82991316231221</v>
+      </c>
+      <c r="D43">
+        <v>1209.6431310916701</v>
+      </c>
+      <c r="E43">
+        <v>315776480.57557988</v>
+      </c>
+      <c r="F43">
+        <v>6546056.7125909813</v>
+      </c>
+      <c r="G43">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H43">
+        <v>32000.007075376889</v>
+      </c>
+      <c r="I43">
         <v>9.8181474074492936</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update LCEO results comparison
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\Nord_H2ub\Spine_Projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D21903-3EFB-41EF-9DC5-2456E97447FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48F1C6B-C085-4BB8-A1D5-0F5EEBFE71AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4590" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
+    <workbookView xWindow="-4575" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_operating_points" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
   <si>
     <t>run_name</t>
   </si>
@@ -290,6 +290,63 @@
   </si>
   <si>
     <t>InvCost</t>
+  </si>
+  <si>
+    <t>sens_10op_demand_05pdown</t>
+  </si>
+  <si>
+    <t>sens_10op_demand_05pdown_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_demand_05pup</t>
+  </si>
+  <si>
+    <t>sens_10op_demand_05pup_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_dhprice_05pdown</t>
+  </si>
+  <si>
+    <t>sens_10op_dhprice_05pdown_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_dhprice_05pup</t>
+  </si>
+  <si>
+    <t>sens_10op_dhprice_05pup_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_elprice_05pdown</t>
+  </si>
+  <si>
+    <t>sens_10op_elprice_05pdown_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_elprice_05pup</t>
+  </si>
+  <si>
+    <t>sens_10op_elprice_05pup_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_elpricevar_05pdown</t>
+  </si>
+  <si>
+    <t>sens_10op_elpricevar_05pdown_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_elpricevar_05pup</t>
+  </si>
+  <si>
+    <t>sens_10op_invc_05pup</t>
+  </si>
+  <si>
+    <t>sens_10op_invc_05pup_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_invc_05pdown</t>
+  </si>
+  <si>
+    <t>sens_10op_invc_05pdown_PV</t>
   </si>
 </sst>
 </file>
@@ -370,7 +427,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -482,7 +539,7 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
+                  <a:shade val="47000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -522,19 +579,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1498.8447471929501</c:v>
+                  <c:v>1460.0010057815159</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1455</c:v>
+                  <c:v>1418.2136820000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1415.6985910000001</c:v>
+                  <c:v>1380.6135220000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1400</c:v>
+                  <c:v>1346.491194521597</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1347.8877936210879</c:v>
+                  <c:v>1316.106550648097</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -564,7 +621,7 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:shade val="70000"/>
+                  <a:shade val="65000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -604,19 +661,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1436.962304287056</c:v>
+                  <c:v>1402.002937</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1425</c:v>
+                  <c:v>1391.308229</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1415.6985910000001</c:v>
+                  <c:v>1380.6135220000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1410</c:v>
+                  <c:v>1369.9188140002141</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1394.183473598318</c:v>
+                  <c:v>1359.2241063280269</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -646,7 +703,7 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:shade val="90000"/>
+                  <a:shade val="82000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -686,19 +743,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1386.4903242285111</c:v>
+                  <c:v>1351.5309569999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1400</c:v>
+                  <c:v>1364.533322</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1415.6985910000001</c:v>
+                  <c:v>1380.6135220000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1430</c:v>
+                  <c:v>1395.6319209999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1446.2267744709779</c:v>
+                  <c:v>1411.267407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -727,9 +784,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:tint val="90000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -768,19 +823,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1413.163937994756</c:v>
+                  <c:v>1378.204571</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1414</c:v>
+                  <c:v>1379.349964</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1415.6985910000001</c:v>
+                  <c:v>1380.6135220000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1416</c:v>
+                  <c:v>1382.02367</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1417.896003930397</c:v>
+                  <c:v>1382.936637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -810,7 +865,7 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:tint val="70000"/>
+                  <a:tint val="83000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -850,19 +905,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1361.6928989999999</c:v>
+                  <c:v>1326.6078299999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1388.395832366482</c:v>
+                  <c:v>1353.436465</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1415.6985910000001</c:v>
+                  <c:v>1380.6135220000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1443.089109</c:v>
+                  <c:v>1408.129741</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1471.0608961910209</c:v>
+                  <c:v>1435.975827</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -892,7 +947,7 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:tint val="50000"/>
+                  <a:tint val="65000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -932,19 +987,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1459.447003719521</c:v>
+                  <c:v>1424.3619349999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1436.0983060000001</c:v>
+                  <c:v>1401.1389389999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1415.6985910000001</c:v>
+                  <c:v>1380.6135220000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1397.35185</c:v>
+                  <c:v>1362.3924830000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1381.239008</c:v>
+                  <c:v>1346.153939</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -953,6 +1008,65 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-20BE-45F6-B90D-79B066E72F95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>InvCost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="48000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison_sensitivities!$R$2:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1326.412694499294</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1336.1931850000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1380.6135220000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1425.065464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1504.5687264186249</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5045-4939-A37F-BD7B21CF5F42}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1023,8 +1137,8 @@
         <c:axId val="1747965359"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1480"/>
-          <c:min val="1350"/>
+          <c:max val="1510"/>
+          <c:min val="1300"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1687,15 +1801,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:colOff>21590</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>326390</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1771,8 +1885,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I43" totalsRowShown="0">
-  <autoFilter ref="A1:I43" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I62" totalsRowShown="0">
+  <autoFilter ref="A1:I62" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8869914E-4BE8-401C-AC76-C6570071019E}" name="run_name"/>
     <tableColumn id="9" xr3:uid="{91B3AAB6-6FBC-4E2C-8674-ECB365CA16C8}" name="PV" dataDxfId="0">
@@ -2109,23 +2223,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB416CA-7C9B-4F0E-AFD4-34077EF25340}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" customWidth="1"/>
-    <col min="7" max="7" width="25.08984375" customWidth="1"/>
-    <col min="8" max="8" width="21.1796875" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="1" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2154,7 +2268,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2163,16 +2277,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C2">
-        <v>256.10627770000002</v>
+        <v>249.7592301</v>
       </c>
       <c r="D2">
-        <v>1415.6985910000001</v>
+        <v>1380.6135220000001</v>
       </c>
       <c r="E2">
         <v>288656108.19999999</v>
       </c>
       <c r="F2">
-        <v>15902102.699999999</v>
+        <v>14779380.25</v>
       </c>
       <c r="G2">
         <v>176888.92800000001</v>
@@ -2184,7 +2298,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2193,16 +2307,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C3">
-        <v>202.8139042</v>
+        <v>196.4895966</v>
       </c>
       <c r="D3">
-        <v>1121.110193</v>
+        <v>1086.1508260000001</v>
       </c>
       <c r="E3">
         <v>288656108.19999999</v>
       </c>
       <c r="F3">
-        <v>6475271.892</v>
+        <v>5356571.892</v>
       </c>
       <c r="G3">
         <v>176888.92800000001</v>
@@ -2214,7 +2328,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2223,16 +2337,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C4">
-        <v>254.96266482664441</v>
+        <v>248.61588475600149</v>
       </c>
       <c r="D4">
-        <v>1409.3769527917291</v>
+        <v>1374.293362956786</v>
       </c>
       <c r="E4">
         <v>286911074.34615147</v>
       </c>
       <c r="F4">
-        <v>15877545.80322974</v>
+        <v>14754870.68028195</v>
       </c>
       <c r="G4">
         <v>176888.92800000001</v>
@@ -2244,7 +2358,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2253,16 +2367,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C5">
-        <v>201.2788905306509</v>
+        <v>194.9545828837642</v>
       </c>
       <c r="D5">
-        <v>1112.6249782110981</v>
+        <v>1077.665610940807</v>
       </c>
       <c r="E5">
         <v>286911074.34615147</v>
       </c>
       <c r="F5">
-        <v>6381480.5170174837</v>
+        <v>5262780.5170174837</v>
       </c>
       <c r="G5">
         <v>176888.92800000001</v>
@@ -2274,7 +2388,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2283,28 +2397,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C6">
-        <v>255.44107389999999</v>
+        <v>249.09406839490649</v>
       </c>
       <c r="D6">
-        <v>1412.0214920000001</v>
+        <v>1376.936655849622</v>
       </c>
       <c r="E6">
-        <v>287398388.39999998</v>
+        <v>287398388.41068858</v>
       </c>
       <c r="F6">
-        <v>15912537.050000001</v>
+        <v>14789822.057691149</v>
       </c>
       <c r="G6">
-        <v>176888.92800000001</v>
+        <v>176888.9279999994</v>
       </c>
       <c r="H6">
-        <v>32000.007079999999</v>
+        <v>32000.00707537678</v>
       </c>
       <c r="I6">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2313,28 +2427,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C7">
-        <v>201.8789865</v>
+        <v>195.5546788889136</v>
       </c>
       <c r="D7">
-        <v>1115.942176</v>
+        <v>1080.9828083026059</v>
       </c>
       <c r="E7">
-        <v>287398388.39999998</v>
+        <v>287398388.41068858</v>
       </c>
       <c r="F7">
-        <v>6437996.8420000002</v>
+        <v>5319296.8422016567</v>
       </c>
       <c r="G7">
-        <v>176888.92800000001</v>
+        <v>176888.9279999994</v>
       </c>
       <c r="H7">
-        <v>32000.007079999999</v>
+        <v>32000.00707537678</v>
       </c>
       <c r="I7">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2343,28 +2457,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C8">
-        <v>255.86895699999999</v>
+        <v>249.52192327091299</v>
       </c>
       <c r="D8">
-        <v>1414.386735</v>
+        <v>1379.3017425253249</v>
       </c>
       <c r="E8">
-        <v>288262500</v>
+        <v>288262499.99587762</v>
       </c>
       <c r="F8">
-        <v>15900213.17</v>
+        <v>14777493.17442679</v>
       </c>
       <c r="G8">
-        <v>176888.92800000001</v>
+        <v>176888.92800000121</v>
       </c>
       <c r="H8">
-        <v>32000.007079999999</v>
+        <v>32000.007075377111</v>
       </c>
       <c r="I8">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2373,28 +2487,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C9">
-        <v>202.50746839999999</v>
+        <v>196.18316071306151</v>
       </c>
       <c r="D9">
-        <v>1119.416283</v>
+        <v>1084.4569161638681</v>
       </c>
       <c r="E9">
-        <v>288262500</v>
+        <v>288262499.99587762</v>
       </c>
       <c r="F9">
-        <v>6461156.6449999996</v>
+        <v>5342456.6447218359</v>
       </c>
       <c r="G9">
-        <v>176888.92800000001</v>
+        <v>176888.92800000121</v>
       </c>
       <c r="H9">
-        <v>32000.007079999999</v>
+        <v>32000.007075377111</v>
       </c>
       <c r="I9">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2403,16 +2517,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C10">
-        <v>256.08701760000002</v>
+        <v>249.74026509999999</v>
       </c>
       <c r="D10">
-        <v>1415.5921249999999</v>
+        <v>1380.5086879999999</v>
       </c>
       <c r="E10">
         <v>288545796.10000002</v>
       </c>
       <c r="F10">
-        <v>15909931.33</v>
+        <v>14787261.09</v>
       </c>
       <c r="G10">
         <v>176888.92800000001</v>
@@ -2424,7 +2538,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2433,16 +2547,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C11">
-        <v>202.75017940000001</v>
+        <v>196.42587169999999</v>
       </c>
       <c r="D11">
-        <v>1120.757936</v>
+        <v>1085.798569</v>
       </c>
       <c r="E11">
         <v>288545796.10000002</v>
       </c>
       <c r="F11">
-        <v>6475235.2039999999</v>
+        <v>5356535.2039999999</v>
       </c>
       <c r="G11">
         <v>176888.92800000001</v>
@@ -2454,7 +2568,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2463,16 +2577,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C12">
-        <v>255.97229770000001</v>
+        <v>249.62509220000001</v>
       </c>
       <c r="D12">
-        <v>1414.957979</v>
+        <v>1379.8720370000001</v>
       </c>
       <c r="E12">
         <v>288420132.5</v>
       </c>
       <c r="F12">
-        <v>15902437.77</v>
+        <v>14779687.390000001</v>
       </c>
       <c r="G12">
         <v>176888.92800000001</v>
@@ -2484,7 +2598,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2493,16 +2607,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C13">
-        <v>202.6404757</v>
+        <v>196.316168</v>
       </c>
       <c r="D13">
-        <v>1120.1515179999999</v>
+        <v>1085.192151</v>
       </c>
       <c r="E13">
         <v>288420132.5</v>
       </c>
       <c r="F13">
-        <v>6468628.9440000001</v>
+        <v>5349928.9440000001</v>
       </c>
       <c r="G13">
         <v>176888.92800000001</v>
@@ -2514,7 +2628,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2523,28 +2637,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C14">
-        <v>256.12943489999998</v>
+        <v>249.78260672031831</v>
       </c>
       <c r="D14">
-        <v>1415.8265980000001</v>
+        <v>1380.742742703982</v>
       </c>
       <c r="E14">
-        <v>288709501.89999998</v>
+        <v>288709501.92547369</v>
       </c>
       <c r="F14">
-        <v>15900760.689999999</v>
+        <v>14778077.05646155</v>
       </c>
       <c r="G14">
         <v>176888.92800000001</v>
       </c>
       <c r="H14">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I14">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2553,28 +2667,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C15">
-        <v>202.83341619999999</v>
+        <v>196.5091085550917</v>
       </c>
       <c r="D15">
-        <v>1121.2180510000001</v>
+        <v>1086.258683401757</v>
       </c>
       <c r="E15">
-        <v>288709501.89999998</v>
+        <v>288709501.92547369</v>
       </c>
       <c r="F15">
-        <v>6473285.0750000002</v>
+        <v>5354585.0752046481</v>
       </c>
       <c r="G15">
         <v>176888.92800000001</v>
       </c>
       <c r="H15">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I15">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -2583,16 +2697,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C16">
-        <v>256.07102687952232</v>
+        <v>249.7243263809365</v>
       </c>
       <c r="D16">
-        <v>1415.5037319173589</v>
+        <v>1380.4205819390661</v>
       </c>
       <c r="E16">
         <v>288705429.34616148</v>
       </c>
       <c r="F16">
-        <v>15890843.7584353</v>
+        <v>14768182.710903389</v>
       </c>
       <c r="G16">
         <v>176888.92800000001</v>
@@ -2604,7 +2718,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2613,16 +2727,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C17">
-        <v>202.75983826205081</v>
+        <v>196.43553061516411</v>
       </c>
       <c r="D17">
-        <v>1120.8113281707811</v>
+        <v>1085.85196090049</v>
       </c>
       <c r="E17">
         <v>288705429.34616148</v>
       </c>
       <c r="F17">
-        <v>6460684.7534849672</v>
+        <v>5341984.7534849672</v>
       </c>
       <c r="G17">
         <v>176888.92800000001</v>
@@ -2634,7 +2748,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -2643,28 +2757,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C18">
-        <v>256.04429678074212</v>
+        <v>249.71998909999999</v>
       </c>
       <c r="D18">
-        <v>1415.3559738713241</v>
+        <v>1380.3966069999999</v>
       </c>
       <c r="E18">
-        <v>288557068.64214009</v>
+        <v>288557068.60000002</v>
       </c>
       <c r="F18">
-        <v>15901226.36532389</v>
+        <v>14782526.369999999</v>
       </c>
       <c r="G18">
         <v>176888.92800000001</v>
       </c>
       <c r="H18">
-        <v>32000.0070753769</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I18">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2673,28 +2787,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C19">
-        <v>202.7734041647862</v>
+        <v>196.4490965</v>
       </c>
       <c r="D19">
-        <v>1120.8863174664571</v>
+        <v>1085.92695</v>
       </c>
       <c r="E19">
-        <v>288557068.64214009</v>
+        <v>288557068.60000002</v>
       </c>
       <c r="F19">
-        <v>6478195.2768843267</v>
+        <v>5359495.2769999998</v>
       </c>
       <c r="G19">
         <v>176888.92800000001</v>
       </c>
       <c r="H19">
-        <v>32000.0070753769</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I19">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -2703,28 +2817,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C20">
-        <v>256.1063924</v>
+        <v>249.75918061460271</v>
       </c>
       <c r="D20">
-        <v>1415.6992250000001</v>
+        <v>1380.613248397387</v>
       </c>
       <c r="E20">
-        <v>288687149.69999999</v>
+        <v>288687149.67850941</v>
       </c>
       <c r="F20">
-        <v>15898961.359999999</v>
+        <v>14776209.863460001</v>
       </c>
       <c r="G20">
-        <v>176888.92800000001</v>
+        <v>176888.92800000089</v>
       </c>
       <c r="H20">
-        <v>32000.007079999999</v>
+        <v>32000.007075377049</v>
       </c>
       <c r="I20">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2733,25 +2847,25 @@
         <v>PV revenue</v>
       </c>
       <c r="C21">
-        <v>202.82884859999999</v>
+        <v>196.50454094876159</v>
       </c>
       <c r="D21">
-        <v>1121.192802</v>
+        <v>1086.2334346889879</v>
       </c>
       <c r="E21">
-        <v>288687149.69999999</v>
+        <v>288687149.67850941</v>
       </c>
       <c r="F21">
-        <v>6474753.7419999996</v>
+        <v>5356053.7419430511</v>
       </c>
       <c r="G21">
-        <v>176888.92800000001</v>
+        <v>176888.92800000089</v>
       </c>
       <c r="H21">
-        <v>32000.007079999999</v>
+        <v>32000.007075377049</v>
       </c>
       <c r="I21">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
   </sheetData>
@@ -2767,22 +2881,22 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.1796875" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="1" max="2" width="11.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="16.90625" customWidth="1"/>
-    <col min="6" max="6" width="13.90625" customWidth="1"/>
-    <col min="7" max="7" width="24.1796875" customWidth="1"/>
-    <col min="8" max="8" width="20.6328125" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="24.21875" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2817,7 +2931,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2826,16 +2940,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C2">
-        <v>256.10627770000002</v>
+        <v>249.7592301</v>
       </c>
       <c r="D2">
-        <v>1415.6985910000001</v>
+        <v>1380.6135220000001</v>
       </c>
       <c r="E2">
         <v>288656108.19999999</v>
       </c>
       <c r="F2">
-        <v>15902102.699999999</v>
+        <v>14779380.25</v>
       </c>
       <c r="G2">
         <v>176888.92800000001</v>
@@ -2854,7 +2968,7 @@
         <v>43.057462085171316</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2863,16 +2977,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C3">
-        <v>202.8139042</v>
+        <v>196.4895966</v>
       </c>
       <c r="D3">
-        <v>1121.110193</v>
+        <v>1086.1508260000001</v>
       </c>
       <c r="E3">
         <v>288656108.19999999</v>
       </c>
       <c r="F3">
-        <v>6475271.892</v>
+        <v>5356571.892</v>
       </c>
       <c r="G3">
         <v>176888.92800000001</v>
@@ -2891,7 +3005,7 @@
         <v>43.057462085171316</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2900,25 +3014,25 @@
         <v>no PV revenue</v>
       </c>
       <c r="C4">
-        <v>254.9626648</v>
+        <v>248.61588475600149</v>
       </c>
       <c r="D4">
-        <v>1409.376953</v>
+        <v>1374.293362956786</v>
       </c>
       <c r="E4">
-        <v>286911074.30000001</v>
+        <v>286911074.34615147</v>
       </c>
       <c r="F4">
-        <v>15877545.800000001</v>
+        <v>14754870.68028195</v>
       </c>
       <c r="G4">
         <v>176888.92800000001</v>
       </c>
       <c r="H4">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I4">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
       <c r="J4">
         <v>0.81315475028895645</v>
@@ -2928,7 +3042,7 @@
         <v>42.284047015025735</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2937,25 +3051,25 @@
         <v>PV revenue</v>
       </c>
       <c r="C5">
-        <v>201.27889049999999</v>
+        <v>194.9545828837642</v>
       </c>
       <c r="D5">
-        <v>1112.6249780000001</v>
+        <v>1077.665610940807</v>
       </c>
       <c r="E5">
-        <v>286911074.30000001</v>
+        <v>286911074.34615147</v>
       </c>
       <c r="F5">
-        <v>6381480.517</v>
+        <v>5262780.5170174837</v>
       </c>
       <c r="G5">
         <v>176888.92800000001</v>
       </c>
       <c r="H5">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I5">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
       <c r="J5">
         <v>0.81315475028895645</v>
@@ -2965,7 +3079,7 @@
         <v>42.284047015025735</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2974,25 +3088,25 @@
         <v>no PV revenue</v>
       </c>
       <c r="C6">
-        <v>654.69774659999996</v>
+        <v>641.50005133764728</v>
       </c>
       <c r="D6">
-        <v>3619.023655</v>
+        <v>3546.0697282275501</v>
       </c>
       <c r="E6">
-        <v>458916187.89999998</v>
+        <v>458916187.90332049</v>
       </c>
       <c r="F6">
-        <v>8753696.3499999996</v>
+        <v>7634996.349609375</v>
       </c>
       <c r="G6">
-        <v>84764.800310000006</v>
+        <v>84764.800312762542</v>
       </c>
       <c r="H6">
-        <v>15334.335730000001</v>
+        <v>15334.335734972119</v>
       </c>
       <c r="I6">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -3002,7 +3116,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -3011,25 +3125,25 @@
         <v>PV revenue</v>
       </c>
       <c r="C7">
-        <v>654.69774659999996</v>
+        <v>641.50005133764728</v>
       </c>
       <c r="D7">
-        <v>3619.023655</v>
+        <v>3546.0697282275501</v>
       </c>
       <c r="E7">
-        <v>458916187.89999998</v>
+        <v>458916187.90332049</v>
       </c>
       <c r="F7">
-        <v>8753696.3499999996</v>
+        <v>7634996.349609375</v>
       </c>
       <c r="G7">
-        <v>84764.800310000006</v>
+        <v>84764.800312762542</v>
       </c>
       <c r="H7">
-        <v>15334.335730000001</v>
+        <v>15334.335734972119</v>
       </c>
       <c r="I7">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -3039,7 +3153,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -3048,25 +3162,25 @@
         <v>no PV revenue</v>
       </c>
       <c r="C8">
-        <v>174.12765110000001</v>
+        <v>167.80334348718441</v>
       </c>
       <c r="D8">
-        <v>962.53896039999995</v>
+        <v>927.5795931652691</v>
       </c>
       <c r="E8">
-        <v>144513502.90000001</v>
+        <v>144513502.90635639</v>
       </c>
       <c r="F8">
-        <v>16082234.07</v>
+        <v>14963534.068480629</v>
       </c>
       <c r="G8">
         <v>176888.92800000001</v>
       </c>
       <c r="H8">
-        <v>32000.007079999999</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I8">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -3076,7 +3190,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -3085,25 +3199,25 @@
         <v>PV revenue</v>
       </c>
       <c r="C9">
-        <v>136.75785540000001</v>
+        <v>130.43354777569829</v>
       </c>
       <c r="D9">
-        <v>755.96703409999998</v>
+        <v>721.00766687122098</v>
       </c>
       <c r="E9">
-        <v>144513502.90000001</v>
+        <v>144513502.90635639</v>
       </c>
       <c r="F9">
-        <v>9471930.9649999999</v>
+        <v>8353230.9654968567</v>
       </c>
       <c r="G9">
         <v>176888.92800000001</v>
       </c>
       <c r="H9">
-        <v>32000.007079999999</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I9">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -3123,26 +3237,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
-  <dimension ref="A1:U43"/>
+  <dimension ref="A1:U62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="16.90625" customWidth="1"/>
-    <col min="6" max="6" width="13.90625" customWidth="1"/>
-    <col min="7" max="7" width="24.1796875" customWidth="1"/>
-    <col min="8" max="8" width="20.6328125" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="24.21875" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3307,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -3204,16 +3316,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C2">
-        <v>256.10627770000002</v>
+        <v>249.7592301</v>
       </c>
       <c r="D2">
-        <v>1415.6985910000001</v>
+        <v>1380.6135220000001</v>
       </c>
       <c r="E2">
         <v>288656108.19999999</v>
       </c>
       <c r="F2">
-        <v>15902102.699999999</v>
+        <v>14779380.25</v>
       </c>
       <c r="G2">
         <v>176888.92800000001</v>
@@ -3229,34 +3341,34 @@
       </c>
       <c r="L2">
         <f>D32</f>
-        <v>1498.8447471929501</v>
+        <v>1460.0010057815159</v>
       </c>
       <c r="M2">
         <f>D36</f>
-        <v>1436.962304287056</v>
+        <v>1402.002937</v>
       </c>
       <c r="N2">
         <f>D16</f>
-        <v>1386.4903242285111</v>
+        <v>1351.5309569999999</v>
       </c>
       <c r="O2">
         <f>D20</f>
-        <v>1413.163937994756</v>
+        <v>1378.204571</v>
       </c>
       <c r="P2">
         <f>D4</f>
-        <v>1361.6928989999999</v>
+        <v>1326.6078299999999</v>
       </c>
       <c r="Q2">
         <f>D8</f>
-        <v>1459.447003719521</v>
+        <v>1424.3619349999999</v>
       </c>
       <c r="R2">
         <f>D40</f>
         <v>1326.412694499294</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3265,16 +3377,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C3">
-        <v>202.8139042</v>
+        <v>196.4895966</v>
       </c>
       <c r="D3">
-        <v>1121.110193</v>
+        <v>1086.1508260000001</v>
       </c>
       <c r="E3">
         <v>288656108.19999999</v>
       </c>
       <c r="F3">
-        <v>6475271.892</v>
+        <v>5356571.892</v>
       </c>
       <c r="G3">
         <v>176888.92800000001</v>
@@ -3289,27 +3401,35 @@
         <v>73</v>
       </c>
       <c r="L3">
-        <v>1455</v>
+        <f>D44</f>
+        <v>1418.2136820000001</v>
       </c>
       <c r="M3">
-        <v>1425</v>
+        <f>D48</f>
+        <v>1391.308229</v>
       </c>
       <c r="N3">
-        <v>1400</v>
+        <f>D52</f>
+        <v>1364.533322</v>
       </c>
       <c r="O3">
-        <v>1414</v>
+        <f>D56</f>
+        <v>1379.349964</v>
       </c>
       <c r="P3">
         <f>D24</f>
-        <v>1388.395832366482</v>
+        <v>1353.436465</v>
       </c>
       <c r="Q3">
         <f>D28</f>
-        <v>1436.0983060000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+        <v>1401.1389389999999</v>
+      </c>
+      <c r="R3">
+        <f>D61</f>
+        <v>1336.1931850000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -3318,16 +3438,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C4">
-        <v>246.33640389999999</v>
+        <v>239.9893563</v>
       </c>
       <c r="D4">
-        <v>1361.6928989999999</v>
+        <v>1326.6078299999999</v>
       </c>
       <c r="E4">
         <v>288656108.19999999</v>
       </c>
       <c r="F4">
-        <v>15902102.699999999</v>
+        <v>14779380.25</v>
       </c>
       <c r="G4">
         <v>176888.92800000001</v>
@@ -3343,42 +3463,42 @@
       </c>
       <c r="L4" s="1">
         <f>$D$2</f>
-        <v>1415.6985910000001</v>
+        <v>1380.6135220000001</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" ref="M4:R4" si="1">$D$2</f>
-        <v>1415.6985910000001</v>
+        <v>1380.6135220000001</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" si="1"/>
-        <v>1415.6985910000001</v>
+        <v>1380.6135220000001</v>
       </c>
       <c r="O4" s="1">
         <f t="shared" si="1"/>
-        <v>1415.6985910000001</v>
+        <v>1380.6135220000001</v>
       </c>
       <c r="P4" s="1">
         <f t="shared" si="1"/>
-        <v>1415.6985910000001</v>
+        <v>1380.6135220000001</v>
       </c>
       <c r="Q4" s="1">
         <f t="shared" si="1"/>
-        <v>1415.6985910000001</v>
+        <v>1380.6135220000001</v>
       </c>
       <c r="R4" s="1">
         <f t="shared" si="1"/>
-        <v>1415.6985910000001</v>
+        <v>1380.6135220000001</v>
       </c>
       <c r="T4" s="4">
         <f>R2/P4</f>
-        <v>0.93693156363344432</v>
+        <v>0.96074149163613209</v>
       </c>
       <c r="U4">
         <f>1-T4</f>
-        <v>6.306843636655568E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+        <v>3.9258508363867906E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -3387,16 +3507,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C5">
-        <v>193.0440304</v>
+        <v>186.7197228</v>
       </c>
       <c r="D5">
-        <v>1067.1045019999999</v>
+        <v>1032.1451340000001</v>
       </c>
       <c r="E5">
         <v>288656108.19999999</v>
       </c>
       <c r="F5">
-        <v>6475271.892</v>
+        <v>5356571.892</v>
       </c>
       <c r="G5">
         <v>176888.92800000001</v>
@@ -3411,35 +3531,43 @@
         <v>74</v>
       </c>
       <c r="L5">
-        <v>1400</v>
+        <f>D46</f>
+        <v>1346.491194521597</v>
       </c>
       <c r="M5">
-        <v>1410</v>
+        <f>D50</f>
+        <v>1369.9188140002141</v>
       </c>
       <c r="N5">
-        <v>1430</v>
+        <f>D54</f>
+        <v>1395.6319209999999</v>
       </c>
       <c r="O5">
-        <v>1416</v>
+        <f>D58</f>
+        <v>1382.02367</v>
       </c>
       <c r="P5">
         <f>D26</f>
-        <v>1443.089109</v>
+        <v>1408.129741</v>
       </c>
       <c r="Q5">
         <f>D30</f>
-        <v>1397.35185</v>
+        <v>1362.3924830000001</v>
+      </c>
+      <c r="R5">
+        <f>D59</f>
+        <v>1425.065464</v>
       </c>
       <c r="T5">
         <f>R6/P4</f>
-        <v>1.0627747572707904</v>
+        <v>1.0897826962023807</v>
       </c>
       <c r="U5">
         <f>T5-1</f>
-        <v>6.2774757270790404E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+        <v>8.9782696202380663E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3448,59 +3576,59 @@
         <v>no PV revenue</v>
       </c>
       <c r="C6">
-        <v>266.12156916018472</v>
+        <v>259.77452149999999</v>
       </c>
       <c r="D6">
-        <v>1471.0608961910209</v>
+        <v>1435.975827</v>
       </c>
       <c r="E6">
-        <v>288656108.20733207</v>
+        <v>288656108.19999999</v>
       </c>
       <c r="F6">
-        <v>15902102.703706119</v>
+        <v>14779380.25</v>
       </c>
       <c r="G6">
-        <v>176888.9279999992</v>
+        <v>176888.92800000001</v>
       </c>
       <c r="H6">
-        <v>32000.00707537675</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I6">
-        <v>9.2601513577926973</v>
+        <v>9.2601513579999999</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>71</v>
       </c>
       <c r="L6">
         <f>D34</f>
-        <v>1347.8877936210879</v>
+        <v>1316.106550648097</v>
       </c>
       <c r="M6">
         <f>D38</f>
-        <v>1394.183473598318</v>
+        <v>1359.2241063280269</v>
       </c>
       <c r="N6">
         <f>D18</f>
-        <v>1446.2267744709779</v>
+        <v>1411.267407</v>
       </c>
       <c r="O6">
         <f>D22</f>
-        <v>1417.896003930397</v>
+        <v>1382.936637</v>
       </c>
       <c r="P6">
         <f>D6</f>
-        <v>1471.0608961910209</v>
+        <v>1435.975827</v>
       </c>
       <c r="Q6">
         <f>D10</f>
-        <v>1381.239008</v>
+        <v>1346.153939</v>
       </c>
       <c r="R6">
         <f>D42</f>
         <v>1504.5687264186249</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -3509,28 +3637,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C7">
-        <v>212.82919570205911</v>
+        <v>206.50488809999999</v>
       </c>
       <c r="D7">
-        <v>1176.47249846416</v>
+        <v>1141.5131309999999</v>
       </c>
       <c r="E7">
-        <v>288656108.20733207</v>
+        <v>288656108.19999999</v>
       </c>
       <c r="F7">
-        <v>6475271.8921226691</v>
+        <v>5356571.892</v>
       </c>
       <c r="G7">
-        <v>176888.9279999992</v>
+        <v>176888.92800000001</v>
       </c>
       <c r="H7">
-        <v>32000.00707537675</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I7">
-        <v>9.2601513577926973</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+        <v>9.2601513579999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -3539,28 +3667,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C8">
-        <v>264.02056348694862</v>
+        <v>257.67351580000002</v>
       </c>
       <c r="D8">
-        <v>1459.447003719521</v>
+        <v>1424.3619349999999</v>
       </c>
       <c r="E8">
-        <v>288656108.20733207</v>
+        <v>288656108.19999999</v>
       </c>
       <c r="F8">
-        <v>15902102.703706119</v>
+        <v>14779380.25</v>
       </c>
       <c r="G8">
-        <v>176888.9279999992</v>
+        <v>176888.92800000001</v>
       </c>
       <c r="H8">
-        <v>32000.00707537675</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I8">
-        <v>9.3718871360488567</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+        <v>9.3718871359999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -3569,28 +3697,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C9">
-        <v>210.72819002882301</v>
+        <v>204.40388239999999</v>
       </c>
       <c r="D9">
-        <v>1164.8586059926599</v>
+        <v>1129.8992390000001</v>
       </c>
       <c r="E9">
-        <v>288656108.20733207</v>
+        <v>288656108.19999999</v>
       </c>
       <c r="F9">
-        <v>6475271.8921226691</v>
+        <v>5356571.892</v>
       </c>
       <c r="G9">
-        <v>176888.9279999992</v>
+        <v>176888.92800000001</v>
       </c>
       <c r="H9">
-        <v>32000.00707537675</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I9">
-        <v>9.3718871360488567</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+        <v>9.3718871359999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -3599,16 +3727,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C10">
-        <v>249.87238339999999</v>
+        <v>243.52533579999999</v>
       </c>
       <c r="D10">
-        <v>1381.239008</v>
+        <v>1346.153939</v>
       </c>
       <c r="E10">
         <v>288656108.19999999</v>
       </c>
       <c r="F10">
-        <v>15902102.699999999</v>
+        <v>14779380.25</v>
       </c>
       <c r="G10">
         <v>176888.92800000001</v>
@@ -3620,7 +3748,7 @@
         <v>10.200743660000001</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -3629,16 +3757,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C11">
-        <v>196.58000989999999</v>
+        <v>190.2557023</v>
       </c>
       <c r="D11">
-        <v>1086.6506099999999</v>
+        <v>1051.691243</v>
       </c>
       <c r="E11">
         <v>288656108.19999999</v>
       </c>
       <c r="F11">
-        <v>6475271.892</v>
+        <v>5356571.892</v>
       </c>
       <c r="G11">
         <v>176888.92800000001</v>
@@ -3650,7 +3778,7 @@
         <v>10.200743660000001</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -3659,28 +3787,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C12">
-        <v>272.18328719130898</v>
+        <v>265.85897949999998</v>
       </c>
       <c r="D12">
-        <v>1504.5687264186249</v>
+        <v>1469.609359</v>
       </c>
       <c r="E12">
-        <v>315776480.57557988</v>
+        <v>315776480.60000002</v>
       </c>
       <c r="F12">
-        <v>15983677.849763259</v>
+        <v>14864977.85</v>
       </c>
       <c r="G12">
         <v>176888.92800000001</v>
       </c>
       <c r="H12">
-        <v>32000.007075376889</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I12">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -3689,28 +3817,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C13">
-        <v>218.82991316231221</v>
+        <v>212.5056055</v>
       </c>
       <c r="D13">
-        <v>1209.6431310916701</v>
+        <v>1174.6837640000001</v>
       </c>
       <c r="E13">
-        <v>315776480.57557988</v>
+        <v>315776480.60000002</v>
       </c>
       <c r="F13">
-        <v>6546056.7125909813</v>
+        <v>5427356.7130000005</v>
       </c>
       <c r="G13">
         <v>176888.92800000001</v>
       </c>
       <c r="H13">
-        <v>32000.007075376889</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I13">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -3719,16 +3847,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C14">
-        <v>239.95405529999999</v>
+        <v>233.6297476</v>
       </c>
       <c r="D14">
-        <v>1326.4126940000001</v>
+        <v>1291.4533269999999</v>
       </c>
       <c r="E14">
         <v>261493301.09999999</v>
       </c>
       <c r="F14">
-        <v>15811545.300000001</v>
+        <v>14692845.300000001</v>
       </c>
       <c r="G14">
         <v>176888.92800000001</v>
@@ -3740,7 +3868,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -3749,16 +3877,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C15">
-        <v>186.7495476</v>
+        <v>180.42523990000001</v>
       </c>
       <c r="D15">
-        <v>1032.3099990000001</v>
+        <v>997.35063170000001</v>
       </c>
       <c r="E15">
         <v>261493301.09999999</v>
       </c>
       <c r="F15">
-        <v>6400256.9589999998</v>
+        <v>5281556.9589999998</v>
       </c>
       <c r="G15">
         <v>176888.92800000001</v>
@@ -3770,7 +3898,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -3779,28 +3907,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C16">
-        <v>250.82237021219291</v>
+        <v>244.4980626</v>
       </c>
       <c r="D16">
-        <v>1386.4903242285111</v>
+        <v>1351.5309569999999</v>
       </c>
       <c r="E16">
-        <v>286416416.59819239</v>
+        <v>286416416.60000002</v>
       </c>
       <c r="F16">
-        <v>15195555.51151634</v>
+        <v>14076855.51</v>
       </c>
       <c r="G16">
         <v>176888.92800000001</v>
       </c>
       <c r="H16">
-        <v>32000.007075376881</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I16">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -3809,28 +3937,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C17">
-        <v>203.0448735543693</v>
+        <v>196.7205659</v>
       </c>
       <c r="D17">
-        <v>1122.386939925542</v>
+        <v>1087.4275729999999</v>
       </c>
       <c r="E17">
-        <v>286416416.59819239</v>
+        <v>286416416.60000002</v>
       </c>
       <c r="F17">
-        <v>6744245.3451903481</v>
+        <v>5625545.3449999997</v>
       </c>
       <c r="G17">
         <v>176888.92800000001</v>
       </c>
       <c r="H17">
-        <v>32000.007075376881</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I17">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3839,28 +3967,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C18">
-        <v>261.62896422590558</v>
+        <v>255.30465659999999</v>
       </c>
       <c r="D18">
-        <v>1446.2267744709779</v>
+        <v>1411.267407</v>
       </c>
       <c r="E18">
-        <v>291333845.31250137</v>
+        <v>291333845.30000001</v>
       </c>
       <c r="F18">
-        <v>16606271.365649</v>
+        <v>15487571.369999999</v>
       </c>
       <c r="G18">
-        <v>176888.9279999944</v>
+        <v>176888.92800000001</v>
       </c>
       <c r="H18">
-        <v>32000.007075375881</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I18">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -3869,28 +3997,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C19">
-        <v>202.72789291196949</v>
+        <v>196.4035853</v>
       </c>
       <c r="D19">
-        <v>1120.6347413744979</v>
+        <v>1085.6753739999999</v>
       </c>
       <c r="E19">
-        <v>291333845.31250137</v>
+        <v>291333845.30000001</v>
       </c>
       <c r="F19">
-        <v>6187324.0028756075</v>
+        <v>5068624.0029999996</v>
       </c>
       <c r="G19">
-        <v>176888.9279999944</v>
+        <v>176888.92800000001</v>
       </c>
       <c r="H19">
-        <v>32000.007075375881</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I19">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -3899,28 +4027,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C20">
-        <v>255.64774757694079</v>
+        <v>249.32343990000001</v>
       </c>
       <c r="D20">
-        <v>1413.163937994756</v>
+        <v>1378.204571</v>
       </c>
       <c r="E20">
-        <v>287503256.69952732</v>
+        <v>287503256.69999999</v>
       </c>
       <c r="F20">
-        <v>15938414.275803531</v>
+        <v>14819714.279999999</v>
       </c>
       <c r="G20">
         <v>176888.92800000001</v>
       </c>
       <c r="H20">
-        <v>32000.007075376889</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I20">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -3929,28 +4057,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C21">
-        <v>202.42988825992089</v>
+        <v>196.1055806</v>
       </c>
       <c r="D21">
-        <v>1118.987437881229</v>
+        <v>1084.028071</v>
       </c>
       <c r="E21">
-        <v>287503256.69952732</v>
+        <v>287503256.69999999</v>
       </c>
       <c r="F21">
-        <v>6524764.1907610623</v>
+        <v>5406064.1909999996</v>
       </c>
       <c r="G21">
         <v>176888.92800000001</v>
       </c>
       <c r="H21">
-        <v>32000.007075376889</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I21">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -3959,28 +4087,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C22">
-        <v>256.50379970600142</v>
+        <v>250.1794921</v>
       </c>
       <c r="D22">
-        <v>1417.896003930397</v>
+        <v>1382.936637</v>
       </c>
       <c r="E22">
-        <v>289790455.41130489</v>
+        <v>289790455.39999998</v>
       </c>
       <c r="F22">
-        <v>15856884.178413169</v>
+        <v>14738184.18</v>
       </c>
       <c r="G22">
         <v>176888.92800000001</v>
       </c>
       <c r="H22">
-        <v>32000.007075376889</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I22">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -3989,28 +4117,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C23">
-        <v>203.14207603492159</v>
+        <v>196.81776840000001</v>
       </c>
       <c r="D23">
-        <v>1122.9242536374829</v>
+        <v>1087.964886</v>
       </c>
       <c r="E23">
-        <v>289790455.41130489</v>
+        <v>289790455.39999998</v>
       </c>
       <c r="F23">
-        <v>6417786.0820036363</v>
+        <v>5299086.0820000004</v>
       </c>
       <c r="G23">
         <v>176888.92800000001</v>
       </c>
       <c r="H23">
-        <v>32000.007075376889</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I23">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -4019,28 +4147,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C24">
-        <v>251.16708525222791</v>
+        <v>244.84277760000001</v>
       </c>
       <c r="D24">
-        <v>1388.395832366482</v>
+        <v>1353.436465</v>
       </c>
       <c r="E24">
-        <v>288656108.20733207</v>
+        <v>288656108.19999999</v>
       </c>
       <c r="F24">
-        <v>15898080.2506778</v>
+        <v>14779380.25</v>
       </c>
       <c r="G24">
-        <v>176888.9279999992</v>
+        <v>176888.92800000001</v>
       </c>
       <c r="H24">
-        <v>32000.00707537675</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I24">
-        <v>10.117422927236451</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+        <v>10.11742293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -4049,28 +4177,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C25">
-        <v>197.89745178735001</v>
+        <v>191.57314410000001</v>
       </c>
       <c r="D25">
-        <v>1093.9331362689629</v>
+        <v>1058.9737689999999</v>
       </c>
       <c r="E25">
-        <v>288656108.20733207</v>
+        <v>288656108.19999999</v>
       </c>
       <c r="F25">
-        <v>6475271.8921226691</v>
+        <v>5356571.892</v>
       </c>
       <c r="G25">
-        <v>176888.9279999992</v>
+        <v>176888.92800000001</v>
       </c>
       <c r="H25">
-        <v>32000.00707537675</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I25">
-        <v>10.117422927236451</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>10.11742293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -4079,16 +4207,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C26">
-        <v>261.06134630000003</v>
+        <v>254.73703860000001</v>
       </c>
       <c r="D26">
-        <v>1443.089109</v>
+        <v>1408.129741</v>
       </c>
       <c r="E26">
         <v>288656108.19999999</v>
       </c>
       <c r="F26">
-        <v>15898080.25</v>
+        <v>14779380.25</v>
       </c>
       <c r="G26">
         <v>176888.92800000001</v>
@@ -4100,7 +4228,7 @@
         <v>9.5326505640000008</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -4109,16 +4237,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C27">
-        <v>207.7917128</v>
+        <v>201.4674052</v>
       </c>
       <c r="D27">
-        <v>1148.6264120000001</v>
+        <v>1113.6670449999999</v>
       </c>
       <c r="E27">
         <v>288656108.19999999</v>
       </c>
       <c r="F27">
-        <v>6475271.892</v>
+        <v>5356571.892</v>
       </c>
       <c r="G27">
         <v>176888.92800000001</v>
@@ -4130,7 +4258,7 @@
         <v>9.5326505640000008</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -4139,16 +4267,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C28">
-        <v>259.79667849999998</v>
+        <v>253.47237079999999</v>
       </c>
       <c r="D28">
-        <v>1436.0983060000001</v>
+        <v>1401.1389389999999</v>
       </c>
       <c r="E28">
         <v>288656108.19999999</v>
       </c>
       <c r="F28">
-        <v>15898080.25</v>
+        <v>14779380.25</v>
       </c>
       <c r="G28">
         <v>176888.92800000001</v>
@@ -4160,7 +4288,7 @@
         <v>9.6035991999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -4169,16 +4297,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C29">
-        <v>206.52704499999999</v>
+        <v>200.20273739999999</v>
       </c>
       <c r="D29">
-        <v>1141.63561</v>
+        <v>1106.6762430000001</v>
       </c>
       <c r="E29">
         <v>288656108.19999999</v>
       </c>
       <c r="F29">
-        <v>6475271.892</v>
+        <v>5356571.892</v>
       </c>
       <c r="G29">
         <v>176888.92800000001</v>
@@ -4190,7 +4318,7 @@
         <v>9.6035991999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -4199,16 +4327,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C30">
-        <v>252.78726940000001</v>
+        <v>246.46296179999999</v>
       </c>
       <c r="D30">
-        <v>1397.35185</v>
+        <v>1362.3924830000001</v>
       </c>
       <c r="E30">
         <v>288656108.19999999</v>
       </c>
       <c r="F30">
-        <v>15898080.25</v>
+        <v>14779380.25</v>
       </c>
       <c r="G30">
         <v>176888.92800000001</v>
@@ -4220,7 +4348,7 @@
         <v>10.01680316</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -4229,16 +4357,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C31">
-        <v>199.51763600000001</v>
+        <v>193.19332829999999</v>
       </c>
       <c r="D31">
-        <v>1102.889154</v>
+        <v>1067.929787</v>
       </c>
       <c r="E31">
         <v>288656108.19999999</v>
       </c>
       <c r="F31">
-        <v>6475271.892</v>
+        <v>5356571.892</v>
       </c>
       <c r="G31">
         <v>176888.92800000001</v>
@@ -4250,7 +4378,7 @@
         <v>10.01680316</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -4259,16 +4387,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C32">
-        <v>271.14779346204119</v>
+        <v>264.12078496550038</v>
       </c>
       <c r="D32">
-        <v>1498.8447471929501</v>
+        <v>1460.0010057815159</v>
       </c>
       <c r="E32">
         <v>277512962.69202578</v>
       </c>
       <c r="F32">
-        <v>14901430.036319871</v>
+        <v>13782730.036319871</v>
       </c>
       <c r="G32">
         <v>159200.03520000001</v>
@@ -4280,7 +4408,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -4289,16 +4417,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C33">
-        <v>209.36483468310021</v>
+        <v>202.3378261865594</v>
       </c>
       <c r="D33">
-        <v>1157.322280609359</v>
+        <v>1118.4785391979251</v>
       </c>
       <c r="E33">
         <v>277512962.69202578</v>
       </c>
       <c r="F33">
-        <v>5065580.8239523079</v>
+        <v>3946880.8239523079</v>
       </c>
       <c r="G33">
         <v>159200.03520000001</v>
@@ -4310,7 +4438,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -4319,16 +4447,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C34">
-        <v>243.83899784100089</v>
+        <v>238.08962725292201</v>
       </c>
       <c r="D34">
-        <v>1347.8877936210879</v>
+        <v>1316.106550648097</v>
       </c>
       <c r="E34">
         <v>299683366.79336238</v>
       </c>
       <c r="F34">
-        <v>16922247.970495451</v>
+        <v>15803547.970495449</v>
       </c>
       <c r="G34">
         <v>194577.82079999999</v>
@@ -4340,7 +4468,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -4349,16 +4477,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C35">
-        <v>197.43082398181659</v>
+        <v>191.68145339373771</v>
       </c>
       <c r="D35">
-        <v>1091.353721455042</v>
+        <v>1059.57247848205</v>
       </c>
       <c r="E35">
         <v>299683366.79336238</v>
       </c>
       <c r="F35">
-        <v>7892246.6336678583</v>
+        <v>6773546.6336678583</v>
       </c>
       <c r="G35">
         <v>194577.82079999999</v>
@@ -4370,7 +4498,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -4379,28 +4507,28 @@
         <v>no PV revenue</v>
       </c>
       <c r="C36">
-        <v>259.95297967002011</v>
+        <v>253.62867199999999</v>
       </c>
       <c r="D36">
-        <v>1436.962304287056</v>
+        <v>1402.002937</v>
       </c>
       <c r="E36">
-        <v>288656108.20669693</v>
+        <v>288656108.19999999</v>
       </c>
       <c r="F36">
-        <v>16582541.6930892</v>
+        <v>15463841.689999999</v>
       </c>
       <c r="G36">
         <v>176888.92800000001</v>
       </c>
       <c r="H36">
-        <v>32000.007075376881</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I36">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -4409,28 +4537,28 @@
         <v>PV revenue</v>
       </c>
       <c r="C37">
-        <v>206.68334620500781</v>
+        <v>200.35903859999999</v>
       </c>
       <c r="D37">
-        <v>1142.499608188793</v>
+        <v>1107.5402409999999</v>
       </c>
       <c r="E37">
-        <v>288656108.20669693</v>
+        <v>288656108.19999999</v>
       </c>
       <c r="F37">
-        <v>7159733.334510237</v>
+        <v>6041033.335</v>
       </c>
       <c r="G37">
         <v>176888.92800000001</v>
       </c>
       <c r="H37">
-        <v>32000.007075376881</v>
+        <v>32000.007079999999</v>
       </c>
       <c r="I37">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -4439,16 +4567,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C38">
-        <v>252.21409572632879</v>
+        <v>245.8897880794421</v>
       </c>
       <c r="D38">
-        <v>1394.183473598318</v>
+        <v>1359.2241063280269</v>
       </c>
       <c r="E38">
         <v>288656108.2073791</v>
       </c>
       <c r="F38">
-        <v>15213618.80830376</v>
+        <v>14094918.80830376</v>
       </c>
       <c r="G38">
         <v>176888.92800000001</v>
@@ -4460,7 +4588,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>80</v>
       </c>
@@ -4469,16 +4597,16 @@
         <v>PV revenue</v>
       </c>
       <c r="C39">
-        <v>198.94446226144731</v>
+        <v>192.62015461456059</v>
       </c>
       <c r="D39">
-        <v>1099.720777500778</v>
+        <v>1064.7614102304881</v>
       </c>
       <c r="E39">
         <v>288656108.2073791</v>
       </c>
       <c r="F39">
-        <v>5790810.4497479387</v>
+        <v>4672110.4497479387</v>
       </c>
       <c r="G39">
         <v>176888.92800000001</v>
@@ -4490,11 +4618,11 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="5" t="str">
+      <c r="B40" t="str">
         <f t="shared" ref="B40:B41" si="3">IF(ISNUMBER(SEARCH("PV", A40)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -4520,11 +4648,11 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="5" t="str">
+      <c r="B41" t="str">
         <f t="shared" si="3"/>
         <v>PV revenue</v>
       </c>
@@ -4550,12 +4678,12 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="5" t="str">
-        <f t="shared" ref="B42:B43" si="4">IF(ISNUMBER(SEARCH("PV", A42)),"PV revenue","no PV revenue")</f>
+      <c r="B42" t="str">
+        <f t="shared" ref="B42:B45" si="4">IF(ISNUMBER(SEARCH("PV", A42)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C42">
@@ -4580,11 +4708,11 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="5" t="str">
+      <c r="B43" t="str">
         <f t="shared" si="4"/>
         <v>PV revenue</v>
       </c>
@@ -4608,6 +4736,576 @@
       </c>
       <c r="I43">
         <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="5" t="str">
+        <f t="shared" ref="B44" si="5">IF(ISNUMBER(SEARCH("PV", A44)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C44">
+        <v>256.5612691</v>
+      </c>
+      <c r="D44">
+        <v>1418.2136820000001</v>
+      </c>
+      <c r="E44">
+        <v>283106894.60000002</v>
+      </c>
+      <c r="F44">
+        <v>14278642.92</v>
+      </c>
+      <c r="G44">
+        <v>168044.4816</v>
+      </c>
+      <c r="H44">
+        <v>30400.006720000001</v>
+      </c>
+      <c r="I44">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="4"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C45">
+        <v>199.2670306</v>
+      </c>
+      <c r="D45">
+        <v>1101.503864</v>
+      </c>
+      <c r="E45">
+        <v>283106894.60000002</v>
+      </c>
+      <c r="F45">
+        <v>4650662.3130000001</v>
+      </c>
+      <c r="G45">
+        <v>168044.4816</v>
+      </c>
+      <c r="H45">
+        <v>30400.006720000001</v>
+      </c>
+      <c r="I45">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="5" t="str">
+        <f t="shared" ref="B46:B47" si="6">IF(ISNUMBER(SEARCH("PV", A46)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C46">
+        <v>243.5863467476255</v>
+      </c>
+      <c r="D46">
+        <v>1346.491194521597</v>
+      </c>
+      <c r="E46">
+        <v>294061734.4402532</v>
+      </c>
+      <c r="F46">
+        <v>15291276.95609845</v>
+      </c>
+      <c r="G46">
+        <v>185733.3744</v>
+      </c>
+      <c r="H46">
+        <v>33600.007429145728</v>
+      </c>
+      <c r="I46">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C47">
+        <v>193.92226225622341</v>
+      </c>
+      <c r="D47">
+        <v>1071.9591719163459</v>
+      </c>
+      <c r="E47">
+        <v>294061734.4402532</v>
+      </c>
+      <c r="F47">
+        <v>6066998.9570236094</v>
+      </c>
+      <c r="G47">
+        <v>185733.3744</v>
+      </c>
+      <c r="H47">
+        <v>33600.007429145728</v>
+      </c>
+      <c r="I47">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="5" t="str">
+        <f t="shared" ref="B48:B51" si="7">IF(ISNUMBER(SEARCH("PV", A48)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C48">
+        <v>251.693951</v>
+      </c>
+      <c r="D48">
+        <v>1391.308229</v>
+      </c>
+      <c r="E48">
+        <v>288656108.19999999</v>
+      </c>
+      <c r="F48">
+        <v>15121610.970000001</v>
+      </c>
+      <c r="G48">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H48">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I48">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C49">
+        <v>198.42431759999999</v>
+      </c>
+      <c r="D49">
+        <v>1096.8455329999999</v>
+      </c>
+      <c r="E49">
+        <v>288656108.19999999</v>
+      </c>
+      <c r="F49">
+        <v>5698802.6129999999</v>
+      </c>
+      <c r="G49">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H49">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I49">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C50">
+        <v>247.82450906536539</v>
+      </c>
+      <c r="D50">
+        <v>1369.9188140002141</v>
+      </c>
+      <c r="E50">
+        <v>288656108.20732808</v>
+      </c>
+      <c r="F50">
+        <v>14437149.52949648</v>
+      </c>
+      <c r="G50">
+        <v>176888.9280000341</v>
+      </c>
+      <c r="H50">
+        <v>32000.007075383051</v>
+      </c>
+      <c r="I50">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C51">
+        <v>194.55487560048911</v>
+      </c>
+      <c r="D51">
+        <v>1075.456117902703</v>
+      </c>
+      <c r="E51">
+        <v>288656108.20732808</v>
+      </c>
+      <c r="F51">
+        <v>5014341.170939764</v>
+      </c>
+      <c r="G51">
+        <v>176888.9280000341</v>
+      </c>
+      <c r="H51">
+        <v>32000.007075383051</v>
+      </c>
+      <c r="I51">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="5" t="str">
+        <f t="shared" ref="B52:B55" si="8">IF(ISNUMBER(SEARCH("PV", A52)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C52">
+        <v>246.8502493</v>
+      </c>
+      <c r="D52">
+        <v>1364.533322</v>
+      </c>
+      <c r="E52">
+        <v>288026061.10000002</v>
+      </c>
+      <c r="F52">
+        <v>14328985.449999999</v>
+      </c>
+      <c r="G52">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H52">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I52">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C53">
+        <v>196.2703564</v>
+      </c>
+      <c r="D53">
+        <v>1084.9389140000001</v>
+      </c>
+      <c r="E53">
+        <v>288026061.10000002</v>
+      </c>
+      <c r="F53">
+        <v>5381962.415</v>
+      </c>
+      <c r="G53">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H53">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I53">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C54">
+        <v>252.47612649999999</v>
+      </c>
+      <c r="D54">
+        <v>1395.6319209999999</v>
+      </c>
+      <c r="E54">
+        <v>289931574.60000002</v>
+      </c>
+      <c r="F54">
+        <v>15130060.08</v>
+      </c>
+      <c r="G54">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H54">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I54">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C55">
+        <v>196.42496990000001</v>
+      </c>
+      <c r="D55">
+        <v>1085.793584</v>
+      </c>
+      <c r="E55">
+        <v>289931574.60000002</v>
+      </c>
+      <c r="F55">
+        <v>5215231.0870000003</v>
+      </c>
+      <c r="G55">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H55">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I55">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="5" t="str">
+        <f t="shared" ref="B56:B58" si="9">IF(ISNUMBER(SEARCH("PV", A56)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C56">
+        <v>249.53064670000001</v>
+      </c>
+      <c r="D56">
+        <v>1379.349964</v>
+      </c>
+      <c r="E56">
+        <v>288026061.10000002</v>
+      </c>
+      <c r="F56">
+        <v>14803118.08</v>
+      </c>
+      <c r="G56">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H56">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I56">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C57">
+        <v>196.2703564</v>
+      </c>
+      <c r="D57">
+        <v>1084.9389140000001</v>
+      </c>
+      <c r="E57">
+        <v>288026061.10000002</v>
+      </c>
+      <c r="F57">
+        <v>5381962.415</v>
+      </c>
+      <c r="G57">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H57">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I57">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C58">
+        <v>250.01433220000001</v>
+      </c>
+      <c r="D58">
+        <v>1382.02367</v>
+      </c>
+      <c r="E58">
+        <v>289280462.80000001</v>
+      </c>
+      <c r="F58">
+        <v>14760913.109999999</v>
+      </c>
+      <c r="G58">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H58">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I58">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="5" t="str">
+        <f t="shared" ref="B59:B62" si="10">IF(ISNUMBER(SEARCH("PV", A59)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C59">
+        <v>257.80078750000001</v>
+      </c>
+      <c r="D59">
+        <v>1425.065464</v>
+      </c>
+      <c r="E59">
+        <v>302186986.10000002</v>
+      </c>
+      <c r="F59">
+        <v>14823692.92</v>
+      </c>
+      <c r="G59">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H59">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I59">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C60">
+        <v>204.48719790000001</v>
+      </c>
+      <c r="D60">
+        <v>1130.3597890000001</v>
+      </c>
+      <c r="E60">
+        <v>302186986.10000002</v>
+      </c>
+      <c r="F60">
+        <v>5393109.2189999996</v>
+      </c>
+      <c r="G60">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H60">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I60">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C61">
+        <v>241.72339030000001</v>
+      </c>
+      <c r="D61">
+        <v>1336.1931850000001</v>
+      </c>
+      <c r="E61">
+        <v>275093145</v>
+      </c>
+      <c r="F61">
+        <v>14739346.93</v>
+      </c>
+      <c r="G61">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H61">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I61">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>102</v>
+      </c>
+      <c r="B62" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C62">
+        <v>188.46969340000001</v>
+      </c>
+      <c r="D62">
+        <v>1041.818583</v>
+      </c>
+      <c r="E62">
+        <v>275093145</v>
+      </c>
+      <c r="F62">
+        <v>5319357.5789999999</v>
+      </c>
+      <c r="G62">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H62">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I62">
+        <v>9.8181474069999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update LCOE for 15 and 20 operating points
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\Nord_H2ub\Spine_Projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48F1C6B-C085-4BB8-A1D5-0F5EEBFE71AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4FBE84-55A4-4C29-855D-BC23C279D508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4575" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
+    <workbookView xWindow="-4575" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_operating_points" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
   <si>
     <t>run_name</t>
   </si>
@@ -347,6 +347,18 @@
   </si>
   <si>
     <t>sens_10op_invc_05pdown_PV</t>
+  </si>
+  <si>
+    <t>base_15op</t>
+  </si>
+  <si>
+    <t>base_15op_PV</t>
+  </si>
+  <si>
+    <t>base_20op</t>
+  </si>
+  <si>
+    <t>base_20op_PV</t>
   </si>
 </sst>
 </file>
@@ -1838,8 +1850,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73A3E7BD-A6FC-4C2D-BF58-717B292B5EEE}" name="Table1" displayName="Table1" ref="A1:I21" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A1:I21" xr:uid="{73A3E7BD-A6FC-4C2D-BF58-717B292B5EEE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73A3E7BD-A6FC-4C2D-BF58-717B292B5EEE}" name="Table1" displayName="Table1" ref="A1:I25" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A1:I25" xr:uid="{73A3E7BD-A6FC-4C2D-BF58-717B292B5EEE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I21">
     <sortCondition ref="A1:A21"/>
   </sortState>
@@ -2221,10 +2233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB416CA-7C9B-4F0E-AFD4-34077EF25340}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2865,6 +2877,126 @@
         <v>32000.007075377049</v>
       </c>
       <c r="I21">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="5" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C22">
+        <v>249.73614149918711</v>
+      </c>
+      <c r="D22">
+        <v>1380.485893287173</v>
+      </c>
+      <c r="E22">
+        <v>288736929.04657698</v>
+      </c>
+      <c r="F22">
+        <v>14767064.360440319</v>
+      </c>
+      <c r="G22">
+        <v>176888.9279999999</v>
+      </c>
+      <c r="H22">
+        <v>32000.00707537687</v>
+      </c>
+      <c r="I22">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="5" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>PV revenue</v>
+      </c>
+      <c r="C23">
+        <v>196.44983468472191</v>
+      </c>
+      <c r="D23">
+        <v>1085.931030618324</v>
+      </c>
+      <c r="E23">
+        <v>288736929.04657698</v>
+      </c>
+      <c r="F23">
+        <v>5341306.6709504724</v>
+      </c>
+      <c r="G23">
+        <v>176888.9279999999</v>
+      </c>
+      <c r="H23">
+        <v>32000.00707537687</v>
+      </c>
+      <c r="I23">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="5" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C24">
+        <v>249.59496612046431</v>
+      </c>
+      <c r="D24">
+        <v>1379.7055071658999</v>
+      </c>
+      <c r="E24">
+        <v>288563658.52300167</v>
+      </c>
+      <c r="F24">
+        <v>14759739.98456678</v>
+      </c>
+      <c r="G24">
+        <v>176888.9279999143</v>
+      </c>
+      <c r="H24">
+        <v>32000.007075361391</v>
+      </c>
+      <c r="I24">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
+        <v>PV revenue</v>
+      </c>
+      <c r="C25">
+        <v>196.2722336916267</v>
+      </c>
+      <c r="D25">
+        <v>1084.949291795381</v>
+      </c>
+      <c r="E25">
+        <v>288563658.52300167</v>
+      </c>
+      <c r="F25">
+        <v>5327539.0072034188</v>
+      </c>
+      <c r="G25">
+        <v>176888.9279999143</v>
+      </c>
+      <c r="H25">
+        <v>32000.007075361391</v>
+      </c>
+      <c r="I25">
         <v>9.8181474074492936</v>
       </c>
     </row>
@@ -3239,7 +3371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
   <dimension ref="A1:U62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4742,7 +4874,7 @@
       <c r="A44" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="5" t="str">
+      <c r="B44" t="str">
         <f t="shared" ref="B44" si="5">IF(ISNUMBER(SEARCH("PV", A44)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -4802,7 +4934,7 @@
       <c r="A46" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="5" t="str">
+      <c r="B46" t="str">
         <f t="shared" ref="B46:B47" si="6">IF(ISNUMBER(SEARCH("PV", A46)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -4832,7 +4964,7 @@
       <c r="A47" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="5" t="str">
+      <c r="B47" t="str">
         <f t="shared" si="6"/>
         <v>PV revenue</v>
       </c>
@@ -4862,7 +4994,7 @@
       <c r="A48" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="5" t="str">
+      <c r="B48" t="str">
         <f t="shared" ref="B48:B51" si="7">IF(ISNUMBER(SEARCH("PV", A48)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -4892,7 +5024,7 @@
       <c r="A49" t="s">
         <v>89</v>
       </c>
-      <c r="B49" s="5" t="str">
+      <c r="B49" t="str">
         <f t="shared" si="7"/>
         <v>PV revenue</v>
       </c>
@@ -4922,7 +5054,7 @@
       <c r="A50" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="5" t="str">
+      <c r="B50" t="str">
         <f t="shared" si="7"/>
         <v>no PV revenue</v>
       </c>
@@ -4952,7 +5084,7 @@
       <c r="A51" t="s">
         <v>91</v>
       </c>
-      <c r="B51" s="5" t="str">
+      <c r="B51" t="str">
         <f t="shared" si="7"/>
         <v>PV revenue</v>
       </c>
@@ -4982,7 +5114,7 @@
       <c r="A52" t="s">
         <v>92</v>
       </c>
-      <c r="B52" s="5" t="str">
+      <c r="B52" t="str">
         <f t="shared" ref="B52:B55" si="8">IF(ISNUMBER(SEARCH("PV", A52)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -5012,7 +5144,7 @@
       <c r="A53" t="s">
         <v>93</v>
       </c>
-      <c r="B53" s="5" t="str">
+      <c r="B53" t="str">
         <f t="shared" si="8"/>
         <v>PV revenue</v>
       </c>
@@ -5042,7 +5174,7 @@
       <c r="A54" t="s">
         <v>94</v>
       </c>
-      <c r="B54" s="5" t="str">
+      <c r="B54" t="str">
         <f t="shared" si="8"/>
         <v>no PV revenue</v>
       </c>
@@ -5072,7 +5204,7 @@
       <c r="A55" t="s">
         <v>95</v>
       </c>
-      <c r="B55" s="5" t="str">
+      <c r="B55" t="str">
         <f t="shared" si="8"/>
         <v>PV revenue</v>
       </c>
@@ -5102,7 +5234,7 @@
       <c r="A56" t="s">
         <v>96</v>
       </c>
-      <c r="B56" s="5" t="str">
+      <c r="B56" t="str">
         <f t="shared" ref="B56:B58" si="9">IF(ISNUMBER(SEARCH("PV", A56)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -5132,7 +5264,7 @@
       <c r="A57" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="5" t="str">
+      <c r="B57" t="str">
         <f t="shared" si="9"/>
         <v>PV revenue</v>
       </c>
@@ -5162,7 +5294,7 @@
       <c r="A58" t="s">
         <v>98</v>
       </c>
-      <c r="B58" s="5" t="str">
+      <c r="B58" t="str">
         <f t="shared" si="9"/>
         <v>no PV revenue</v>
       </c>
@@ -5192,7 +5324,7 @@
       <c r="A59" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="5" t="str">
+      <c r="B59" t="str">
         <f t="shared" ref="B59:B62" si="10">IF(ISNUMBER(SEARCH("PV", A59)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -5222,7 +5354,7 @@
       <c r="A60" t="s">
         <v>100</v>
       </c>
-      <c r="B60" s="5" t="str">
+      <c r="B60" t="str">
         <f t="shared" si="10"/>
         <v>PV revenue</v>
       </c>
@@ -5252,7 +5384,7 @@
       <c r="A61" t="s">
         <v>101</v>
       </c>
-      <c r="B61" s="5" t="str">
+      <c r="B61" t="str">
         <f t="shared" si="10"/>
         <v>no PV revenue</v>
       </c>
@@ -5282,7 +5414,7 @@
       <c r="A62" t="s">
         <v>102</v>
       </c>
-      <c r="B62" s="5" t="str">
+      <c r="B62" t="str">
         <f t="shared" si="10"/>
         <v>PV revenue</v>
       </c>

</xml_diff>

<commit_message>
add prepared results for eff 10p down for comparison
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\Nord_H2ub\Spine_Projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4FBE84-55A4-4C29-855D-BC23C279D508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE922D6F-D018-457B-85DF-89E8D1A42F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4575" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_operating_points" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="110">
   <si>
     <t>run_name</t>
   </si>
@@ -359,6 +359,15 @@
   </si>
   <si>
     <t>base_20op_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_eff_10pdown</t>
+  </si>
+  <si>
+    <t>sens_10op_eff_10pdown_PV</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
   </si>
 </sst>
 </file>
@@ -551,7 +560,7 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:shade val="47000"/>
+                  <a:shade val="45000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -633,7 +642,7 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:shade val="65000"/>
+                  <a:shade val="61000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -715,7 +724,7 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:shade val="82000"/>
+                  <a:shade val="76000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -796,7 +805,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:shade val="92000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -877,7 +888,7 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:tint val="83000"/>
+                  <a:tint val="93000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -959,7 +970,7 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:tint val="65000"/>
+                  <a:tint val="77000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1041,7 +1052,7 @@
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:tint val="48000"/>
+                  <a:tint val="62000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1051,6 +1062,29 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$K$2:$K$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-10 %</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5 %</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Base</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>+5 %</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>+10 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Comparison_sensitivities!$R$2:$R$6</c:f>
@@ -1079,6 +1113,82 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5045-4939-A37F-BD7B21CF5F42}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Efficiency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="46000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison_sensitivities!$K$2:$K$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-10 %</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5 %</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Base</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>+5 %</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>+10 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison_sensitivities!$S$2:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1451.739909044454</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1380.6135220000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-877A-4F6C-98F4-EAA42CC01476}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1897,8 +2007,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I62" totalsRowShown="0">
-  <autoFilter ref="A1:I62" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I64" totalsRowShown="0">
+  <autoFilter ref="A1:I64" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8869914E-4BE8-401C-AC76-C6570071019E}" name="run_name"/>
     <tableColumn id="9" xr3:uid="{91B3AAB6-6FBC-4E2C-8674-ECB365CA16C8}" name="PV" dataDxfId="0">
@@ -2235,23 +2345,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB416CA-7C9B-4F0E-AFD4-34077EF25340}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" customWidth="1"/>
-    <col min="8" max="8" width="21.21875" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="1" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
+    <col min="7" max="7" width="25.08984375" customWidth="1"/>
+    <col min="8" max="8" width="21.1796875" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2280,7 +2390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2310,7 +2420,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2340,7 +2450,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2370,7 +2480,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2400,7 +2510,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2430,7 +2540,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2460,7 +2570,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2490,7 +2600,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2520,7 +2630,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2550,7 +2660,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2580,7 +2690,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2610,7 +2720,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2640,7 +2750,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2670,7 +2780,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2700,7 +2810,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -2730,7 +2840,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2760,7 +2870,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -2790,7 +2900,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2820,7 +2930,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -2850,7 +2960,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2880,11 +2990,11 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="5" t="str">
+      <c r="B22" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -2910,11 +3020,11 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="5" t="str">
+      <c r="B23" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
@@ -2940,11 +3050,11 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="5" t="str">
+      <c r="B24" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -2970,11 +3080,11 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>106</v>
       </c>
-      <c r="B25" s="5" t="str">
+      <c r="B25" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", Table1[[#This Row],[run_name]])),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
@@ -3016,19 +3126,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="1" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
-    <col min="7" max="7" width="24.21875" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" customWidth="1"/>
+    <col min="7" max="7" width="24.1796875" customWidth="1"/>
+    <col min="8" max="8" width="20.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3063,7 +3173,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -3100,7 +3210,7 @@
         <v>43.057462085171316</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3137,7 +3247,7 @@
         <v>43.057462085171316</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3174,7 +3284,7 @@
         <v>42.284047015025735</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3211,7 +3321,7 @@
         <v>42.284047015025735</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -3248,7 +3358,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -3285,7 +3395,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -3322,7 +3432,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -3369,24 +3479,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
-  <dimension ref="A1:U62"/>
+  <dimension ref="A1:V64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
-    <col min="7" max="7" width="24.21875" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" customWidth="1"/>
+    <col min="7" max="7" width="24.1796875" customWidth="1"/>
+    <col min="8" max="8" width="20.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3438,8 +3550,11 @@
       <c r="R1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -3499,8 +3614,12 @@
         <f>D40</f>
         <v>1326.412694499294</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S2">
+        <f>D63</f>
+        <v>1451.739909044454</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3560,8 +3679,11 @@
         <f>D61</f>
         <v>1336.1931850000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S3">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -3598,7 +3720,7 @@
         <v>1380.6135220000001</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" ref="M4:R4" si="1">$D$2</f>
+        <f t="shared" ref="M4:S4" si="1">$D$2</f>
         <v>1380.6135220000001</v>
       </c>
       <c r="N4" s="1">
@@ -3621,16 +3743,20 @@
         <f t="shared" si="1"/>
         <v>1380.6135220000001</v>
       </c>
-      <c r="T4" s="4">
+      <c r="S4" s="1">
+        <f t="shared" si="1"/>
+        <v>1380.6135220000001</v>
+      </c>
+      <c r="U4" s="4">
         <f>R2/P4</f>
         <v>0.96074149163613209</v>
       </c>
-      <c r="U4">
-        <f>1-T4</f>
+      <c r="V4">
+        <f>1-U4</f>
         <v>3.9258508363867906E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -3690,16 +3816,16 @@
         <f>D59</f>
         <v>1425.065464</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <f>R6/P4</f>
         <v>1.0897826962023807</v>
       </c>
-      <c r="U5">
-        <f>T5-1</f>
+      <c r="V5">
+        <f>U5-1</f>
         <v>8.9782696202380663E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3760,7 +3886,7 @@
         <v>1504.5687264186249</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -3790,7 +3916,7 @@
         <v>9.2601513579999999</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -3820,7 +3946,7 @@
         <v>9.3718871359999998</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -3850,7 +3976,7 @@
         <v>9.3718871359999998</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -3880,7 +4006,7 @@
         <v>10.200743660000001</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -3910,7 +4036,7 @@
         <v>10.200743660000001</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -3940,7 +4066,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -3970,7 +4096,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -4000,7 +4126,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -4030,7 +4156,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -4060,7 +4186,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -4090,7 +4216,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -4120,7 +4246,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -4150,7 +4276,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -4180,7 +4306,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -4210,7 +4336,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -4240,7 +4366,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -4270,7 +4396,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -4300,7 +4426,7 @@
         <v>10.11742293</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -4330,7 +4456,7 @@
         <v>10.11742293</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -4360,7 +4486,7 @@
         <v>9.5326505640000008</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -4390,7 +4516,7 @@
         <v>9.5326505640000008</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -4420,7 +4546,7 @@
         <v>9.6035991999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -4450,7 +4576,7 @@
         <v>9.6035991999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -4480,7 +4606,7 @@
         <v>10.01680316</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -4510,7 +4636,7 @@
         <v>10.01680316</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -4540,7 +4666,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -4570,7 +4696,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -4600,7 +4726,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -4630,7 +4756,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -4660,7 +4786,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -4690,7 +4816,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -4720,7 +4846,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>80</v>
       </c>
@@ -4750,7 +4876,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -4780,7 +4906,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -4810,7 +4936,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -4840,7 +4966,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -4870,7 +4996,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -4900,7 +5026,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -4930,7 +5056,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -4960,7 +5086,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -4990,7 +5116,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -5020,7 +5146,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>89</v>
       </c>
@@ -5050,7 +5176,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>90</v>
       </c>
@@ -5080,7 +5206,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>91</v>
       </c>
@@ -5110,7 +5236,7 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>92</v>
       </c>
@@ -5140,7 +5266,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>93</v>
       </c>
@@ -5170,7 +5296,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>94</v>
       </c>
@@ -5200,7 +5326,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>95</v>
       </c>
@@ -5230,7 +5356,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>96</v>
       </c>
@@ -5260,7 +5386,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>97</v>
       </c>
@@ -5290,7 +5416,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>98</v>
       </c>
@@ -5320,7 +5446,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>99</v>
       </c>
@@ -5350,7 +5476,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>100</v>
       </c>
@@ -5380,7 +5506,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -5410,7 +5536,7 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>102</v>
       </c>
@@ -5438,6 +5564,66 @@
       </c>
       <c r="I62">
         <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="5" t="str">
+        <f t="shared" ref="B63:B64" si="11">IF(ISNUMBER(SEARCH("PV", A63)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C63">
+        <v>262.62631520402192</v>
+      </c>
+      <c r="D63">
+        <v>1451.739909044454</v>
+      </c>
+      <c r="E63">
+        <v>298331833.89240187</v>
+      </c>
+      <c r="F63">
+        <v>16069931.11681715</v>
+      </c>
+      <c r="G63">
+        <v>176888.92799996189</v>
+      </c>
+      <c r="H63">
+        <v>32000.007075370009</v>
+      </c>
+      <c r="I63">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C64">
+        <v>211.80775199938211</v>
+      </c>
+      <c r="D64">
+        <v>1170.8261846632511</v>
+      </c>
+      <c r="E64">
+        <v>298331833.89240187</v>
+      </c>
+      <c r="F64">
+        <v>7080689.949050107</v>
+      </c>
+      <c r="G64">
+        <v>176888.92799996189</v>
+      </c>
+      <c r="H64">
+        <v>32000.007075370009</v>
+      </c>
+      <c r="I64">
+        <v>9.8181474074492936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add prepared results for efficiency sensitivities
05p down and 10p up runs
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE922D6F-D018-457B-85DF-89E8D1A42F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E75B69-DB37-47B5-9A3E-8745BD97FC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="116">
   <si>
     <t>run_name</t>
   </si>
@@ -368,6 +368,24 @@
   </si>
   <si>
     <t>Efficiency</t>
+  </si>
+  <si>
+    <t>sens_10op_eff_05pdown</t>
+  </si>
+  <si>
+    <t>sens_10op_eff_05pdown_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_eff_10pup</t>
+  </si>
+  <si>
+    <t>sens_10op_eff_10pup_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_eff_05pup</t>
+  </si>
+  <si>
+    <t>sens_10op_eff_05pup_PV</t>
   </si>
 </sst>
 </file>
@@ -1177,10 +1195,16 @@
                   <c:v>1451.739909044454</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1400</c:v>
+                  <c:v>1413.9417530000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1380.6135220000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1322.950869015936</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2007,8 +2031,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I64" totalsRowShown="0">
-  <autoFilter ref="A1:I64" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I70" totalsRowShown="0">
+  <autoFilter ref="A1:I70" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8869914E-4BE8-401C-AC76-C6570071019E}" name="run_name"/>
     <tableColumn id="9" xr3:uid="{91B3AAB6-6FBC-4E2C-8674-ECB365CA16C8}" name="PV" dataDxfId="0">
@@ -3479,10 +3503,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
-  <dimension ref="A1:V64"/>
+  <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="H18" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3680,7 +3704,8 @@
         <v>1336.1931850000001</v>
       </c>
       <c r="S3">
-        <v>1400</v>
+        <f>D65</f>
+        <v>1413.9417530000001</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
@@ -3816,6 +3841,10 @@
         <f>D59</f>
         <v>1425.065464</v>
       </c>
+      <c r="S5">
+        <f>D69</f>
+        <v>0</v>
+      </c>
       <c r="U5">
         <f>R6/P4</f>
         <v>1.0897826962023807</v>
@@ -3885,6 +3914,10 @@
         <f>D42</f>
         <v>1504.5687264186249</v>
       </c>
+      <c r="S6">
+        <f>D67</f>
+        <v>1322.950869015936</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -5570,7 +5603,7 @@
       <c r="A63" t="s">
         <v>107</v>
       </c>
-      <c r="B63" s="5" t="str">
+      <c r="B63" t="str">
         <f t="shared" ref="B63:B64" si="11">IF(ISNUMBER(SEARCH("PV", A63)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -5600,7 +5633,7 @@
       <c r="A64" t="s">
         <v>108</v>
       </c>
-      <c r="B64" s="5" t="str">
+      <c r="B64" t="str">
         <f t="shared" si="11"/>
         <v>PV revenue</v>
       </c>
@@ -5624,6 +5657,144 @@
       </c>
       <c r="I64">
         <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" s="5" t="str">
+        <f t="shared" ref="B65:B66" si="12">IF(ISNUMBER(SEARCH("PV", A65)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C65">
+        <v>255.7884578</v>
+      </c>
+      <c r="D65">
+        <v>1413.9417530000001</v>
+      </c>
+      <c r="E65">
+        <v>293126897.89999998</v>
+      </c>
+      <c r="F65">
+        <v>15390524.08</v>
+      </c>
+      <c r="G65">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H65">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I65">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C66">
+        <v>203.69102849999999</v>
+      </c>
+      <c r="D66">
+        <v>1125.9587409999999</v>
+      </c>
+      <c r="E66">
+        <v>293126897.89999998</v>
+      </c>
+      <c r="F66">
+        <v>6175065.6540000001</v>
+      </c>
+      <c r="G66">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H66">
+        <v>32000.007079999999</v>
+      </c>
+      <c r="I66">
+        <v>9.8181474069999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" s="5" t="str">
+        <f t="shared" ref="B67:B70" si="13">IF(ISNUMBER(SEARCH("PV", A67)),"PV revenue","no PV revenue")</f>
+        <v>no PV revenue</v>
+      </c>
+      <c r="C67">
+        <v>239.3277953998678</v>
+      </c>
+      <c r="D67">
+        <v>1322.950869015936</v>
+      </c>
+      <c r="E67">
+        <v>280769564.06627142</v>
+      </c>
+      <c r="F67">
+        <v>13737436.898423109</v>
+      </c>
+      <c r="G67">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H67">
+        <v>32000.007075376889</v>
+      </c>
+      <c r="I67">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C68">
+        <v>183.9854727249064</v>
+      </c>
+      <c r="D68">
+        <v>1017.030807562677</v>
+      </c>
+      <c r="E68">
+        <v>280769564.06627142</v>
+      </c>
+      <c r="F68">
+        <v>3947992.767419091</v>
+      </c>
+      <c r="G68">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H68">
+        <v>32000.007075376889</v>
+      </c>
+      <c r="I68">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>114</v>
+      </c>
+      <c r="B69" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>no PV revenue</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>115</v>
+      </c>
+      <c r="B70" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>PV revenue</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add prepared result for 05p up efficiency sensitivity
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E75B69-DB37-47B5-9A3E-8745BD97FC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70E3544-5B3E-49A7-B985-6DE3AEBD69F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -467,7 +467,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1201,7 +1200,7 @@
                   <c:v>1380.6135220000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1350.335787788548</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1322.950869015936</c:v>
@@ -3505,8 +3504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
   <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H18" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3843,7 +3842,7 @@
       </c>
       <c r="S5">
         <f>D69</f>
-        <v>0</v>
+        <v>1350.335787788548</v>
       </c>
       <c r="U5">
         <f>R6/P4</f>
@@ -5663,7 +5662,7 @@
       <c r="A65" t="s">
         <v>110</v>
       </c>
-      <c r="B65" s="5" t="str">
+      <c r="B65" t="str">
         <f t="shared" ref="B65:B66" si="12">IF(ISNUMBER(SEARCH("PV", A65)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -5693,7 +5692,7 @@
       <c r="A66" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="5" t="str">
+      <c r="B66" t="str">
         <f t="shared" si="12"/>
         <v>PV revenue</v>
       </c>
@@ -5723,7 +5722,7 @@
       <c r="A67" t="s">
         <v>112</v>
       </c>
-      <c r="B67" s="5" t="str">
+      <c r="B67" t="str">
         <f t="shared" ref="B67:B70" si="13">IF(ISNUMBER(SEARCH("PV", A67)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
@@ -5753,7 +5752,7 @@
       <c r="A68" t="s">
         <v>113</v>
       </c>
-      <c r="B68" s="5" t="str">
+      <c r="B68" t="str">
         <f t="shared" si="13"/>
         <v>PV revenue</v>
       </c>
@@ -5783,18 +5782,60 @@
       <c r="A69" t="s">
         <v>114</v>
       </c>
-      <c r="B69" s="5" t="str">
+      <c r="B69" t="str">
         <f t="shared" si="13"/>
         <v>no PV revenue</v>
+      </c>
+      <c r="C69">
+        <v>244.28185105722491</v>
+      </c>
+      <c r="D69">
+        <v>1350.335787788548</v>
+      </c>
+      <c r="E69">
+        <v>284513063.26602769</v>
+      </c>
+      <c r="F69">
+        <v>14232470.830683179</v>
+      </c>
+      <c r="G69">
+        <v>176888.9280000029</v>
+      </c>
+      <c r="H69">
+        <v>32000.007075377409</v>
+      </c>
+      <c r="I69">
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>115</v>
       </c>
-      <c r="B70" s="5" t="str">
+      <c r="B70" t="str">
         <f t="shared" si="13"/>
         <v>PV revenue</v>
+      </c>
+      <c r="C70">
+        <v>189.9325502857827</v>
+      </c>
+      <c r="D70">
+        <v>1049.9049307464099</v>
+      </c>
+      <c r="E70">
+        <v>284513063.26602769</v>
+      </c>
+      <c r="F70">
+        <v>4618681.2796730399</v>
+      </c>
+      <c r="G70">
+        <v>176888.9280000029</v>
+      </c>
+      <c r="H70">
+        <v>32000.007075377409</v>
+      </c>
+      <c r="I70">
+        <v>9.8181474074492936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update LCOM values part II
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\Nord_H2ub\Spine_Projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89E3CB6-8441-4F6F-85C8-B3143742ADC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB25A8D5-2DCF-4870-9E70-E63E6172A55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
+    <workbookView xWindow="-4575" yWindow="-21720" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_operating_points" sheetId="1" r:id="rId1"/>
@@ -863,7 +863,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1378.204571</c:v>
+                  <c:v>1373.036302463961</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1379.349964</c:v>
@@ -875,7 +875,7 @@
                   <c:v>1382.02367</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1382.936637</c:v>
+                  <c:v>1377.619467249845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -945,19 +945,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1326.6078299999999</c:v>
+                  <c:v>1321.3008680363121</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1353.436465</c:v>
+                  <c:v>1348.129502674258</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1375.306559250821</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1408.129741</c:v>
+                  <c:v>1402.8227788869131</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1435.975827</c:v>
+                  <c:v>1430.6688648694551</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1027,19 +1027,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1424.3619349999999</c:v>
+                  <c:v>1419.0549723979559</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1401.1389389999999</c:v>
+                  <c:v>1395.831976429542</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1375.306559250821</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1362.3924830000001</c:v>
+                  <c:v>1357.0855207888719</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1346.153939</c:v>
+                  <c:v>1340.846976901094</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1112,13 +1112,13 @@
                   <c:v>1326.412694499294</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1336.1931850000001</c:v>
+                  <c:v>1330.918454510864</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1375.306559250821</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1425.065464</c:v>
+                  <c:v>1419.729822900282</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1504.5687264186249</c:v>
@@ -3145,7 +3145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66730D5D-FFCC-4E02-B3EF-17A6B47B78F2}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -3504,8 +3504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
   <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:I3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3582,7 +3582,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B37" si="0">IF(ISNUMBER(SEARCH("PV", A2)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A2)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C2">
@@ -3623,15 +3623,15 @@
       </c>
       <c r="O2">
         <f>D20</f>
-        <v>1378.204571</v>
+        <v>1373.036302463961</v>
       </c>
       <c r="P2">
         <f>D4</f>
-        <v>1326.6078299999999</v>
+        <v>1321.3008680363121</v>
       </c>
       <c r="Q2">
         <f>D8</f>
-        <v>1424.3619349999999</v>
+        <v>1419.0549723979559</v>
       </c>
       <c r="R2">
         <f>D40</f>
@@ -3647,7 +3647,7 @@
         <v>27</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A3)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C3">
@@ -3692,15 +3692,15 @@
       </c>
       <c r="P3">
         <f>D24</f>
-        <v>1353.436465</v>
+        <v>1348.129502674258</v>
       </c>
       <c r="Q3">
         <f>D28</f>
-        <v>1401.1389389999999</v>
+        <v>1395.831976429542</v>
       </c>
       <c r="R3">
         <f>D61</f>
-        <v>1336.1931850000001</v>
+        <v>1330.918454510864</v>
       </c>
       <c r="S3">
         <f>D65</f>
@@ -3712,29 +3712,29 @@
         <v>41</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A4)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C4">
-        <v>239.9893563</v>
+        <v>239.0293027603378</v>
       </c>
       <c r="D4">
-        <v>1326.6078299999999</v>
+        <v>1321.3008680363121</v>
       </c>
       <c r="E4">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F4">
-        <v>14779380.25</v>
+        <v>14609557.41562718</v>
       </c>
       <c r="G4">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H4">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I4">
-        <v>10.431312399999999</v>
+        <v>10.43131239971656</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>59</v>
@@ -3744,31 +3744,31 @@
         <v>1375.306559250821</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" ref="M4:S4" si="1">$D$2</f>
+        <f t="shared" ref="M4:S4" si="0">$D$2</f>
         <v>1375.306559250821</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1375.306559250821</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1375.306559250821</v>
       </c>
       <c r="P4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1375.306559250821</v>
       </c>
       <c r="Q4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1375.306559250821</v>
       </c>
       <c r="R4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1375.306559250821</v>
       </c>
       <c r="S4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1375.306559250821</v>
       </c>
       <c r="U4" s="4">
@@ -3785,29 +3785,29 @@
         <v>43</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A5)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C5">
-        <v>186.7197228</v>
+        <v>186.7197227989252</v>
       </c>
       <c r="D5">
-        <v>1032.1451340000001</v>
+        <v>1032.145134360725</v>
       </c>
       <c r="E5">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F5">
-        <v>5356571.892</v>
+        <v>5356571.8921226691</v>
       </c>
       <c r="G5">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H5">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I5">
-        <v>10.431312399999999</v>
+        <v>10.43131239971656</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>74</v>
@@ -3830,15 +3830,15 @@
       </c>
       <c r="P5">
         <f>D26</f>
-        <v>1408.129741</v>
+        <v>1402.8227788869131</v>
       </c>
       <c r="Q5">
         <f>D30</f>
-        <v>1362.3924830000001</v>
+        <v>1357.0855207888719</v>
       </c>
       <c r="R5">
         <f>D59</f>
-        <v>1425.065464</v>
+        <v>1419.729822900282</v>
       </c>
       <c r="S5">
         <f>D69</f>
@@ -3858,29 +3858,29 @@
         <v>44</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A6)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C6">
-        <v>259.77452149999999</v>
+        <v>258.81446801658478</v>
       </c>
       <c r="D6">
-        <v>1435.975827</v>
+        <v>1430.6688648694551</v>
       </c>
       <c r="E6">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F6">
-        <v>14779380.25</v>
+        <v>14609557.41562718</v>
       </c>
       <c r="G6">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H6">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I6">
-        <v>9.2601513579999999</v>
+        <v>9.2601513577926973</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>71</v>
@@ -3899,15 +3899,15 @@
       </c>
       <c r="O6">
         <f>D22</f>
-        <v>1382.936637</v>
+        <v>1377.619467249845</v>
       </c>
       <c r="P6">
         <f>D6</f>
-        <v>1435.975827</v>
+        <v>1430.6688648694551</v>
       </c>
       <c r="Q6">
         <f>D10</f>
-        <v>1346.153939</v>
+        <v>1340.846976901094</v>
       </c>
       <c r="R6">
         <f>D42</f>
@@ -3923,29 +3923,29 @@
         <v>42</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A7)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C7">
-        <v>206.50488809999999</v>
+        <v>206.5048880551723</v>
       </c>
       <c r="D7">
-        <v>1141.5131309999999</v>
+        <v>1141.513131193869</v>
       </c>
       <c r="E7">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F7">
-        <v>5356571.892</v>
+        <v>5356571.8921226691</v>
       </c>
       <c r="G7">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H7">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I7">
-        <v>9.2601513579999999</v>
+        <v>9.2601513577926973</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
@@ -3953,29 +3953,29 @@
         <v>45</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A8)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C8">
-        <v>257.67351580000002</v>
+        <v>256.71346234334891</v>
       </c>
       <c r="D8">
-        <v>1424.3619349999999</v>
+        <v>1419.0549723979559</v>
       </c>
       <c r="E8">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F8">
-        <v>14779380.25</v>
+        <v>14609557.41562718</v>
       </c>
       <c r="G8">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H8">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I8">
-        <v>9.3718871359999998</v>
+        <v>9.3718871360488567</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
@@ -3983,29 +3983,29 @@
         <v>46</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A9)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C9">
-        <v>204.40388239999999</v>
+        <v>204.4038823819362</v>
       </c>
       <c r="D9">
-        <v>1129.8992390000001</v>
+        <v>1129.89923872237</v>
       </c>
       <c r="E9">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F9">
-        <v>5356571.892</v>
+        <v>5356571.8921226691</v>
       </c>
       <c r="G9">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H9">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I9">
-        <v>9.3718871359999998</v>
+        <v>9.3718871360488567</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
@@ -4013,29 +4013,29 @@
         <v>47</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A10)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C10">
-        <v>243.52533579999999</v>
+        <v>242.56528225346429</v>
       </c>
       <c r="D10">
-        <v>1346.153939</v>
+        <v>1340.846976901094</v>
       </c>
       <c r="E10">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F10">
-        <v>14779380.25</v>
+        <v>14609557.41562718</v>
       </c>
       <c r="G10">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H10">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I10">
-        <v>10.200743660000001</v>
+        <v>10.200743662079301</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -4043,29 +4043,29 @@
         <v>48</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A11)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C11">
-        <v>190.2557023</v>
+        <v>190.25570229205169</v>
       </c>
       <c r="D11">
-        <v>1051.691243</v>
+        <v>1051.6912432255081</v>
       </c>
       <c r="E11">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F11">
-        <v>5356571.892</v>
+        <v>5356571.8921226691</v>
       </c>
       <c r="G11">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H11">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I11">
-        <v>10.200743660000001</v>
+        <v>10.200743662079301</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
@@ -4073,29 +4073,29 @@
         <v>39</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A12)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C12">
-        <v>265.85897949999998</v>
+        <v>264.88871206184581</v>
       </c>
       <c r="D12">
-        <v>1469.609359</v>
+        <v>1464.245936119647</v>
       </c>
       <c r="E12">
-        <v>315776480.60000002</v>
+        <v>315776480.57557988</v>
       </c>
       <c r="F12">
-        <v>14864977.85</v>
+        <v>14693348.27489705</v>
       </c>
       <c r="G12">
         <v>176888.92800000001</v>
       </c>
       <c r="H12">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I12">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
@@ -4103,29 +4103,29 @@
         <v>40</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A13)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C13">
-        <v>212.5056055</v>
+        <v>212.50560551542549</v>
       </c>
       <c r="D13">
-        <v>1174.6837640000001</v>
+        <v>1174.6837638213799</v>
       </c>
       <c r="E13">
-        <v>315776480.60000002</v>
+        <v>315776480.57557988</v>
       </c>
       <c r="F13">
-        <v>5427356.7130000005</v>
+        <v>5427356.7125909813</v>
       </c>
       <c r="G13">
         <v>176888.92800000001</v>
       </c>
       <c r="H13">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I13">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
@@ -4133,29 +4133,29 @@
         <v>37</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A14)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C14">
-        <v>233.6297476</v>
+        <v>232.67786899660581</v>
       </c>
       <c r="D14">
-        <v>1291.4533269999999</v>
+        <v>1286.1915536201259</v>
       </c>
       <c r="E14">
-        <v>261493301.09999999</v>
+        <v>261493301.12125921</v>
       </c>
       <c r="F14">
-        <v>14692845.300000001</v>
+        <v>14524468.504476029</v>
       </c>
       <c r="G14">
-        <v>176888.92800000001</v>
+        <v>176888.9279999978</v>
       </c>
       <c r="H14">
-        <v>32000.007079999999</v>
+        <v>32000.007075376489</v>
       </c>
       <c r="I14">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
@@ -4163,29 +4163,29 @@
         <v>38</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A15)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C15">
-        <v>180.42523990000001</v>
+        <v>180.4252399032205</v>
       </c>
       <c r="D15">
-        <v>997.35063170000001</v>
+        <v>997.35063168724673</v>
       </c>
       <c r="E15">
-        <v>261493301.09999999</v>
+        <v>261493301.12125921</v>
       </c>
       <c r="F15">
-        <v>5281556.9589999998</v>
+        <v>5281556.9589656191</v>
       </c>
       <c r="G15">
-        <v>176888.92800000001</v>
+        <v>176888.9279999978</v>
       </c>
       <c r="H15">
-        <v>32000.007079999999</v>
+        <v>32000.007075376489</v>
       </c>
       <c r="I15">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
@@ -4193,7 +4193,7 @@
         <v>33</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A16)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C16">
@@ -4223,7 +4223,7 @@
         <v>34</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A17)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C17">
@@ -4253,7 +4253,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A18)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C18">
@@ -4283,7 +4283,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A19)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C19">
@@ -4313,29 +4313,29 @@
         <v>49</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A20)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C20">
-        <v>249.32343990000001</v>
+        <v>248.3884768276512</v>
       </c>
       <c r="D20">
-        <v>1378.204571</v>
+        <v>1373.036302463961</v>
       </c>
       <c r="E20">
-        <v>287503256.69999999</v>
+        <v>287503256.69952732</v>
       </c>
       <c r="F20">
-        <v>14819714.279999999</v>
+        <v>14654329.654899949</v>
       </c>
       <c r="G20">
         <v>176888.92800000001</v>
       </c>
       <c r="H20">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I20">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -4343,29 +4343,29 @@
         <v>50</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A21)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C21">
-        <v>196.1055806</v>
+        <v>196.10558061303411</v>
       </c>
       <c r="D21">
-        <v>1084.028071</v>
+        <v>1084.0280706109379</v>
       </c>
       <c r="E21">
-        <v>287503256.69999999</v>
+        <v>287503256.69952732</v>
       </c>
       <c r="F21">
-        <v>5406064.1909999996</v>
+        <v>5406064.1907610623</v>
       </c>
       <c r="G21">
         <v>176888.92800000001</v>
       </c>
       <c r="H21">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I21">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -4373,29 +4373,29 @@
         <v>61</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A22)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C22">
-        <v>250.1794921</v>
+        <v>249.2175920652985</v>
       </c>
       <c r="D22">
-        <v>1382.936637</v>
+        <v>1377.619467249845</v>
       </c>
       <c r="E22">
-        <v>289790455.39999998</v>
+        <v>289790455.41130489</v>
       </c>
       <c r="F22">
-        <v>14738184.18</v>
+        <v>14568034.719663819</v>
       </c>
       <c r="G22">
         <v>176888.92800000001</v>
       </c>
       <c r="H22">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I22">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -4403,29 +4403,29 @@
         <v>62</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A23)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C23">
-        <v>196.81776840000001</v>
+        <v>196.81776838803489</v>
       </c>
       <c r="D23">
-        <v>1087.964886</v>
+        <v>1087.964886367193</v>
       </c>
       <c r="E23">
-        <v>289790455.39999998</v>
+        <v>289790455.41130489</v>
       </c>
       <c r="F23">
-        <v>5299086.0820000004</v>
+        <v>5299086.0820036363</v>
       </c>
       <c r="G23">
         <v>176888.92800000001</v>
       </c>
       <c r="H23">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I23">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -4433,29 +4433,29 @@
         <v>63</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A24)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C24">
-        <v>244.84277760000001</v>
+        <v>243.88272410187591</v>
       </c>
       <c r="D24">
-        <v>1353.436465</v>
+        <v>1348.129502674258</v>
       </c>
       <c r="E24">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F24">
-        <v>14779380.25</v>
+        <v>14609557.41562718</v>
       </c>
       <c r="G24">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H24">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I24">
-        <v>10.11742293</v>
+        <v>10.117422927236451</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -4463,29 +4463,29 @@
         <v>64</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A25)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C25">
-        <v>191.57314410000001</v>
+        <v>191.57314414046331</v>
       </c>
       <c r="D25">
-        <v>1058.9737689999999</v>
+        <v>1058.9737689986721</v>
       </c>
       <c r="E25">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F25">
-        <v>5356571.892</v>
+        <v>5356571.8921226691</v>
       </c>
       <c r="G25">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H25">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I25">
-        <v>10.11742293</v>
+        <v>10.117422927236451</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -4493,29 +4493,29 @@
         <v>65</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A26)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C26">
-        <v>254.73703860000001</v>
+        <v>253.77698512527061</v>
       </c>
       <c r="D26">
-        <v>1408.129741</v>
+        <v>1402.8227788869131</v>
       </c>
       <c r="E26">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F26">
-        <v>14779380.25</v>
+        <v>14609557.41562718</v>
       </c>
       <c r="G26">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H26">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I26">
-        <v>9.5326505640000008</v>
+        <v>9.5326505636609351</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -4523,29 +4523,29 @@
         <v>66</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A27)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C27">
-        <v>201.4674052</v>
+        <v>201.4674051638581</v>
       </c>
       <c r="D27">
-        <v>1113.6670449999999</v>
+        <v>1113.667045211326</v>
       </c>
       <c r="E27">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F27">
-        <v>5356571.892</v>
+        <v>5356571.8921226691</v>
       </c>
       <c r="G27">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H27">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I27">
-        <v>9.5326505640000008</v>
+        <v>9.5326505636609351</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -4553,29 +4553,29 @@
         <v>67</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A28)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C28">
-        <v>253.47237079999999</v>
+        <v>252.51231734403791</v>
       </c>
       <c r="D28">
-        <v>1401.1389389999999</v>
+        <v>1395.831976429542</v>
       </c>
       <c r="E28">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F28">
-        <v>14779380.25</v>
+        <v>14609557.41562718</v>
       </c>
       <c r="G28">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H28">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I28">
-        <v>9.6035991999999997</v>
+        <v>9.6035992000452381</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -4583,29 +4583,29 @@
         <v>68</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A29)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C29">
-        <v>200.20273739999999</v>
+        <v>200.20273738262529</v>
       </c>
       <c r="D29">
-        <v>1106.6762430000001</v>
+        <v>1106.6762427539561</v>
       </c>
       <c r="E29">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F29">
-        <v>5356571.892</v>
+        <v>5356571.8921226691</v>
       </c>
       <c r="G29">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H29">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I29">
-        <v>9.6035991999999997</v>
+        <v>9.6035992000452381</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -4613,29 +4613,29 @@
         <v>69</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A30)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C30">
-        <v>246.46296179999999</v>
+        <v>245.50290828341409</v>
       </c>
       <c r="D30">
-        <v>1362.3924830000001</v>
+        <v>1357.0855207888719</v>
       </c>
       <c r="E30">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F30">
-        <v>14779380.25</v>
+        <v>14609557.41562718</v>
       </c>
       <c r="G30">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H30">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I30">
-        <v>10.01680316</v>
+        <v>10.01680315504564</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -4643,29 +4643,29 @@
         <v>70</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A31)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C31">
-        <v>193.19332829999999</v>
+        <v>193.19332832200149</v>
       </c>
       <c r="D31">
-        <v>1067.929787</v>
+        <v>1067.929787113286</v>
       </c>
       <c r="E31">
-        <v>288656108.19999999</v>
+        <v>288656108.20733207</v>
       </c>
       <c r="F31">
-        <v>5356571.892</v>
+        <v>5356571.8921226691</v>
       </c>
       <c r="G31">
-        <v>176888.92800000001</v>
+        <v>176888.9279999992</v>
       </c>
       <c r="H31">
-        <v>32000.007079999999</v>
+        <v>32000.00707537675</v>
       </c>
       <c r="I31">
-        <v>10.01680316</v>
+        <v>10.01680315504564</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -4673,7 +4673,7 @@
         <v>75</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A32)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C32">
@@ -4703,7 +4703,7 @@
         <v>76</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A33)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C33">
@@ -4733,7 +4733,7 @@
         <v>77</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A34)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C34">
@@ -4763,7 +4763,7 @@
         <v>78</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A35)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C35">
@@ -4793,7 +4793,7 @@
         <v>81</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A36)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C36">
@@ -4823,7 +4823,7 @@
         <v>82</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A37)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C37">
@@ -4853,7 +4853,7 @@
         <v>79</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" ref="B38:B39" si="2">IF(ISNUMBER(SEARCH("PV", A38)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A38)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C38">
@@ -4883,7 +4883,7 @@
         <v>80</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A39)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C39">
@@ -4913,7 +4913,7 @@
         <v>37</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" ref="B40:B41" si="3">IF(ISNUMBER(SEARCH("PV", A40)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A40)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C40">
@@ -4943,7 +4943,7 @@
         <v>38</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A41)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C41">
@@ -4973,7 +4973,7 @@
         <v>39</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" ref="B42:B45" si="4">IF(ISNUMBER(SEARCH("PV", A42)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A42)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C42">
@@ -5003,7 +5003,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A43)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C43">
@@ -5033,7 +5033,7 @@
         <v>84</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" ref="B44" si="5">IF(ISNUMBER(SEARCH("PV", A44)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A44)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C44">
@@ -5063,7 +5063,7 @@
         <v>85</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A45)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C45">
@@ -5093,7 +5093,7 @@
         <v>86</v>
       </c>
       <c r="B46" t="str">
-        <f t="shared" ref="B46:B47" si="6">IF(ISNUMBER(SEARCH("PV", A46)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A46)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C46">
@@ -5123,7 +5123,7 @@
         <v>87</v>
       </c>
       <c r="B47" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A47)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C47">
@@ -5153,7 +5153,7 @@
         <v>88</v>
       </c>
       <c r="B48" t="str">
-        <f t="shared" ref="B48:B51" si="7">IF(ISNUMBER(SEARCH("PV", A48)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A48)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C48">
@@ -5178,12 +5178,12 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>89</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A49)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C49">
@@ -5208,12 +5208,12 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>90</v>
       </c>
       <c r="B50" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A50)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C50">
@@ -5238,12 +5238,12 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>91</v>
       </c>
       <c r="B51" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A51)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C51">
@@ -5268,12 +5268,12 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>92</v>
       </c>
       <c r="B52" t="str">
-        <f t="shared" ref="B52:B55" si="8">IF(ISNUMBER(SEARCH("PV", A52)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A52)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C52">
@@ -5298,12 +5298,12 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>93</v>
       </c>
       <c r="B53" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A53)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C53">
@@ -5328,12 +5328,12 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>94</v>
       </c>
       <c r="B54" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A54)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C54">
@@ -5358,12 +5358,12 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>95</v>
       </c>
       <c r="B55" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A55)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C55">
@@ -5388,12 +5388,12 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>96</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" ref="B56:B58" si="9">IF(ISNUMBER(SEARCH("PV", A56)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A56)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C56">
@@ -5417,13 +5417,34 @@
       <c r="I56">
         <v>9.8181474069999997</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K56">
+        <v>249.0571825508363</v>
+      </c>
+      <c r="L56">
+        <v>1376.732759100456</v>
+      </c>
+      <c r="M56">
+        <v>289280462.7805413</v>
+      </c>
+      <c r="N56">
+        <v>14591603.928536391</v>
+      </c>
+      <c r="O56">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="P56">
+        <v>32000.007075376881</v>
+      </c>
+      <c r="Q56">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>97</v>
       </c>
       <c r="B57" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A57)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C57">
@@ -5447,13 +5468,34 @@
       <c r="I57">
         <v>9.8181474069999997</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K57">
+        <v>196.6836710467953</v>
+      </c>
+      <c r="L57">
+        <v>1087.2236260642289</v>
+      </c>
+      <c r="M57">
+        <v>289280462.7805413</v>
+      </c>
+      <c r="N57">
+        <v>5327309.622990909</v>
+      </c>
+      <c r="O57">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="P57">
+        <v>32000.007075376881</v>
+      </c>
+      <c r="Q57">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>98</v>
       </c>
       <c r="B58" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A58)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C58">
@@ -5478,132 +5520,132 @@
         <v>9.8181474069999997</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>99</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" ref="B59:B62" si="10">IF(ISNUMBER(SEARCH("PV", A59)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A59)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C59">
-        <v>257.80078750000001</v>
+        <v>256.83554585130742</v>
       </c>
       <c r="D59">
-        <v>1425.065464</v>
+        <v>1419.729822900282</v>
       </c>
       <c r="E59">
-        <v>302186986.10000002</v>
+        <v>302186986.11188918</v>
       </c>
       <c r="F59">
-        <v>14823692.92</v>
+        <v>14652952.36482597</v>
       </c>
       <c r="G59">
         <v>176888.92800000001</v>
       </c>
       <c r="H59">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I59">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>100</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" si="10"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A60)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C60">
-        <v>204.48719790000001</v>
+        <v>204.4871979357284</v>
       </c>
       <c r="D60">
-        <v>1130.3597890000001</v>
+        <v>1130.359788589165</v>
       </c>
       <c r="E60">
-        <v>302186986.10000002</v>
+        <v>302186986.11188918</v>
       </c>
       <c r="F60">
-        <v>5393109.2189999996</v>
+        <v>5393109.2194681587</v>
       </c>
       <c r="G60">
         <v>176888.92800000001</v>
       </c>
       <c r="H60">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I60">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>101</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="10"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A61)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C61">
-        <v>241.72339030000001</v>
+        <v>240.76916765020661</v>
       </c>
       <c r="D61">
-        <v>1336.1931850000001</v>
+        <v>1330.918454510864</v>
       </c>
       <c r="E61">
-        <v>275093145</v>
+        <v>275093144.98216528</v>
       </c>
       <c r="F61">
-        <v>14739346.93</v>
+        <v>14570555.512556581</v>
       </c>
       <c r="G61">
         <v>176888.92800000001</v>
       </c>
       <c r="H61">
-        <v>32000.007079999999</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I61">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>102</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="10"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A62)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C62">
-        <v>188.46969340000001</v>
+        <v>188.46969340611801</v>
       </c>
       <c r="D62">
-        <v>1041.818583</v>
+        <v>1041.81858299493</v>
       </c>
       <c r="E62">
-        <v>275093145</v>
+        <v>275093144.98216528</v>
       </c>
       <c r="F62">
-        <v>5319357.5789999999</v>
+        <v>5319357.578556139</v>
       </c>
       <c r="G62">
         <v>176888.92800000001</v>
       </c>
       <c r="H62">
-        <v>32000.007079999999</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I62">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>107</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" ref="B63:B64" si="11">IF(ISNUMBER(SEARCH("PV", A63)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A63)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C63">
@@ -5628,12 +5670,12 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>108</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="11"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A64)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C64">
@@ -5663,7 +5705,7 @@
         <v>110</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" ref="B65:B66" si="12">IF(ISNUMBER(SEARCH("PV", A65)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A65)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C65">
@@ -5693,7 +5735,7 @@
         <v>111</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A66)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C66">
@@ -5723,7 +5765,7 @@
         <v>112</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B70" si="13">IF(ISNUMBER(SEARCH("PV", A67)),"PV revenue","no PV revenue")</f>
+        <f>IF(ISNUMBER(SEARCH("PV", A67)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C67">
@@ -5753,7 +5795,7 @@
         <v>113</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="13"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A68)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C68">
@@ -5783,7 +5825,7 @@
         <v>114</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="13"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A69)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C69">
@@ -5813,7 +5855,7 @@
         <v>115</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="13"/>
+        <f>IF(ISNUMBER(SEARCH("PV", A70)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C70">

</xml_diff>

<commit_message>
update LCOE comparison file
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\Nord_H2ub\Spine_Projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB25A8D5-2DCF-4870-9E70-E63E6172A55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080F5BAF-17EA-474A-8728-19A3CFB906B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4575" yWindow="-21720" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
+    <workbookView xWindow="-4575" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_operating_points" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="117">
   <si>
     <t>run_name</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>sens_10op_eff_05pup_PV</t>
+  </si>
+  <si>
+    <t>sens_10op_elpricevar_05pup_PV</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -467,6 +470,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,19 +621,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1460.0010057815159</c:v>
+                  <c:v>1454.045405478545</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1418.2136820000001</c:v>
+                  <c:v>1412.603841081253</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1375.306559250821</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1346.491194521597</c:v>
+                  <c:v>1341.454298811055</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1316.106550648097</c:v>
+                  <c:v>1311.327752139872</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -699,19 +703,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1402.002937</c:v>
+                  <c:v>1396.6959745948291</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1391.308229</c:v>
+                  <c:v>1386.00126692346</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1375.306559250821</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1369.9188140002141</c:v>
+                  <c:v>1364.611851578283</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1359.2241063280269</c:v>
+                  <c:v>1353.917143906094</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,19 +785,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1351.5309569999999</c:v>
+                  <c:v>1346.6594790660861</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1364.533322</c:v>
+                  <c:v>1359.37264784218</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1375.306559250821</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1395.6319209999999</c:v>
+                  <c:v>1390.098427253407</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1411.267407</c:v>
+                  <c:v>1405.5186829752231</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -866,13 +870,13 @@
                   <c:v>1373.036302463961</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1379.349964</c:v>
+                  <c:v>1374.0552236487399</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1375.306559250821</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1382.02367</c:v>
+                  <c:v>1376.732759100456</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1377.619467249845</c:v>
@@ -1191,19 +1195,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1451.739909044454</c:v>
+                  <c:v>1446.557610246537</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1413.9417530000001</c:v>
+                  <c:v>1408.6894464016571</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1375.306559250821</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1350.335787788548</c:v>
+                  <c:v>1344.982327779471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1322.950869015936</c:v>
+                  <c:v>1317.5571897504819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2030,8 +2034,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I70" totalsRowShown="0">
-  <autoFilter ref="A1:I70" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}" name="Table3" displayName="Table3" ref="A1:I71" totalsRowShown="0">
+  <autoFilter ref="A1:I71" xr:uid="{1ED8C3B7-1CFE-4D76-BF2B-418405C32F6D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8869914E-4BE8-401C-AC76-C6570071019E}" name="run_name"/>
     <tableColumn id="9" xr3:uid="{91B3AAB6-6FBC-4E2C-8674-ECB365CA16C8}" name="PV" dataDxfId="0">
@@ -2368,8 +2372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB416CA-7C9B-4F0E-AFD4-34077EF25340}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2482,16 +2486,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C4">
-        <v>248.61588475600149</v>
+        <v>247.65971332537151</v>
       </c>
       <c r="D4">
-        <v>1374.293362956786</v>
+        <v>1369.007859770803</v>
       </c>
       <c r="E4">
         <v>286911074.34615147</v>
       </c>
       <c r="F4">
-        <v>14754870.68028195</v>
+        <v>14585734.54093357</v>
       </c>
       <c r="G4">
         <v>176888.92800000001</v>
@@ -2542,16 +2546,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C6">
-        <v>249.09406839490649</v>
+        <v>248.1410992801309</v>
       </c>
       <c r="D6">
-        <v>1376.936655849622</v>
+        <v>1371.668854354057</v>
       </c>
       <c r="E6">
         <v>287398388.41068858</v>
       </c>
       <c r="F6">
-        <v>14789822.057691149</v>
+        <v>14621252.372561401</v>
       </c>
       <c r="G6">
         <v>176888.9279999994</v>
@@ -2602,16 +2606,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C8">
-        <v>249.52192327091299</v>
+        <v>248.55909255802581</v>
       </c>
       <c r="D8">
-        <v>1379.3017425253249</v>
+        <v>1373.979428306865</v>
       </c>
       <c r="E8">
         <v>288262499.99587762</v>
       </c>
       <c r="F8">
-        <v>14777493.17442679</v>
+        <v>14607179.0817787</v>
       </c>
       <c r="G8">
         <v>176888.92800000121</v>
@@ -2662,25 +2666,25 @@
         <v>no PV revenue</v>
       </c>
       <c r="C10">
-        <v>249.74026509999999</v>
+        <v>248.78092043399039</v>
       </c>
       <c r="D10">
-        <v>1380.5086879999999</v>
+        <v>1375.205643510114</v>
       </c>
       <c r="E10">
-        <v>288545796.10000002</v>
+        <v>288545796.10135227</v>
       </c>
       <c r="F10">
-        <v>14787261.09</v>
+        <v>14617563.64286468</v>
       </c>
       <c r="G10">
-        <v>176888.92800000001</v>
+        <v>176888.9279999999</v>
       </c>
       <c r="H10">
-        <v>32000.007079999999</v>
+        <v>32000.00707537687</v>
       </c>
       <c r="I10">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2692,25 +2696,25 @@
         <v>PV revenue</v>
       </c>
       <c r="C11">
-        <v>196.42587169999999</v>
+        <v>196.42587174282141</v>
       </c>
       <c r="D11">
-        <v>1085.798569</v>
+        <v>1085.7985688005961</v>
       </c>
       <c r="E11">
-        <v>288545796.10000002</v>
+        <v>288545796.10135227</v>
       </c>
       <c r="F11">
-        <v>5356535.2039999999</v>
+        <v>5356535.2044959934</v>
       </c>
       <c r="G11">
-        <v>176888.92800000001</v>
+        <v>176888.9279999999</v>
       </c>
       <c r="H11">
-        <v>32000.007079999999</v>
+        <v>32000.00707537687</v>
       </c>
       <c r="I11">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -2722,25 +2726,25 @@
         <v>no PV revenue</v>
       </c>
       <c r="C12">
-        <v>249.62509220000001</v>
+        <v>248.6645878463564</v>
       </c>
       <c r="D12">
-        <v>1379.8720370000001</v>
+        <v>1374.562582817359</v>
       </c>
       <c r="E12">
-        <v>288420132.5</v>
+        <v>288420132.5394364</v>
       </c>
       <c r="F12">
-        <v>14779687.390000001</v>
+        <v>14609784.807496339</v>
       </c>
       <c r="G12">
-        <v>176888.92800000001</v>
+        <v>176888.9279999999</v>
       </c>
       <c r="H12">
-        <v>32000.007079999999</v>
+        <v>32000.00707537687</v>
       </c>
       <c r="I12">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2752,25 +2756,25 @@
         <v>PV revenue</v>
       </c>
       <c r="C13">
-        <v>196.316168</v>
+        <v>196.31616803455429</v>
       </c>
       <c r="D13">
-        <v>1085.192151</v>
+        <v>1085.192151079897</v>
       </c>
       <c r="E13">
-        <v>288420132.5</v>
+        <v>288420132.5394364</v>
       </c>
       <c r="F13">
-        <v>5349928.9440000001</v>
+        <v>5349928.9444927163</v>
       </c>
       <c r="G13">
-        <v>176888.92800000001</v>
+        <v>176888.9279999999</v>
       </c>
       <c r="H13">
-        <v>32000.007079999999</v>
+        <v>32000.00707537687</v>
       </c>
       <c r="I13">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2782,16 +2786,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C14">
-        <v>249.78260672031831</v>
+        <v>248.82119706348129</v>
       </c>
       <c r="D14">
-        <v>1380.742742703982</v>
+        <v>1375.4282837675771</v>
       </c>
       <c r="E14">
         <v>288709501.92547369</v>
       </c>
       <c r="F14">
-        <v>14778077.05646155</v>
+        <v>14608014.33289481</v>
       </c>
       <c r="G14">
         <v>176888.92800000001</v>
@@ -2842,16 +2846,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C16">
-        <v>249.7243263809365</v>
+        <v>248.76446967345879</v>
       </c>
       <c r="D16">
-        <v>1380.4205819390661</v>
+        <v>1375.11470736162</v>
       </c>
       <c r="E16">
         <v>288705429.34616148</v>
       </c>
       <c r="F16">
-        <v>14768182.710903389</v>
+        <v>14598394.686884061</v>
       </c>
       <c r="G16">
         <v>176888.92800000001</v>
@@ -2902,25 +2906,25 @@
         <v>no PV revenue</v>
       </c>
       <c r="C18">
-        <v>249.71998909999999</v>
+        <v>248.76067696964361</v>
       </c>
       <c r="D18">
-        <v>1380.3966069999999</v>
+        <v>1375.0937421377521</v>
       </c>
       <c r="E18">
-        <v>288557068.60000002</v>
+        <v>288557068.64214009</v>
       </c>
       <c r="F18">
-        <v>14782526.369999999</v>
+        <v>14612834.6649791</v>
       </c>
       <c r="G18">
         <v>176888.92800000001</v>
       </c>
       <c r="H18">
-        <v>32000.007079999999</v>
+        <v>32000.0070753769</v>
       </c>
       <c r="I18">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -2932,25 +2936,25 @@
         <v>PV revenue</v>
       </c>
       <c r="C19">
-        <v>196.4490965</v>
+        <v>196.44909651789939</v>
       </c>
       <c r="D19">
-        <v>1085.92695</v>
+        <v>1085.926950196166</v>
       </c>
       <c r="E19">
-        <v>288557068.60000002</v>
+        <v>288557068.64214009</v>
       </c>
       <c r="F19">
-        <v>5359495.2769999998</v>
+        <v>5359495.2768843267</v>
       </c>
       <c r="G19">
         <v>176888.92800000001</v>
       </c>
       <c r="H19">
-        <v>32000.007079999999</v>
+        <v>32000.0070753769</v>
       </c>
       <c r="I19">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -2962,16 +2966,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C20">
-        <v>249.75918061460271</v>
+        <v>248.79969047828581</v>
       </c>
       <c r="D20">
-        <v>1380.613248397387</v>
+        <v>1375.3094001438581</v>
       </c>
       <c r="E20">
         <v>288687149.67850941</v>
       </c>
       <c r="F20">
-        <v>14776209.863460001</v>
+        <v>14606486.68182034</v>
       </c>
       <c r="G20">
         <v>176888.92800000089</v>
@@ -3022,16 +3026,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C22">
-        <v>249.73614149918711</v>
+        <v>248.777993090921</v>
       </c>
       <c r="D22">
-        <v>1380.485893287173</v>
+        <v>1375.189461808146</v>
       </c>
       <c r="E22">
         <v>288736929.04657698</v>
       </c>
       <c r="F22">
-        <v>14767064.360440319</v>
+        <v>14597578.51563721</v>
       </c>
       <c r="G22">
         <v>176888.9279999999</v>
@@ -3082,16 +3086,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C24">
-        <v>249.59496612046431</v>
+        <v>248.63789198365541</v>
       </c>
       <c r="D24">
-        <v>1379.7055071658999</v>
+        <v>1374.415014020761</v>
       </c>
       <c r="E24">
         <v>288563658.52300167</v>
       </c>
       <c r="F24">
-        <v>14759739.98456678</v>
+        <v>14590444.166490201</v>
       </c>
       <c r="G24">
         <v>176888.9279999143</v>
@@ -3146,7 +3150,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C4" sqref="C4:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3279,16 +3283,16 @@
         <v>no PV revenue</v>
       </c>
       <c r="C4">
-        <v>248.61588475600149</v>
+        <v>247.65971332537151</v>
       </c>
       <c r="D4">
-        <v>1374.293362956786</v>
+        <v>1369.007859770803</v>
       </c>
       <c r="E4">
         <v>286911074.34615147</v>
       </c>
       <c r="F4">
-        <v>14754870.68028195</v>
+        <v>14585734.54093357</v>
       </c>
       <c r="G4">
         <v>176888.92800000001</v>
@@ -3502,10 +3506,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
-  <dimension ref="A1:V70"/>
+  <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="Q51" sqref="Q51"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3582,7 +3586,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A2)),"PV revenue","no PV revenue")</f>
+        <f t="shared" ref="B2:B33" si="0">IF(ISNUMBER(SEARCH("PV", A2)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C2">
@@ -3611,15 +3615,15 @@
       </c>
       <c r="L2">
         <f>D32</f>
-        <v>1460.0010057815159</v>
+        <v>1454.045405478545</v>
       </c>
       <c r="M2">
         <f>D36</f>
-        <v>1402.002937</v>
+        <v>1396.6959745948291</v>
       </c>
       <c r="N2">
         <f>D16</f>
-        <v>1351.5309569999999</v>
+        <v>1346.6594790660861</v>
       </c>
       <c r="O2">
         <f>D20</f>
@@ -3638,8 +3642,8 @@
         <v>1326.412694499294</v>
       </c>
       <c r="S2">
-        <f>D63</f>
-        <v>1451.739909044454</v>
+        <f>D64</f>
+        <v>1446.557610246537</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
@@ -3647,7 +3651,7 @@
         <v>27</v>
       </c>
       <c r="B3" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A3)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C3">
@@ -3676,19 +3680,19 @@
       </c>
       <c r="L3">
         <f>D44</f>
-        <v>1418.2136820000001</v>
+        <v>1412.603841081253</v>
       </c>
       <c r="M3">
         <f>D48</f>
-        <v>1391.308229</v>
+        <v>1386.00126692346</v>
       </c>
       <c r="N3">
         <f>D52</f>
-        <v>1364.533322</v>
+        <v>1359.37264784218</v>
       </c>
       <c r="O3">
         <f>D56</f>
-        <v>1379.349964</v>
+        <v>1374.0552236487399</v>
       </c>
       <c r="P3">
         <f>D24</f>
@@ -3699,12 +3703,12 @@
         <v>1395.831976429542</v>
       </c>
       <c r="R3">
-        <f>D61</f>
+        <f>D62</f>
         <v>1330.918454510864</v>
       </c>
       <c r="S3">
-        <f>D65</f>
-        <v>1413.9417530000001</v>
+        <f>D66</f>
+        <v>1408.6894464016571</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
@@ -3712,7 +3716,7 @@
         <v>41</v>
       </c>
       <c r="B4" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A4)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C4">
@@ -3744,31 +3748,31 @@
         <v>1375.306559250821</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" ref="M4:S4" si="0">$D$2</f>
+        <f t="shared" ref="M4:S4" si="1">$D$2</f>
         <v>1375.306559250821</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1375.306559250821</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1375.306559250821</v>
       </c>
       <c r="P4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1375.306559250821</v>
       </c>
       <c r="Q4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1375.306559250821</v>
       </c>
       <c r="R4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1375.306559250821</v>
       </c>
       <c r="S4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1375.306559250821</v>
       </c>
       <c r="U4" s="4">
@@ -3785,7 +3789,7 @@
         <v>43</v>
       </c>
       <c r="B5" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A5)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C5">
@@ -3814,19 +3818,19 @@
       </c>
       <c r="L5">
         <f>D46</f>
-        <v>1346.491194521597</v>
+        <v>1341.454298811055</v>
       </c>
       <c r="M5">
         <f>D50</f>
-        <v>1369.9188140002141</v>
+        <v>1364.611851578283</v>
       </c>
       <c r="N5">
         <f>D54</f>
-        <v>1395.6319209999999</v>
+        <v>1390.098427253407</v>
       </c>
       <c r="O5">
         <f>D58</f>
-        <v>1382.02367</v>
+        <v>1376.732759100456</v>
       </c>
       <c r="P5">
         <f>D26</f>
@@ -3837,12 +3841,12 @@
         <v>1357.0855207888719</v>
       </c>
       <c r="R5">
-        <f>D59</f>
+        <f>D60</f>
         <v>1419.729822900282</v>
       </c>
       <c r="S5">
-        <f>D69</f>
-        <v>1350.335787788548</v>
+        <f>D70</f>
+        <v>1344.982327779471</v>
       </c>
       <c r="U5">
         <f>R6/P4</f>
@@ -3858,7 +3862,7 @@
         <v>44</v>
       </c>
       <c r="B6" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A6)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C6">
@@ -3887,15 +3891,15 @@
       </c>
       <c r="L6">
         <f>D34</f>
-        <v>1316.106550648097</v>
+        <v>1311.327752139872</v>
       </c>
       <c r="M6">
         <f>D38</f>
-        <v>1359.2241063280269</v>
+        <v>1353.917143906094</v>
       </c>
       <c r="N6">
         <f>D18</f>
-        <v>1411.267407</v>
+        <v>1405.5186829752231</v>
       </c>
       <c r="O6">
         <f>D22</f>
@@ -3914,8 +3918,8 @@
         <v>1504.5687264186249</v>
       </c>
       <c r="S6">
-        <f>D67</f>
-        <v>1322.950869015936</v>
+        <f>D68</f>
+        <v>1317.5571897504819</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
@@ -3923,7 +3927,7 @@
         <v>42</v>
       </c>
       <c r="B7" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A7)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C7">
@@ -3953,7 +3957,7 @@
         <v>45</v>
       </c>
       <c r="B8" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A8)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C8">
@@ -3983,7 +3987,7 @@
         <v>46</v>
       </c>
       <c r="B9" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A9)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C9">
@@ -4013,7 +4017,7 @@
         <v>47</v>
       </c>
       <c r="B10" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A10)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C10">
@@ -4043,7 +4047,7 @@
         <v>48</v>
       </c>
       <c r="B11" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A11)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C11">
@@ -4073,7 +4077,7 @@
         <v>39</v>
       </c>
       <c r="B12" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A12)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C12">
@@ -4103,7 +4107,7 @@
         <v>40</v>
       </c>
       <c r="B13" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A13)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C13">
@@ -4133,7 +4137,7 @@
         <v>37</v>
       </c>
       <c r="B14" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A14)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C14">
@@ -4163,7 +4167,7 @@
         <v>38</v>
       </c>
       <c r="B15" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A15)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C15">
@@ -4193,29 +4197,29 @@
         <v>33</v>
       </c>
       <c r="B16" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A16)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C16">
-        <v>244.4980626</v>
+        <v>243.61679018280961</v>
       </c>
       <c r="D16">
-        <v>1351.5309569999999</v>
+        <v>1346.6594790660861</v>
       </c>
       <c r="E16">
-        <v>286416416.60000002</v>
+        <v>286416416.59819239</v>
       </c>
       <c r="F16">
-        <v>14076855.51</v>
+        <v>13920968.184500519</v>
       </c>
       <c r="G16">
         <v>176888.92800000001</v>
       </c>
       <c r="H16">
-        <v>32000.007079999999</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I16">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -4223,29 +4227,29 @@
         <v>34</v>
       </c>
       <c r="B17" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A17)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C17">
-        <v>196.7205659</v>
+        <v>196.72056590748261</v>
       </c>
       <c r="D17">
-        <v>1087.4275729999999</v>
+        <v>1087.427572655251</v>
       </c>
       <c r="E17">
-        <v>286416416.60000002</v>
+        <v>286416416.59819239</v>
       </c>
       <c r="F17">
-        <v>5625545.3449999997</v>
+        <v>5625545.3451903481</v>
       </c>
       <c r="G17">
         <v>176888.92800000001</v>
       </c>
       <c r="H17">
-        <v>32000.007079999999</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I17">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -4253,29 +4257,29 @@
         <v>35</v>
       </c>
       <c r="B18" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A18)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C18">
-        <v>255.30465659999999</v>
+        <v>254.26468636737701</v>
       </c>
       <c r="D18">
-        <v>1411.267407</v>
+        <v>1405.5186829752231</v>
       </c>
       <c r="E18">
-        <v>291333845.30000001</v>
+        <v>291333845.31250137</v>
       </c>
       <c r="F18">
-        <v>15487571.369999999</v>
+        <v>15303612.149759781</v>
       </c>
       <c r="G18">
-        <v>176888.92800000001</v>
+        <v>176888.9279999944</v>
       </c>
       <c r="H18">
-        <v>32000.007079999999</v>
+        <v>32000.007075375881</v>
       </c>
       <c r="I18">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -4283,29 +4287,29 @@
         <v>36</v>
       </c>
       <c r="B19" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A19)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C19">
-        <v>196.4035853</v>
+        <v>196.40358526508251</v>
       </c>
       <c r="D19">
-        <v>1085.6753739999999</v>
+        <v>1085.675374104206</v>
       </c>
       <c r="E19">
-        <v>291333845.30000001</v>
+        <v>291333845.31250137</v>
       </c>
       <c r="F19">
-        <v>5068624.0029999996</v>
+        <v>5068624.0028756075</v>
       </c>
       <c r="G19">
-        <v>176888.92800000001</v>
+        <v>176888.9279999944</v>
       </c>
       <c r="H19">
-        <v>32000.007079999999</v>
+        <v>32000.007075375881</v>
       </c>
       <c r="I19">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -4313,7 +4317,7 @@
         <v>49</v>
       </c>
       <c r="B20" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A20)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C20">
@@ -4343,7 +4347,7 @@
         <v>50</v>
       </c>
       <c r="B21" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A21)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C21">
@@ -4373,7 +4377,7 @@
         <v>61</v>
       </c>
       <c r="B22" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A22)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C22">
@@ -4403,7 +4407,7 @@
         <v>62</v>
       </c>
       <c r="B23" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A23)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C23">
@@ -4433,7 +4437,7 @@
         <v>63</v>
       </c>
       <c r="B24" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A24)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C24">
@@ -4463,7 +4467,7 @@
         <v>64</v>
       </c>
       <c r="B25" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A25)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C25">
@@ -4493,7 +4497,7 @@
         <v>65</v>
       </c>
       <c r="B26" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A26)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C26">
@@ -4523,7 +4527,7 @@
         <v>66</v>
       </c>
       <c r="B27" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A27)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C27">
@@ -4553,7 +4557,7 @@
         <v>67</v>
       </c>
       <c r="B28" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A28)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C28">
@@ -4583,7 +4587,7 @@
         <v>68</v>
       </c>
       <c r="B29" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A29)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C29">
@@ -4613,7 +4617,7 @@
         <v>69</v>
       </c>
       <c r="B30" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A30)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C30">
@@ -4643,7 +4647,7 @@
         <v>70</v>
       </c>
       <c r="B31" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A31)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C31">
@@ -4673,20 +4677,20 @@
         <v>75</v>
       </c>
       <c r="B32" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A32)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>no PV revenue</v>
       </c>
       <c r="C32">
-        <v>264.12078496550038</v>
+        <v>263.04338993581717</v>
       </c>
       <c r="D32">
-        <v>1460.0010057815159</v>
+        <v>1454.045405478545</v>
       </c>
       <c r="E32">
         <v>277512962.69202578</v>
       </c>
       <c r="F32">
-        <v>13782730.036319871</v>
+        <v>13611208.709670009</v>
       </c>
       <c r="G32">
         <v>159200.03520000001</v>
@@ -4703,7 +4707,7 @@
         <v>76</v>
       </c>
       <c r="B33" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A33)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="0"/>
         <v>PV revenue</v>
       </c>
       <c r="C33">
@@ -4733,20 +4737,20 @@
         <v>77</v>
       </c>
       <c r="B34" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A34)),"PV revenue","no PV revenue")</f>
+        <f t="shared" ref="B34:B66" si="2">IF(ISNUMBER(SEARCH("PV", A34)),"PV revenue","no PV revenue")</f>
         <v>no PV revenue</v>
       </c>
       <c r="C34">
-        <v>238.08962725292201</v>
+        <v>237.22512099012761</v>
       </c>
       <c r="D34">
-        <v>1316.106550648097</v>
+        <v>1311.327752139872</v>
       </c>
       <c r="E34">
         <v>299683366.79336238</v>
       </c>
       <c r="F34">
-        <v>15803547.970495449</v>
+        <v>15635334.22581296</v>
       </c>
       <c r="G34">
         <v>194577.82079999999</v>
@@ -4763,7 +4767,7 @@
         <v>78</v>
       </c>
       <c r="B35" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A35)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C35">
@@ -4793,29 +4797,29 @@
         <v>81</v>
       </c>
       <c r="B36" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A36)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C36">
-        <v>253.62867199999999</v>
+        <v>252.6686185196676</v>
       </c>
       <c r="D36">
-        <v>1402.002937</v>
+        <v>1396.6959745948291</v>
       </c>
       <c r="E36">
-        <v>288656108.19999999</v>
+        <v>288656108.20669693</v>
       </c>
       <c r="F36">
-        <v>15463841.689999999</v>
+        <v>15294018.858038491</v>
       </c>
       <c r="G36">
         <v>176888.92800000001</v>
       </c>
       <c r="H36">
-        <v>32000.007079999999</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I36">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -4823,29 +4827,29 @@
         <v>82</v>
       </c>
       <c r="B37" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A37)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C37">
-        <v>200.35903859999999</v>
+        <v>200.359038558121</v>
       </c>
       <c r="D37">
-        <v>1107.5402409999999</v>
+        <v>1107.5402409185019</v>
       </c>
       <c r="E37">
-        <v>288656108.19999999</v>
+        <v>288656108.20669693</v>
       </c>
       <c r="F37">
-        <v>6041033.335</v>
+        <v>6041033.334510237</v>
       </c>
       <c r="G37">
         <v>176888.92800000001</v>
       </c>
       <c r="H37">
-        <v>32000.007079999999</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I37">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -4853,20 +4857,20 @@
         <v>79</v>
       </c>
       <c r="B38" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A38)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C38">
-        <v>245.8897880794421</v>
+        <v>244.92973457597691</v>
       </c>
       <c r="D38">
-        <v>1359.2241063280269</v>
+        <v>1353.917143906094</v>
       </c>
       <c r="E38">
         <v>288656108.2073791</v>
       </c>
       <c r="F38">
-        <v>14094918.80830376</v>
+        <v>13925095.97325315</v>
       </c>
       <c r="G38">
         <v>176888.92800000001</v>
@@ -4883,7 +4887,7 @@
         <v>80</v>
       </c>
       <c r="B39" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A39)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C39">
@@ -4913,7 +4917,7 @@
         <v>37</v>
       </c>
       <c r="B40" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A40)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C40">
@@ -4943,7 +4947,7 @@
         <v>38</v>
       </c>
       <c r="B41" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A41)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C41">
@@ -4973,7 +4977,7 @@
         <v>39</v>
       </c>
       <c r="B42" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A42)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C42">
@@ -5003,7 +5007,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A43)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C43">
@@ -5033,29 +5037,29 @@
         <v>84</v>
       </c>
       <c r="B44" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A44)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C44">
-        <v>256.5612691</v>
+        <v>255.54642351218649</v>
       </c>
       <c r="D44">
-        <v>1418.2136820000001</v>
+        <v>1412.603841081253</v>
       </c>
       <c r="E44">
-        <v>283106894.60000002</v>
+        <v>283106894.6123057</v>
       </c>
       <c r="F44">
-        <v>14278642.92</v>
+        <v>14108103.714289149</v>
       </c>
       <c r="G44">
-        <v>168044.4816</v>
+        <v>168044.48159912319</v>
       </c>
       <c r="H44">
-        <v>30400.006720000001</v>
+        <v>30400.006721449441</v>
       </c>
       <c r="I44">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -5063,29 +5067,29 @@
         <v>85</v>
       </c>
       <c r="B45" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A45)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C45">
-        <v>199.2670306</v>
+        <v>199.2670306329203</v>
       </c>
       <c r="D45">
-        <v>1101.503864</v>
+        <v>1101.503863776421</v>
       </c>
       <c r="E45">
-        <v>283106894.60000002</v>
+        <v>283106894.6123057</v>
       </c>
       <c r="F45">
-        <v>4650662.3130000001</v>
+        <v>4650662.3131794576</v>
       </c>
       <c r="G45">
-        <v>168044.4816</v>
+        <v>168044.48159912319</v>
       </c>
       <c r="H45">
-        <v>30400.006720000001</v>
+        <v>30400.006721449441</v>
       </c>
       <c r="I45">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -5093,20 +5097,20 @@
         <v>86</v>
       </c>
       <c r="B46" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A46)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C46">
-        <v>243.5863467476255</v>
+        <v>242.67514953365821</v>
       </c>
       <c r="D46">
-        <v>1346.491194521597</v>
+        <v>1341.454298811055</v>
       </c>
       <c r="E46">
         <v>294061734.4402532</v>
       </c>
       <c r="F46">
-        <v>15291276.95609845</v>
+        <v>15122037.22280442</v>
       </c>
       <c r="G46">
         <v>185733.3744</v>
@@ -5123,7 +5127,7 @@
         <v>87</v>
       </c>
       <c r="B47" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A47)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C47">
@@ -5153,80 +5157,80 @@
         <v>88</v>
       </c>
       <c r="B48" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A48)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C48">
-        <v>251.693951</v>
+        <v>250.7338975338923</v>
       </c>
       <c r="D48">
-        <v>1391.308229</v>
+        <v>1386.00126692346</v>
       </c>
       <c r="E48">
-        <v>288656108.19999999</v>
+        <v>288656108.20738328</v>
       </c>
       <c r="F48">
-        <v>15121610.970000001</v>
+        <v>14951788.13681569</v>
       </c>
       <c r="G48">
         <v>176888.92800000001</v>
       </c>
       <c r="H48">
-        <v>32000.007079999999</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I48">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>89</v>
       </c>
       <c r="B49" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A49)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C49">
-        <v>198.42431759999999</v>
+        <v>198.42431757247661</v>
       </c>
       <c r="D49">
-        <v>1096.8455329999999</v>
+        <v>1096.845533247857</v>
       </c>
       <c r="E49">
-        <v>288656108.19999999</v>
+        <v>288656108.20738328</v>
       </c>
       <c r="F49">
-        <v>5698802.6129999999</v>
+        <v>5698802.6133105904</v>
       </c>
       <c r="G49">
         <v>176888.92800000001</v>
       </c>
       <c r="H49">
-        <v>32000.007079999999</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I49">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>90</v>
       </c>
       <c r="B50" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A50)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C50">
-        <v>247.82450906536539</v>
+        <v>246.8644555619004</v>
       </c>
       <c r="D50">
-        <v>1369.9188140002141</v>
+        <v>1364.611851578283</v>
       </c>
       <c r="E50">
         <v>288656108.20732808</v>
       </c>
       <c r="F50">
-        <v>14437149.52949648</v>
+        <v>14267326.694445871</v>
       </c>
       <c r="G50">
         <v>176888.9280000341</v>
@@ -5238,12 +5242,12 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>91</v>
       </c>
       <c r="B51" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A51)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C51">
@@ -5268,307 +5272,265 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>92</v>
       </c>
       <c r="B52" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A52)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C52">
-        <v>246.8502493</v>
+        <v>245.9166599111482</v>
       </c>
       <c r="D52">
-        <v>1364.533322</v>
+        <v>1359.37264784218</v>
       </c>
       <c r="E52">
-        <v>288026061.10000002</v>
+        <v>288026061.1040557</v>
       </c>
       <c r="F52">
-        <v>14328985.449999999</v>
+        <v>14163843.826943729</v>
       </c>
       <c r="G52">
-        <v>176888.92800000001</v>
+        <v>176888.92799999981</v>
       </c>
       <c r="H52">
-        <v>32000.007079999999</v>
+        <v>32000.00707537686</v>
       </c>
       <c r="I52">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>93</v>
       </c>
       <c r="B53" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A53)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C53">
-        <v>196.2703564</v>
+        <v>196.27035637253809</v>
       </c>
       <c r="D53">
-        <v>1084.9389140000001</v>
+        <v>1084.938914392641</v>
       </c>
       <c r="E53">
-        <v>288026061.10000002</v>
+        <v>288026061.1040557</v>
       </c>
       <c r="F53">
-        <v>5381962.415</v>
+        <v>5381962.4148363862</v>
       </c>
       <c r="G53">
-        <v>176888.92800000001</v>
+        <v>176888.92799999981</v>
       </c>
       <c r="H53">
-        <v>32000.007079999999</v>
+        <v>32000.00707537686</v>
       </c>
       <c r="I53">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>94</v>
       </c>
       <c r="B54" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A54)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C54">
-        <v>252.47612649999999</v>
+        <v>251.47509236745049</v>
       </c>
       <c r="D54">
-        <v>1395.6319209999999</v>
+        <v>1390.098427253407</v>
       </c>
       <c r="E54">
-        <v>289931574.60000002</v>
+        <v>289931574.57543099</v>
       </c>
       <c r="F54">
-        <v>15130060.08</v>
+        <v>14952988.229497639</v>
       </c>
       <c r="G54">
         <v>176888.92800000001</v>
       </c>
       <c r="H54">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I54">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>95</v>
       </c>
       <c r="B55" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A55)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C55">
-        <v>196.42496990000001</v>
+        <v>196.4249699390179</v>
       </c>
       <c r="D55">
-        <v>1085.793584</v>
+        <v>1085.7935838295709</v>
       </c>
       <c r="E55">
-        <v>289931574.60000002</v>
+        <v>289931574.57543099</v>
       </c>
       <c r="F55">
-        <v>5215231.0870000003</v>
+        <v>5215231.0868634386</v>
       </c>
       <c r="G55">
         <v>176888.92800000001</v>
       </c>
       <c r="H55">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I55">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>96</v>
       </c>
       <c r="B56" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A56)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C56">
-        <v>249.53064670000001</v>
+        <v>248.572804278164</v>
       </c>
       <c r="D56">
-        <v>1379.349964</v>
+        <v>1374.0552236487399</v>
       </c>
       <c r="E56">
-        <v>288026061.10000002</v>
+        <v>288026061.1040557</v>
       </c>
       <c r="F56">
-        <v>14803118.08</v>
+        <v>14633686.3566384</v>
       </c>
       <c r="G56">
-        <v>176888.92800000001</v>
+        <v>176888.92799999981</v>
       </c>
       <c r="H56">
-        <v>32000.007079999999</v>
+        <v>32000.00707537686</v>
       </c>
       <c r="I56">
-        <v>9.8181474069999997</v>
-      </c>
-      <c r="K56">
-        <v>249.0571825508363</v>
-      </c>
-      <c r="L56">
-        <v>1376.732759100456</v>
-      </c>
-      <c r="M56">
-        <v>289280462.7805413</v>
-      </c>
-      <c r="N56">
-        <v>14591603.928536391</v>
-      </c>
-      <c r="O56">
-        <v>176888.92800000001</v>
-      </c>
-      <c r="P56">
-        <v>32000.007075376881</v>
-      </c>
-      <c r="Q56">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>97</v>
       </c>
       <c r="B57" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A57)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>PV revenue</v>
       </c>
       <c r="C57">
-        <v>196.2703564</v>
+        <v>196.27035637253809</v>
       </c>
       <c r="D57">
-        <v>1084.9389140000001</v>
+        <v>1084.938914392641</v>
       </c>
       <c r="E57">
-        <v>288026061.10000002</v>
+        <v>288026061.1040557</v>
       </c>
       <c r="F57">
-        <v>5381962.415</v>
+        <v>5381962.4148363862</v>
       </c>
       <c r="G57">
-        <v>176888.92800000001</v>
+        <v>176888.92799999981</v>
       </c>
       <c r="H57">
-        <v>32000.007079999999</v>
+        <v>32000.00707537686</v>
       </c>
       <c r="I57">
-        <v>9.8181474069999997</v>
-      </c>
-      <c r="K57">
-        <v>196.6836710467953</v>
-      </c>
-      <c r="L57">
-        <v>1087.2236260642289</v>
-      </c>
-      <c r="M57">
-        <v>289280462.7805413</v>
-      </c>
-      <c r="N57">
-        <v>5327309.622990909</v>
-      </c>
-      <c r="O57">
-        <v>176888.92800000001</v>
-      </c>
-      <c r="P57">
-        <v>32000.007075376881</v>
-      </c>
-      <c r="Q57">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>98</v>
       </c>
       <c r="B58" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A58)),"PV revenue","no PV revenue")</f>
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
       <c r="C58">
-        <v>250.01433220000001</v>
+        <v>249.0571825508363</v>
       </c>
       <c r="D58">
-        <v>1382.02367</v>
+        <v>1376.732759100456</v>
       </c>
       <c r="E58">
-        <v>289280462.80000001</v>
+        <v>289280462.7805413</v>
       </c>
       <c r="F58">
-        <v>14760913.109999999</v>
+        <v>14591603.928536391</v>
       </c>
       <c r="G58">
         <v>176888.92800000001</v>
       </c>
       <c r="H58">
-        <v>32000.007079999999</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I58">
-        <v>9.8181474069999997</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>99</v>
-      </c>
-      <c r="B59" t="str">
+        <v>116</v>
+      </c>
+      <c r="B59" s="5" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", A59)),"PV revenue","no PV revenue")</f>
-        <v>no PV revenue</v>
+        <v>PV revenue</v>
       </c>
       <c r="C59">
-        <v>256.83554585130742</v>
+        <v>196.6836710467953</v>
       </c>
       <c r="D59">
-        <v>1419.729822900282</v>
+        <v>1087.2236260642289</v>
       </c>
       <c r="E59">
-        <v>302186986.11188918</v>
+        <v>289280462.7805413</v>
       </c>
       <c r="F59">
-        <v>14652952.36482597</v>
+        <v>5327309.622990909</v>
       </c>
       <c r="G59">
         <v>176888.92800000001</v>
       </c>
       <c r="H59">
-        <v>32000.007075376889</v>
+        <v>32000.007075376881</v>
       </c>
       <c r="I59">
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B60" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A60)),"PV revenue","no PV revenue")</f>
-        <v>PV revenue</v>
+        <f t="shared" si="2"/>
+        <v>no PV revenue</v>
       </c>
       <c r="C60">
-        <v>204.4871979357284</v>
+        <v>256.83554585130742</v>
       </c>
       <c r="D60">
-        <v>1130.359788589165</v>
+        <v>1419.729822900282</v>
       </c>
       <c r="E60">
         <v>302186986.11188918</v>
       </c>
       <c r="F60">
-        <v>5393109.2194681587</v>
+        <v>14652952.36482597</v>
       </c>
       <c r="G60">
         <v>176888.92800000001</v>
@@ -5580,55 +5542,55 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B61" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A61)),"PV revenue","no PV revenue")</f>
-        <v>no PV revenue</v>
+        <f t="shared" si="2"/>
+        <v>PV revenue</v>
       </c>
       <c r="C61">
-        <v>240.76916765020661</v>
+        <v>204.4871979357284</v>
       </c>
       <c r="D61">
-        <v>1330.918454510864</v>
+        <v>1130.359788589165</v>
       </c>
       <c r="E61">
-        <v>275093144.98216528</v>
+        <v>302186986.11188918</v>
       </c>
       <c r="F61">
-        <v>14570555.512556581</v>
+        <v>5393109.2194681587</v>
       </c>
       <c r="G61">
         <v>176888.92800000001</v>
       </c>
       <c r="H61">
-        <v>32000.007075376881</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I61">
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B62" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A62)),"PV revenue","no PV revenue")</f>
-        <v>PV revenue</v>
+        <f t="shared" si="2"/>
+        <v>no PV revenue</v>
       </c>
       <c r="C62">
-        <v>188.46969340611801</v>
+        <v>240.76916765020661</v>
       </c>
       <c r="D62">
-        <v>1041.81858299493</v>
+        <v>1330.918454510864</v>
       </c>
       <c r="E62">
         <v>275093144.98216528</v>
       </c>
       <c r="F62">
-        <v>5319357.578556139</v>
+        <v>14570555.512556581</v>
       </c>
       <c r="G62">
         <v>176888.92800000001</v>
@@ -5640,55 +5602,55 @@
         <v>9.8181474074492936</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>102</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="2"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C63">
+        <v>188.46969340611801</v>
+      </c>
+      <c r="D63">
+        <v>1041.81858299493</v>
+      </c>
+      <c r="E63">
+        <v>275093144.98216528</v>
+      </c>
+      <c r="F63">
+        <v>5319357.578556139</v>
+      </c>
+      <c r="G63">
+        <v>176888.92800000001</v>
+      </c>
+      <c r="H63">
+        <v>32000.007075376881</v>
+      </c>
+      <c r="I63">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>107</v>
       </c>
-      <c r="B63" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A63)),"PV revenue","no PV revenue")</f>
+      <c r="B64" t="str">
+        <f t="shared" si="2"/>
         <v>no PV revenue</v>
       </c>
-      <c r="C63">
-        <v>262.62631520402192</v>
-      </c>
-      <c r="D63">
-        <v>1451.739909044454</v>
-      </c>
-      <c r="E63">
-        <v>298331833.89240187</v>
-      </c>
-      <c r="F63">
-        <v>16069931.11681715</v>
-      </c>
-      <c r="G63">
-        <v>176888.92799996189</v>
-      </c>
-      <c r="H63">
-        <v>32000.007075370009</v>
-      </c>
-      <c r="I63">
-        <v>9.8181474074492936</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>108</v>
-      </c>
-      <c r="B64" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A64)),"PV revenue","no PV revenue")</f>
-        <v>PV revenue</v>
-      </c>
       <c r="C64">
-        <v>211.80775199938211</v>
+        <v>261.68881391394638</v>
       </c>
       <c r="D64">
-        <v>1170.8261846632511</v>
+        <v>1446.557610246537</v>
       </c>
       <c r="E64">
         <v>298331833.89240187</v>
       </c>
       <c r="F64">
-        <v>7080689.949050107</v>
+        <v>15904097.51861711</v>
       </c>
       <c r="G64">
         <v>176888.92799996189</v>
@@ -5702,83 +5664,83 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B65" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A65)),"PV revenue","no PV revenue")</f>
-        <v>no PV revenue</v>
+        <f t="shared" si="2"/>
+        <v>PV revenue</v>
       </c>
       <c r="C65">
-        <v>255.7884578</v>
+        <v>211.80775199938211</v>
       </c>
       <c r="D65">
-        <v>1413.9417530000001</v>
+        <v>1170.8261846632511</v>
       </c>
       <c r="E65">
-        <v>293126897.89999998</v>
+        <v>298331833.89240187</v>
       </c>
       <c r="F65">
-        <v>15390524.08</v>
+        <v>7080689.949050107</v>
       </c>
       <c r="G65">
-        <v>176888.92800000001</v>
+        <v>176888.92799996189</v>
       </c>
       <c r="H65">
-        <v>32000.007079999999</v>
+        <v>32000.007075370009</v>
       </c>
       <c r="I65">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B66" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A66)),"PV revenue","no PV revenue")</f>
-        <v>PV revenue</v>
+        <f t="shared" si="2"/>
+        <v>no PV revenue</v>
       </c>
       <c r="C66">
-        <v>203.69102849999999</v>
+        <v>254.83829181135499</v>
       </c>
       <c r="D66">
-        <v>1125.9587409999999</v>
+        <v>1408.6894464016571</v>
       </c>
       <c r="E66">
-        <v>293126897.89999998</v>
+        <v>293126897.9251197</v>
       </c>
       <c r="F66">
-        <v>6175065.6540000001</v>
+        <v>15222450.232710131</v>
       </c>
       <c r="G66">
         <v>176888.92800000001</v>
       </c>
       <c r="H66">
-        <v>32000.007079999999</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I66">
-        <v>9.8181474069999997</v>
+        <v>9.8181474074492936</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B67" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A67)),"PV revenue","no PV revenue")</f>
-        <v>no PV revenue</v>
+        <f t="shared" ref="B67:B98" si="3">IF(ISNUMBER(SEARCH("PV", A67)),"PV revenue","no PV revenue")</f>
+        <v>PV revenue</v>
       </c>
       <c r="C67">
-        <v>239.3277953998678</v>
+        <v>203.69102849292591</v>
       </c>
       <c r="D67">
-        <v>1322.950869015936</v>
+        <v>1125.958740835895</v>
       </c>
       <c r="E67">
-        <v>280769564.06627142</v>
+        <v>293126897.9251197</v>
       </c>
       <c r="F67">
-        <v>13737436.898423109</v>
+        <v>6175065.6541794688</v>
       </c>
       <c r="G67">
         <v>176888.92800000001</v>
@@ -5792,23 +5754,23 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B68" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A68)),"PV revenue","no PV revenue")</f>
-        <v>PV revenue</v>
+        <f t="shared" si="3"/>
+        <v>no PV revenue</v>
       </c>
       <c r="C68">
-        <v>183.9854727249064</v>
+        <v>238.35205442722281</v>
       </c>
       <c r="D68">
-        <v>1017.030807562677</v>
+        <v>1317.5571897504819</v>
       </c>
       <c r="E68">
         <v>280769564.06627142</v>
       </c>
       <c r="F68">
-        <v>3947992.767419091</v>
+        <v>13564839.12376626</v>
       </c>
       <c r="G68">
         <v>176888.92800000001</v>
@@ -5822,29 +5784,29 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B69" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A69)),"PV revenue","no PV revenue")</f>
-        <v>no PV revenue</v>
+        <f t="shared" si="3"/>
+        <v>PV revenue</v>
       </c>
       <c r="C69">
-        <v>244.28185105722491</v>
+        <v>183.9854727249064</v>
       </c>
       <c r="D69">
-        <v>1350.335787788548</v>
+        <v>1017.030807562677</v>
       </c>
       <c r="E69">
-        <v>284513063.26602769</v>
+        <v>280769564.06627142</v>
       </c>
       <c r="F69">
-        <v>14232470.830683179</v>
+        <v>3947992.767419091</v>
       </c>
       <c r="G69">
-        <v>176888.9280000029</v>
+        <v>176888.92800000001</v>
       </c>
       <c r="H69">
-        <v>32000.007075377409</v>
+        <v>32000.007075376889</v>
       </c>
       <c r="I69">
         <v>9.8181474074492936</v>
@@ -5852,23 +5814,23 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B70" t="str">
-        <f>IF(ISNUMBER(SEARCH("PV", A70)),"PV revenue","no PV revenue")</f>
-        <v>PV revenue</v>
+        <f t="shared" si="3"/>
+        <v>no PV revenue</v>
       </c>
       <c r="C70">
-        <v>189.9325502857827</v>
+        <v>243.31338592995459</v>
       </c>
       <c r="D70">
-        <v>1049.9049307464099</v>
+        <v>1344.982327779471</v>
       </c>
       <c r="E70">
         <v>284513063.26602769</v>
       </c>
       <c r="F70">
-        <v>4618681.2796730399</v>
+        <v>14061160.07251494</v>
       </c>
       <c r="G70">
         <v>176888.9280000029</v>
@@ -5877,6 +5839,36 @@
         <v>32000.007075377409</v>
       </c>
       <c r="I70">
+        <v>9.8181474074492936</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>115</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="3"/>
+        <v>PV revenue</v>
+      </c>
+      <c r="C71">
+        <v>189.9325502857827</v>
+      </c>
+      <c r="D71">
+        <v>1049.9049307464099</v>
+      </c>
+      <c r="E71">
+        <v>284513063.26602769</v>
+      </c>
+      <c r="F71">
+        <v>4618681.2796730399</v>
+      </c>
+      <c r="G71">
+        <v>176888.9280000029</v>
+      </c>
+      <c r="H71">
+        <v>32000.007075377409</v>
+      </c>
+      <c r="I71">
         <v>9.8181474074492936</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding PV generation and power price to example weeks file
</commit_message>
<xml_diff>
--- a/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
+++ b/spine_projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/output_LCOE_comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\Nord_H2ub\Spine_Projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080F5BAF-17EA-474A-8728-19A3CFB906B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DA984C-E54D-4CB1-B99F-F65F05DFDAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4575" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{3BB5C906-8FA9-43D8-B9CC-89F65EA8A47E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_operating_points" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -470,7 +470,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2372,7 +2371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB416CA-7C9B-4F0E-AFD4-34077EF25340}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -3150,7 +3149,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:I5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3508,8 +3507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5837E54A-3435-47A0-958D-D2D4B44DC326}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3776,12 +3775,12 @@
         <v>1375.306559250821</v>
       </c>
       <c r="U4" s="4">
-        <f>R2/P4</f>
-        <v>0.96444875186361267</v>
+        <f>O2/P4</f>
+        <v>0.9983492721883791</v>
       </c>
       <c r="V4">
         <f>1-U4</f>
-        <v>3.5551248136387326E-2</v>
+        <v>1.6507278116209001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -3849,12 +3848,12 @@
         <v>1344.982327779471</v>
       </c>
       <c r="U5">
-        <f>R6/P4</f>
-        <v>1.0939878940432144</v>
+        <f>O6/P4</f>
+        <v>1.0016817399607865</v>
       </c>
       <c r="V5">
         <f>U5-1</f>
-        <v>9.3987894043214393E-2</v>
+        <v>1.6817399607864658E-3</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
@@ -5486,7 +5485,7 @@
       <c r="A59" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="5" t="str">
+      <c r="B59" t="str">
         <f>IF(ISNUMBER(SEARCH("PV", A59)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
@@ -5727,7 +5726,7 @@
         <v>111</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B98" si="3">IF(ISNUMBER(SEARCH("PV", A67)),"PV revenue","no PV revenue")</f>
+        <f t="shared" ref="B67:B71" si="3">IF(ISNUMBER(SEARCH("PV", A67)),"PV revenue","no PV revenue")</f>
         <v>PV revenue</v>
       </c>
       <c r="C67">

</xml_diff>